<commit_message>
New tests for Zij
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/LMDIR/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="17080" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="with matrices - incremental" sheetId="1" r:id="rId1"/>
     <sheet name="with matrices - for testing" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="27">
   <si>
     <t>V</t>
   </si>
@@ -414,12 +414,59 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = L(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)_hat </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -628,16 +675,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -676,6 +723,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -950,7 +1000,7 @@
       <selection activeCell="D45" sqref="D45:F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -986,97 +1036,97 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:42" ht="26">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="AJ2" s="27" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+    </row>
+    <row r="2" spans="1:42">
+      <c r="AJ2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AN2" s="27" t="s">
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AN2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="D3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="X3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AE3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AJ3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AN3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="R3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="X3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AE3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AJ3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AN3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
+    </row>
+    <row r="4" spans="1:42">
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -1147,11 +1197,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>1950</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21">
@@ -1190,7 +1240,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -1208,7 +1258,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -1226,7 +1276,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AC5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -1247,8 +1297,8 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
+    <row r="6" spans="1:42">
+      <c r="B6" s="28"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -1273,7 +1323,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -1289,7 +1339,7 @@
         <f t="shared" ref="T6" si="3">LN(F13) - LN(F6)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="25"/>
+      <c r="V6" s="28"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -1305,7 +1355,7 @@
         <f t="shared" ref="Z6" si="5">$M6*T6</f>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="25"/>
+      <c r="AC6" s="28"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -1324,35 +1374,35 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+    <row r="7" spans="1:42">
+      <c r="D7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="X7" s="26" t="s">
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="X7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AE7" s="26" t="s">
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AE7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
@@ -1419,63 +1469,63 @@
         <v>1.3794101155854785</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="G9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="X9" s="27" t="s">
+      <c r="X9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
       <c r="AA9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
       <c r="AH9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D10" s="27" t="s">
+    <row r="10" spans="1:42">
+      <c r="D10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="1"/>
-      <c r="R10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="X10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AE10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
+      <c r="R10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="X10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AE10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42">
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -1520,11 +1570,11 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42">
       <c r="A12">
         <v>1960</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="21">
@@ -1565,7 +1615,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="P12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -1583,7 +1633,7 @@
         <f t="shared" ref="T12:T13" si="13">LN(F19) - LN(F12)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -1601,7 +1651,7 @@
         <f t="shared" ref="Z12:Z13" si="15">$M12*T12</f>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="25" t="s">
+      <c r="AC12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -1622,8 +1672,8 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
+    <row r="13" spans="1:42">
+      <c r="B13" s="28"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -1652,7 +1702,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="25"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -1668,7 +1718,7 @@
         <f t="shared" si="13"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -1684,7 +1734,7 @@
         <f t="shared" si="15"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="25"/>
+      <c r="AC13" s="28"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -1703,12 +1753,12 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+    <row r="14" spans="1:42">
+      <c r="D14" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -1716,25 +1766,25 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="X14" s="26" t="s">
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="X14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AE14" s="26" t="s">
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AE14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -1807,7 +1857,7 @@
         <v>1.7570566194986847</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1821,56 +1871,56 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="27" t="s">
+      <c r="X16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
       <c r="AA16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="26" t="s">
+      <c r="AE16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D17" s="27" t="s">
+    <row r="17" spans="1:42">
+      <c r="D17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="1"/>
-      <c r="R17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="X17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AE17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
+      <c r="R17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="X17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AE17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42">
       <c r="D18" s="1">
         <v>1</v>
       </c>
@@ -1915,11 +1965,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42">
       <c r="A19">
         <v>1970</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="21">
@@ -1960,7 +2010,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="25" t="s">
+      <c r="P19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -1978,7 +2028,7 @@
         <f t="shared" ref="T19:T20" si="23">LN(F26) - LN(F19)</f>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="25" t="s">
+      <c r="V19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -1996,7 +2046,7 @@
         <f t="shared" ref="Z19:Z20" si="25">$M19*T19</f>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="25" t="s">
+      <c r="AC19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -2017,8 +2067,8 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
+    <row r="20" spans="1:42">
+      <c r="B20" s="28"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -2047,7 +2097,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="25"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -2063,7 +2113,7 @@
         <f t="shared" si="23"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -2079,7 +2129,7 @@
         <f t="shared" si="25"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="25"/>
+      <c r="AC20" s="28"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -2098,12 +2148,12 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+    <row r="21" spans="1:42">
+      <c r="D21" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -2111,25 +2161,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="26" t="s">
+      <c r="R21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="X21" s="26" t="s">
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="X21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AE21" s="26" t="s">
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AE21" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2202,7 +2252,7 @@
         <v>2.1227707766832733</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2216,56 +2266,56 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="27" t="s">
+      <c r="X23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
       <c r="AA23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="26" t="s">
+      <c r="AE23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
       <c r="AH23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D24" s="27" t="s">
+    <row r="24" spans="1:42">
+      <c r="D24" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="N24" s="1"/>
-      <c r="R24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="X24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AE24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="27"/>
+      <c r="R24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="X24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AE24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42">
       <c r="D25" s="1">
         <v>1</v>
       </c>
@@ -2310,11 +2360,11 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42">
       <c r="A26">
         <v>1980</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="21">
@@ -2355,7 +2405,7 @@
         <f>M26/L$26</f>
         <v>0.10561476584617054</v>
       </c>
-      <c r="P26" s="25" t="s">
+      <c r="P26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q26" s="21">
@@ -2373,7 +2423,7 @@
         <f t="shared" ref="T26:T27" si="35">LN(F33) - LN(F26)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V26" s="25" t="s">
+      <c r="V26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
@@ -2391,7 +2441,7 @@
         <f t="shared" ref="Z26:Z27" si="37">$M26*T26</f>
         <v>7.7700766953751215</v>
       </c>
-      <c r="AC26" s="25" t="s">
+      <c r="AC26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD26" s="21">
@@ -2412,8 +2462,8 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+    <row r="27" spans="1:42">
+      <c r="B27" s="28"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -2442,7 +2492,7 @@
         <f>M27/L$26</f>
         <v>0.88988350592239895</v>
       </c>
-      <c r="P27" s="25"/>
+      <c r="P27" s="28"/>
       <c r="Q27" s="21">
         <v>2</v>
       </c>
@@ -2458,7 +2508,7 @@
         <f t="shared" si="35"/>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V27" s="25"/>
+      <c r="V27" s="28"/>
       <c r="W27" s="21">
         <v>2</v>
       </c>
@@ -2474,7 +2524,7 @@
         <f t="shared" si="37"/>
         <v>55.353010514175885</v>
       </c>
-      <c r="AC27" s="25"/>
+      <c r="AC27" s="28"/>
       <c r="AD27" s="21">
         <v>2</v>
       </c>
@@ -2493,12 +2543,12 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+    <row r="28" spans="1:42">
+      <c r="D28" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2506,25 +2556,25 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="R28" s="26" t="s">
+      <c r="R28" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="X28" s="26" t="s">
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="X28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AE28" s="26" t="s">
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AE28" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF28" s="26"/>
-      <c r="AG28" s="26"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="27"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2596,7 +2646,7 @@
         <v>2.4822221852499999</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2609,55 +2659,55 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="X30" s="27" t="s">
+      <c r="X30" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="27"/>
+      <c r="Y30" s="25"/>
+      <c r="Z30" s="25"/>
       <c r="AA30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB30" s="8"/>
-      <c r="AE30" s="26" t="s">
+      <c r="AE30" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF30" s="26"/>
-      <c r="AG30" s="26"/>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
       <c r="AH30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D31" s="27" t="s">
+    <row r="31" spans="1:42">
+      <c r="D31" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="N31" s="1"/>
-      <c r="R31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="X31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="27"/>
-      <c r="Z31" s="27"/>
-      <c r="AE31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="27"/>
-      <c r="AG31" s="27"/>
+      <c r="R31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="X31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AE31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42">
       <c r="D32" s="1">
         <v>1</v>
       </c>
@@ -2701,11 +2751,11 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:42">
       <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="21">
@@ -2745,7 +2795,7 @@
         <f>M33/L$33</f>
         <v>5.7396961403155373E-2</v>
       </c>
-      <c r="P33" s="25" t="s">
+      <c r="P33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q33" s="21">
@@ -2763,7 +2813,7 @@
         <f t="shared" ref="T33:T34" si="47">LN(F40) - LN(F33)</f>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V33" s="25" t="s">
+      <c r="V33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W33" s="21">
@@ -2781,7 +2831,7 @@
         <f t="shared" ref="Z33:Z34" si="49">$M33*T33</f>
         <v>5.0235683675903013</v>
       </c>
-      <c r="AC33" s="25" t="s">
+      <c r="AC33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD33" s="21">
@@ -2802,8 +2852,8 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
+    <row r="34" spans="1:42">
+      <c r="B34" s="28"/>
       <c r="C34" s="21">
         <v>2</v>
       </c>
@@ -2831,7 +2881,7 @@
         <f>M34/L$33</f>
         <v>0.94110538842717861</v>
       </c>
-      <c r="P34" s="25"/>
+      <c r="P34" s="28"/>
       <c r="Q34" s="21">
         <v>2</v>
       </c>
@@ -2847,7 +2897,7 @@
         <f t="shared" si="47"/>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V34" s="25"/>
+      <c r="V34" s="28"/>
       <c r="W34" s="21">
         <v>2</v>
       </c>
@@ -2863,7 +2913,7 @@
         <f t="shared" si="49"/>
         <v>71.350925324956492</v>
       </c>
-      <c r="AC34" s="25"/>
+      <c r="AC34" s="28"/>
       <c r="AD34" s="21">
         <v>2</v>
       </c>
@@ -2882,37 +2932,37 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D35" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+    <row r="35" spans="1:42">
+      <c r="D35" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="R35" s="26" t="s">
+      <c r="R35" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="X35" s="26" t="s">
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="X35" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AE35" s="26" t="s">
+      <c r="Y35" s="27"/>
+      <c r="Z35" s="27"/>
+      <c r="AE35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF35" s="26"/>
-      <c r="AG35" s="26"/>
+      <c r="AF35" s="27"/>
+      <c r="AG35" s="27"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:42">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -2984,7 +3034,7 @@
         <v>2.8396167479260592</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2997,55 +3047,55 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="X37" s="27" t="s">
+      <c r="X37" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y37" s="27"/>
-      <c r="Z37" s="27"/>
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
       <c r="AA37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB37" s="8"/>
-      <c r="AE37" s="26" t="s">
+      <c r="AE37" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF37" s="26"/>
-      <c r="AG37" s="26"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
       <c r="AH37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D38" s="27" t="s">
+    <row r="38" spans="1:42">
+      <c r="D38" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="N38" s="1"/>
-      <c r="R38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="X38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="27"/>
-      <c r="Z38" s="27"/>
-      <c r="AE38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="27"/>
-      <c r="AG38" s="27"/>
+      <c r="R38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38" s="25"/>
+      <c r="T38" s="25"/>
+      <c r="X38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AE38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="25"/>
+      <c r="AG38" s="25"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:42">
       <c r="D39" s="1">
         <v>1</v>
       </c>
@@ -3089,11 +3139,11 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:42">
       <c r="A40">
         <v>2000</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="21">
@@ -3133,7 +3183,7 @@
         <f>M40/L$40</f>
         <v>2.5568845446814027E-2</v>
       </c>
-      <c r="P40" s="25" t="s">
+      <c r="P40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q40" s="21">
@@ -3151,7 +3201,7 @@
         <f t="shared" ref="T40:T41" si="59">LN(F47) - LN(F40)</f>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V40" s="25" t="s">
+      <c r="V40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W40" s="21">
@@ -3169,7 +3219,7 @@
         <f t="shared" ref="Z40:Z41" si="61">$M40*T40</f>
         <v>2.665651423580965</v>
       </c>
-      <c r="AC40" s="25" t="s">
+      <c r="AC40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD40" s="21">
@@ -3190,8 +3240,8 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B41" s="25"/>
+    <row r="41" spans="1:42">
+      <c r="B41" s="28"/>
       <c r="C41" s="21">
         <v>2</v>
       </c>
@@ -3219,7 +3269,7 @@
         <f>M41/L$40</f>
         <v>0.97162630393947746</v>
       </c>
-      <c r="P41" s="25"/>
+      <c r="P41" s="28"/>
       <c r="Q41" s="21">
         <v>2</v>
       </c>
@@ -3235,7 +3285,7 @@
         <f t="shared" si="59"/>
         <v>0.11778303565638382</v>
       </c>
-      <c r="V41" s="25"/>
+      <c r="V41" s="28"/>
       <c r="W41" s="21">
         <v>2</v>
       </c>
@@ -3251,7 +3301,7 @@
         <f t="shared" si="61"/>
         <v>89.349241143602967</v>
       </c>
-      <c r="AC41" s="25"/>
+      <c r="AC41" s="28"/>
       <c r="AD41" s="21">
         <v>2</v>
       </c>
@@ -3270,37 +3320,37 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D42" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+    <row r="42" spans="1:42">
+      <c r="D42" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
       <c r="G42" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="R42" s="26" t="s">
+      <c r="R42" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="X42" s="26" t="s">
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="X42" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y42" s="26"/>
-      <c r="Z42" s="26"/>
-      <c r="AE42" s="26" t="s">
+      <c r="Y42" s="27"/>
+      <c r="Z42" s="27"/>
+      <c r="AE42" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF42" s="26"/>
-      <c r="AG42" s="26"/>
+      <c r="AF42" s="27"/>
+      <c r="AG42" s="27"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:42">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -3372,7 +3422,7 @@
         <v>3.1947998282292427</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:42">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3385,36 +3435,36 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="X44" s="27" t="s">
+      <c r="X44" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y44" s="27"/>
-      <c r="Z44" s="27"/>
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
       <c r="AA44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB44" s="8"/>
-      <c r="AE44" s="26" t="s">
+      <c r="AE44" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF44" s="26"/>
-      <c r="AG44" s="26"/>
+      <c r="AF44" s="27"/>
+      <c r="AG44" s="27"/>
       <c r="AH44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D45" s="27" t="s">
+    <row r="45" spans="1:42">
+      <c r="D45" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:42">
       <c r="D46" s="1">
         <v>1</v>
       </c>
@@ -3427,11 +3477,11 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:42">
       <c r="A47">
         <v>2010</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="21">
@@ -3453,8 +3503,8 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B48" s="25"/>
+    <row r="48" spans="1:42">
+      <c r="B48" s="28"/>
       <c r="C48" s="21">
         <v>2</v>
       </c>
@@ -3474,12 +3524,12 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D49" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
+    <row r="49" spans="1:37">
+      <c r="D49" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
       <c r="G49" s="7" t="s">
         <v>4</v>
       </c>
@@ -3494,7 +3544,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -3508,7 +3558,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -3521,15 +3571,15 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37">
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37">
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" ht="17">
       <c r="P54" s="20" t="s">
         <v>14</v>
       </c>
@@ -3542,13 +3592,13 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37">
       <c r="U55" s="6"/>
       <c r="V55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37">
       <c r="U56" s="6"/>
       <c r="V56" t="s">
         <v>17</v>
@@ -3556,50 +3606,38 @@
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="A1:AP1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="X42:Z42"/>
-    <mergeCell ref="AE42:AG42"/>
-    <mergeCell ref="X44:Z44"/>
-    <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="X38:Z38"/>
-    <mergeCell ref="AE38:AG38"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="V40:V41"/>
-    <mergeCell ref="AC40:AC41"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="X35:Z35"/>
-    <mergeCell ref="AE35:AG35"/>
-    <mergeCell ref="X37:Z37"/>
-    <mergeCell ref="AE37:AG37"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="V33:V34"/>
-    <mergeCell ref="AC33:AC34"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="X28:Z28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="X30:Z30"/>
-    <mergeCell ref="AE30:AG30"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AE24:AG24"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE9:AG9"/>
     <mergeCell ref="AE16:AG16"/>
     <mergeCell ref="X9:Z9"/>
     <mergeCell ref="X16:Z16"/>
@@ -3616,38 +3654,50 @@
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="X23:Z23"/>
     <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="AE30:AG30"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="AC33:AC34"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="X35:Z35"/>
+    <mergeCell ref="AE35:AG35"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="AE37:AG37"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="X38:Z38"/>
+    <mergeCell ref="AE38:AG38"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="V40:V41"/>
+    <mergeCell ref="AC40:AC41"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="X42:Z42"/>
+    <mergeCell ref="AE42:AG42"/>
+    <mergeCell ref="X44:Z44"/>
+    <mergeCell ref="AE44:AG44"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="A1:AP1"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3659,10 +3709,10 @@
   <dimension ref="A1:AP47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -3698,97 +3748,97 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:42" ht="26">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="AJ2" s="27" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+    </row>
+    <row r="2" spans="1:42">
+      <c r="AJ2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AN2" s="27" t="s">
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AN2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="D3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="X3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AE3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AJ3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AN3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="R3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="X3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AE3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AJ3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AN3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
+    </row>
+    <row r="4" spans="1:42">
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -3859,11 +3909,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>1971</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="21">
@@ -3902,7 +3952,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -3920,7 +3970,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -3938,7 +3988,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AC5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -3959,8 +4009,8 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
+    <row r="6" spans="1:42">
+      <c r="B6" s="28"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -3985,7 +4035,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -4001,7 +4051,7 @@
         <f t="shared" si="2"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="25"/>
+      <c r="V6" s="28"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -4017,7 +4067,7 @@
         <f t="shared" si="0"/>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="25"/>
+      <c r="AC6" s="28"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -4036,35 +4086,35 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+    <row r="7" spans="1:42">
+      <c r="D7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="X7" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AE7" s="26" t="s">
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="X7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AE7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
@@ -4131,7 +4181,7 @@
         <v>1.3794101155854785</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="8" t="s">
@@ -4142,56 +4192,56 @@
         <v>0.41594614744177039</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="X9" s="27" t="s">
+      <c r="X9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
       <c r="AA9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
       <c r="AH9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D10" s="27" t="s">
+    <row r="10" spans="1:42">
+      <c r="D10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="2"/>
-      <c r="R10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="X10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AE10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
+      <c r="R10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="X10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AE10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42">
       <c r="D11" s="2">
         <v>1</v>
       </c>
@@ -4236,11 +4286,11 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" ht="16" customHeight="1">
       <c r="A12">
         <v>1972</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="21">
@@ -4281,7 +4331,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="P12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -4299,7 +4349,7 @@
         <f t="shared" si="7"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -4317,7 +4367,7 @@
         <f t="shared" si="8"/>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="25" t="s">
+      <c r="AC12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -4338,8 +4388,8 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
+    <row r="13" spans="1:42">
+      <c r="B13" s="28"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -4368,7 +4418,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="25"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -4384,7 +4434,7 @@
         <f t="shared" si="7"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -4400,7 +4450,7 @@
         <f t="shared" si="8"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="25"/>
+      <c r="AC13" s="28"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -4419,12 +4469,12 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+    <row r="14" spans="1:42">
+      <c r="D14" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -4432,25 +4482,25 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="X14" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AE14" s="26" t="s">
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="X14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AE14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -4523,7 +4573,7 @@
         <v>1.7570566194986847</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -4537,56 +4587,56 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="27" t="s">
+      <c r="X16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
       <c r="AA16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="26" t="s">
+      <c r="AE16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D17" s="27" t="s">
+    <row r="17" spans="1:42">
+      <c r="D17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="2"/>
-      <c r="R17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="X17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AE17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
+      <c r="R17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="X17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AE17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42">
       <c r="D18" s="2">
         <v>1</v>
       </c>
@@ -4631,11 +4681,11 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" ht="16" customHeight="1">
       <c r="A19">
         <v>1973</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="21">
@@ -4676,7 +4726,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="25" t="s">
+      <c r="P19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -4694,7 +4744,7 @@
         <f t="shared" si="14"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="25" t="s">
+      <c r="V19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -4712,7 +4762,7 @@
         <f t="shared" si="15"/>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="25" t="s">
+      <c r="AC19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -4733,8 +4783,8 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
+    <row r="20" spans="1:42">
+      <c r="B20" s="28"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -4763,7 +4813,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="25"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -4779,7 +4829,7 @@
         <f t="shared" si="14"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -4795,7 +4845,7 @@
         <f t="shared" si="15"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="25"/>
+      <c r="AC20" s="28"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -4814,12 +4864,12 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+    <row r="21" spans="1:42">
+      <c r="D21" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -4827,25 +4877,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="26" t="s">
+      <c r="R21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="X21" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AE21" s="26" t="s">
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="X21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AE21" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -4918,7 +4968,7 @@
         <v>2.1227707766832733</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4932,32 +4982,32 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="27" t="s">
+      <c r="X23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
       <c r="AA23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="26" t="s">
+      <c r="AE23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
       <c r="AH23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D24" s="27" t="s">
+    <row r="24" spans="1:42">
+      <c r="D24" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -4993,7 +5043,7 @@
       <c r="AO24" s="9"/>
       <c r="AP24" s="9"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42">
       <c r="D25" s="2">
         <v>1</v>
       </c>
@@ -5038,11 +5088,11 @@
       <c r="AO25" s="9"/>
       <c r="AP25" s="9"/>
     </row>
-    <row r="26" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" ht="16" customHeight="1">
       <c r="A26">
         <v>1974</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="21">
@@ -5096,8 +5146,8 @@
       <c r="AO26" s="9"/>
       <c r="AP26" s="9"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+    <row r="27" spans="1:42">
+      <c r="B27" s="28"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -5149,12 +5199,12 @@
       <c r="AO27" s="9"/>
       <c r="AP27" s="9"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+    <row r="28" spans="1:42">
+      <c r="D28" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -5193,7 +5243,7 @@
       <c r="AO28" s="9"/>
       <c r="AP28" s="9"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -5239,7 +5289,7 @@
       <c r="AO29" s="8"/>
       <c r="AP29" s="8"/>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -5284,7 +5334,7 @@
       <c r="AO30" s="9"/>
       <c r="AP30" s="9"/>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42">
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -5319,7 +5369,7 @@
       <c r="AO31" s="9"/>
       <c r="AP31" s="9"/>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42">
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -5354,11 +5404,52 @@
       <c r="AO32" s="9"/>
       <c r="AP32" s="9"/>
     </row>
-    <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="16" customHeight="1"/>
+    <row r="40" ht="16" customHeight="1"/>
+    <row r="47" ht="16" customHeight="1"/>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="AE21:AG21"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="X7:Z7"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="AN2:AP2"/>
@@ -5368,47 +5459,6 @@
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AJ3:AL3"/>
     <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="AE21:AG21"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="AE23:AG23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Just re-saved the .xlsx file
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/LMDIR/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LMDIR/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="with matrices - incremental" sheetId="1" r:id="rId1"/>
     <sheet name="with matrices - for testing" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -465,8 +465,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -675,16 +675,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -1000,7 +1000,7 @@
       <selection activeCell="D45" sqref="D45:F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -1036,97 +1036,97 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="AJ2" s="25" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AN2" s="25" t="s">
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AN2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-    </row>
-    <row r="3" spans="1:42">
-      <c r="D3" s="25" t="s">
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="R3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="X3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AE3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AJ3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AN3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="R3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="X3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AE3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AJ3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AN3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -1197,11 +1197,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1950</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21">
@@ -1240,7 +1240,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -1258,7 +1258,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -1276,7 +1276,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -1297,8 +1297,8 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:42">
-      <c r="B6" s="28"/>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B6" s="25"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -1323,7 +1323,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="28"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -1339,7 +1339,7 @@
         <f t="shared" ref="T6" si="3">LN(F13) - LN(F6)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="28"/>
+      <c r="V6" s="25"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -1355,7 +1355,7 @@
         <f t="shared" ref="Z6" si="5">$M6*T6</f>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="28"/>
+      <c r="AC6" s="25"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -1374,35 +1374,35 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:42">
-      <c r="D7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="X7" s="27" t="s">
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="X7" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AE7" s="27" t="s">
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AE7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
@@ -1469,63 +1469,63 @@
         <v>1.3794101155854785</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="G9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="X9" s="25" t="s">
+      <c r="X9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="27" t="s">
+      <c r="AE9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
       <c r="AH9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:42">
-      <c r="D10" s="25" t="s">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="1"/>
-      <c r="R10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="X10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AE10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
+      <c r="R10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="X10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AE10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -1570,11 +1570,11 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1960</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="21">
@@ -1615,7 +1615,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -1633,7 +1633,7 @@
         <f t="shared" ref="T12:T13" si="13">LN(F19) - LN(F12)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="28" t="s">
+      <c r="V12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -1651,7 +1651,7 @@
         <f t="shared" ref="Z12:Z13" si="15">$M12*T12</f>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="28" t="s">
+      <c r="AC12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -1672,8 +1672,8 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:42">
-      <c r="B13" s="28"/>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B13" s="25"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -1702,7 +1702,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="28"/>
+      <c r="P13" s="25"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -1718,7 +1718,7 @@
         <f t="shared" si="13"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="28"/>
+      <c r="V13" s="25"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -1734,7 +1734,7 @@
         <f t="shared" si="15"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="28"/>
+      <c r="AC13" s="25"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -1753,12 +1753,12 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:42">
-      <c r="D14" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -1766,25 +1766,25 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="27" t="s">
+      <c r="R14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="X14" s="27" t="s">
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="X14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AE14" s="27" t="s">
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AE14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -1857,7 +1857,7 @@
         <v>1.7570566194986847</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1871,56 +1871,56 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="25" t="s">
+      <c r="X16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
       <c r="AA16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="27" t="s">
+      <c r="AE16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
+      <c r="AF16" s="26"/>
+      <c r="AG16" s="26"/>
       <c r="AH16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:42">
-      <c r="D17" s="25" t="s">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="1"/>
-      <c r="R17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="X17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AE17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
+      <c r="R17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="X17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AE17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D18" s="1">
         <v>1</v>
       </c>
@@ -1965,11 +1965,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1970</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="21">
@@ -2010,7 +2010,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="28" t="s">
+      <c r="P19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -2028,7 +2028,7 @@
         <f t="shared" ref="T19:T20" si="23">LN(F26) - LN(F19)</f>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="28" t="s">
+      <c r="V19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -2046,7 +2046,7 @@
         <f t="shared" ref="Z19:Z20" si="25">$M19*T19</f>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="28" t="s">
+      <c r="AC19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -2067,8 +2067,8 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:42">
-      <c r="B20" s="28"/>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B20" s="25"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -2097,7 +2097,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="28"/>
+      <c r="P20" s="25"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -2113,7 +2113,7 @@
         <f t="shared" si="23"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="28"/>
+      <c r="V20" s="25"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -2129,7 +2129,7 @@
         <f t="shared" si="25"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="28"/>
+      <c r="AC20" s="25"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -2148,12 +2148,12 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:42">
-      <c r="D21" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D21" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -2161,25 +2161,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="27" t="s">
+      <c r="R21" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="X21" s="27" t="s">
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="X21" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
-      <c r="AE21" s="27" t="s">
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AE21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="27"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="26"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2252,7 +2252,7 @@
         <v>2.1227707766832733</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2266,56 +2266,56 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="25" t="s">
+      <c r="X23" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
       <c r="AA23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="27" t="s">
+      <c r="AE23" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="27"/>
-      <c r="AG23" s="27"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="26"/>
       <c r="AH23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:42">
-      <c r="D24" s="25" t="s">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="N24" s="1"/>
-      <c r="R24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="X24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
-      <c r="AE24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="25"/>
+      <c r="R24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="X24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AE24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="27"/>
+      <c r="AG24" s="27"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D25" s="1">
         <v>1</v>
       </c>
@@ -2360,11 +2360,11 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1980</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="21">
@@ -2405,7 +2405,7 @@
         <f>M26/L$26</f>
         <v>0.10561476584617054</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q26" s="21">
@@ -2423,7 +2423,7 @@
         <f t="shared" ref="T26:T27" si="35">LN(F33) - LN(F26)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V26" s="28" t="s">
+      <c r="V26" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
@@ -2441,7 +2441,7 @@
         <f t="shared" ref="Z26:Z27" si="37">$M26*T26</f>
         <v>7.7700766953751215</v>
       </c>
-      <c r="AC26" s="28" t="s">
+      <c r="AC26" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD26" s="21">
@@ -2462,8 +2462,8 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:42">
-      <c r="B27" s="28"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B27" s="25"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -2492,7 +2492,7 @@
         <f>M27/L$26</f>
         <v>0.88988350592239895</v>
       </c>
-      <c r="P27" s="28"/>
+      <c r="P27" s="25"/>
       <c r="Q27" s="21">
         <v>2</v>
       </c>
@@ -2508,7 +2508,7 @@
         <f t="shared" si="35"/>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V27" s="28"/>
+      <c r="V27" s="25"/>
       <c r="W27" s="21">
         <v>2</v>
       </c>
@@ -2524,7 +2524,7 @@
         <f t="shared" si="37"/>
         <v>55.353010514175885</v>
       </c>
-      <c r="AC27" s="28"/>
+      <c r="AC27" s="25"/>
       <c r="AD27" s="21">
         <v>2</v>
       </c>
@@ -2543,12 +2543,12 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:42">
-      <c r="D28" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2556,25 +2556,25 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="R28" s="27" t="s">
+      <c r="R28" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="X28" s="27" t="s">
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="X28" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y28" s="27"/>
-      <c r="Z28" s="27"/>
-      <c r="AE28" s="27" t="s">
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AE28" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF28" s="27"/>
-      <c r="AG28" s="27"/>
+      <c r="AF28" s="26"/>
+      <c r="AG28" s="26"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2646,7 +2646,7 @@
         <v>2.4822221852499999</v>
       </c>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2659,55 +2659,55 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="X30" s="25" t="s">
+      <c r="X30" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
       <c r="AA30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB30" s="8"/>
-      <c r="AE30" s="27" t="s">
+      <c r="AE30" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF30" s="27"/>
-      <c r="AG30" s="27"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="26"/>
       <c r="AH30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:42">
-      <c r="D31" s="25" t="s">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D31" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="N31" s="1"/>
-      <c r="R31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="X31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AE31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="25"/>
-      <c r="AG31" s="25"/>
+      <c r="R31" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="X31" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="27"/>
+      <c r="AE31" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D32" s="1">
         <v>1</v>
       </c>
@@ -2751,11 +2751,11 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="21">
@@ -2795,7 +2795,7 @@
         <f>M33/L$33</f>
         <v>5.7396961403155373E-2</v>
       </c>
-      <c r="P33" s="28" t="s">
+      <c r="P33" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q33" s="21">
@@ -2813,7 +2813,7 @@
         <f t="shared" ref="T33:T34" si="47">LN(F40) - LN(F33)</f>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V33" s="28" t="s">
+      <c r="V33" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W33" s="21">
@@ -2831,7 +2831,7 @@
         <f t="shared" ref="Z33:Z34" si="49">$M33*T33</f>
         <v>5.0235683675903013</v>
       </c>
-      <c r="AC33" s="28" t="s">
+      <c r="AC33" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD33" s="21">
@@ -2852,8 +2852,8 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:42">
-      <c r="B34" s="28"/>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B34" s="25"/>
       <c r="C34" s="21">
         <v>2</v>
       </c>
@@ -2881,7 +2881,7 @@
         <f>M34/L$33</f>
         <v>0.94110538842717861</v>
       </c>
-      <c r="P34" s="28"/>
+      <c r="P34" s="25"/>
       <c r="Q34" s="21">
         <v>2</v>
       </c>
@@ -2897,7 +2897,7 @@
         <f t="shared" si="47"/>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V34" s="28"/>
+      <c r="V34" s="25"/>
       <c r="W34" s="21">
         <v>2</v>
       </c>
@@ -2913,7 +2913,7 @@
         <f t="shared" si="49"/>
         <v>71.350925324956492</v>
       </c>
-      <c r="AC34" s="28"/>
+      <c r="AC34" s="25"/>
       <c r="AD34" s="21">
         <v>2</v>
       </c>
@@ -2932,37 +2932,37 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:42">
-      <c r="D35" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D35" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
       <c r="G35" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="R35" s="27" t="s">
+      <c r="R35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="X35" s="27" t="s">
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="X35" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y35" s="27"/>
-      <c r="Z35" s="27"/>
-      <c r="AE35" s="27" t="s">
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AE35" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF35" s="27"/>
-      <c r="AG35" s="27"/>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="26"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -3034,7 +3034,7 @@
         <v>2.8396167479260592</v>
       </c>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3047,55 +3047,55 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="X37" s="25" t="s">
+      <c r="X37" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
       <c r="AA37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB37" s="8"/>
-      <c r="AE37" s="27" t="s">
+      <c r="AE37" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF37" s="27"/>
-      <c r="AG37" s="27"/>
+      <c r="AF37" s="26"/>
+      <c r="AG37" s="26"/>
       <c r="AH37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:42">
-      <c r="D38" s="25" t="s">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D38" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="N38" s="1"/>
-      <c r="R38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
-      <c r="X38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
-      <c r="AE38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="25"/>
-      <c r="AG38" s="25"/>
+      <c r="R38" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="X38" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="27"/>
+      <c r="Z38" s="27"/>
+      <c r="AE38" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="27"/>
+      <c r="AG38" s="27"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D39" s="1">
         <v>1</v>
       </c>
@@ -3139,11 +3139,11 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2000</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="21">
@@ -3183,7 +3183,7 @@
         <f>M40/L$40</f>
         <v>2.5568845446814027E-2</v>
       </c>
-      <c r="P40" s="28" t="s">
+      <c r="P40" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q40" s="21">
@@ -3201,7 +3201,7 @@
         <f t="shared" ref="T40:T41" si="59">LN(F47) - LN(F40)</f>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V40" s="28" t="s">
+      <c r="V40" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W40" s="21">
@@ -3219,7 +3219,7 @@
         <f t="shared" ref="Z40:Z41" si="61">$M40*T40</f>
         <v>2.665651423580965</v>
       </c>
-      <c r="AC40" s="28" t="s">
+      <c r="AC40" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD40" s="21">
@@ -3240,8 +3240,8 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="1:42">
-      <c r="B41" s="28"/>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B41" s="25"/>
       <c r="C41" s="21">
         <v>2</v>
       </c>
@@ -3269,7 +3269,7 @@
         <f>M41/L$40</f>
         <v>0.97162630393947746</v>
       </c>
-      <c r="P41" s="28"/>
+      <c r="P41" s="25"/>
       <c r="Q41" s="21">
         <v>2</v>
       </c>
@@ -3285,7 +3285,7 @@
         <f t="shared" si="59"/>
         <v>0.11778303565638382</v>
       </c>
-      <c r="V41" s="28"/>
+      <c r="V41" s="25"/>
       <c r="W41" s="21">
         <v>2</v>
       </c>
@@ -3301,7 +3301,7 @@
         <f t="shared" si="61"/>
         <v>89.349241143602967</v>
       </c>
-      <c r="AC41" s="28"/>
+      <c r="AC41" s="25"/>
       <c r="AD41" s="21">
         <v>2</v>
       </c>
@@ -3320,37 +3320,37 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="1:42">
-      <c r="D42" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D42" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="R42" s="27" t="s">
+      <c r="R42" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="X42" s="27" t="s">
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="X42" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="27"/>
-      <c r="AE42" s="27" t="s">
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AE42" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF42" s="27"/>
-      <c r="AG42" s="27"/>
+      <c r="AF42" s="26"/>
+      <c r="AG42" s="26"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -3422,7 +3422,7 @@
         <v>3.1947998282292427</v>
       </c>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3435,36 +3435,36 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="X44" s="25" t="s">
+      <c r="X44" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y44" s="25"/>
-      <c r="Z44" s="25"/>
+      <c r="Y44" s="27"/>
+      <c r="Z44" s="27"/>
       <c r="AA44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB44" s="8"/>
-      <c r="AE44" s="27" t="s">
+      <c r="AE44" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF44" s="27"/>
-      <c r="AG44" s="27"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="26"/>
       <c r="AH44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="1:42">
-      <c r="D45" s="25" t="s">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D45" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D46" s="1">
         <v>1</v>
       </c>
@@ -3477,11 +3477,11 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2010</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="21">
@@ -3503,8 +3503,8 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="1:42">
-      <c r="B48" s="28"/>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B48" s="25"/>
       <c r="C48" s="21">
         <v>2</v>
       </c>
@@ -3524,12 +3524,12 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="1:37">
-      <c r="D49" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="D49" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="7" t="s">
         <v>4</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -3558,7 +3558,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -3571,15 +3571,15 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="1:37" ht="17">
+    <row r="54" spans="1:37" ht="17" x14ac:dyDescent="0.2">
       <c r="P54" s="20" t="s">
         <v>14</v>
       </c>
@@ -3592,13 +3592,13 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="U55" s="6"/>
       <c r="V55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="U56" s="6"/>
       <c r="V56" t="s">
         <v>17</v>
@@ -3606,38 +3606,50 @@
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="A1:AP1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="X42:Z42"/>
+    <mergeCell ref="AE42:AG42"/>
+    <mergeCell ref="X44:Z44"/>
+    <mergeCell ref="AE44:AG44"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="X38:Z38"/>
+    <mergeCell ref="AE38:AG38"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="V40:V41"/>
+    <mergeCell ref="AC40:AC41"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="X35:Z35"/>
+    <mergeCell ref="AE35:AG35"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="AE37:AG37"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="AC33:AC34"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="AE30:AG30"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="AC26:AC27"/>
     <mergeCell ref="AE16:AG16"/>
     <mergeCell ref="X9:Z9"/>
     <mergeCell ref="X16:Z16"/>
@@ -3654,50 +3666,38 @@
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="X23:Z23"/>
     <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AE24:AG24"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="X28:Z28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="X30:Z30"/>
-    <mergeCell ref="AE30:AG30"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="V33:V34"/>
-    <mergeCell ref="AC33:AC34"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="X35:Z35"/>
-    <mergeCell ref="AE35:AG35"/>
-    <mergeCell ref="X37:Z37"/>
-    <mergeCell ref="AE37:AG37"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="X38:Z38"/>
-    <mergeCell ref="AE38:AG38"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="V40:V41"/>
-    <mergeCell ref="AC40:AC41"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="X42:Z42"/>
-    <mergeCell ref="AE42:AG42"/>
-    <mergeCell ref="X44:Z44"/>
-    <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="A1:AP1"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3709,10 +3709,10 @@
   <dimension ref="A1:AP47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -3748,97 +3748,97 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="AJ2" s="25" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AN2" s="25" t="s">
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AN2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-    </row>
-    <row r="3" spans="1:42">
-      <c r="D3" s="25" t="s">
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="R3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="X3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AE3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AJ3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AN3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="R3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="X3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AE3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AJ3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AN3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -3909,11 +3909,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1971</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="21">
@@ -3952,7 +3952,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -3970,7 +3970,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -3988,7 +3988,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -4009,8 +4009,8 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:42">
-      <c r="B6" s="28"/>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B6" s="25"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -4035,7 +4035,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="28"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -4051,7 +4051,7 @@
         <f t="shared" si="2"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="28"/>
+      <c r="V6" s="25"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -4067,7 +4067,7 @@
         <f t="shared" si="0"/>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="28"/>
+      <c r="AC6" s="25"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -4086,35 +4086,35 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:42">
-      <c r="D7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="X7" s="27" t="s">
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="X7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AE7" s="27" t="s">
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AE7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
@@ -4181,7 +4181,7 @@
         <v>1.3794101155854785</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="8" t="s">
@@ -4192,56 +4192,56 @@
         <v>0.41594614744177039</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="X9" s="25" t="s">
+      <c r="X9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="27" t="s">
+      <c r="AE9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
       <c r="AH9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:42">
-      <c r="D10" s="25" t="s">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="2"/>
-      <c r="R10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="X10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AE10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
+      <c r="R10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="X10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AE10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D11" s="2">
         <v>1</v>
       </c>
@@ -4286,11 +4286,11 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:42" ht="16" customHeight="1">
+    <row r="12" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1972</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="21">
@@ -4331,7 +4331,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -4349,7 +4349,7 @@
         <f t="shared" si="7"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="28" t="s">
+      <c r="V12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -4367,7 +4367,7 @@
         <f t="shared" si="8"/>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="28" t="s">
+      <c r="AC12" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -4388,8 +4388,8 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:42">
-      <c r="B13" s="28"/>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B13" s="25"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -4418,7 +4418,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="28"/>
+      <c r="P13" s="25"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -4434,7 +4434,7 @@
         <f t="shared" si="7"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="28"/>
+      <c r="V13" s="25"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -4443,14 +4443,14 @@
         <v>0</v>
       </c>
       <c r="Y13" s="4">
-        <f t="shared" si="8"/>
+        <f>$M13*S13</f>
         <v>22.471288163746728</v>
       </c>
       <c r="Z13" s="4">
         <f t="shared" si="8"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="28"/>
+      <c r="AC13" s="25"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -4469,12 +4469,12 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:42">
-      <c r="D14" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -4482,25 +4482,25 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="27" t="s">
+      <c r="R14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="X14" s="27" t="s">
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="X14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AE14" s="27" t="s">
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AE14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -4573,7 +4573,7 @@
         <v>1.7570566194986847</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -4587,56 +4587,56 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="25" t="s">
+      <c r="X16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
       <c r="AA16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="27" t="s">
+      <c r="AE16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
+      <c r="AF16" s="26"/>
+      <c r="AG16" s="26"/>
       <c r="AH16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:42">
-      <c r="D17" s="25" t="s">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="2"/>
-      <c r="R17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="X17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AE17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
+      <c r="R17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="X17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AE17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D18" s="2">
         <v>1</v>
       </c>
@@ -4681,11 +4681,11 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="1:42" ht="16" customHeight="1">
+    <row r="19" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1973</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="21">
@@ -4726,7 +4726,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="28" t="s">
+      <c r="P19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -4744,7 +4744,7 @@
         <f t="shared" si="14"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="28" t="s">
+      <c r="V19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -4762,7 +4762,7 @@
         <f t="shared" si="15"/>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="28" t="s">
+      <c r="AC19" s="25" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -4783,8 +4783,8 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:42">
-      <c r="B20" s="28"/>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B20" s="25"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -4813,7 +4813,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="28"/>
+      <c r="P20" s="25"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -4829,7 +4829,7 @@
         <f t="shared" si="14"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="28"/>
+      <c r="V20" s="25"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -4845,7 +4845,7 @@
         <f t="shared" si="15"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="28"/>
+      <c r="AC20" s="25"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -4864,12 +4864,12 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:42">
-      <c r="D21" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D21" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -4877,25 +4877,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="27" t="s">
+      <c r="R21" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="X21" s="27" t="s">
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="X21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
-      <c r="AE21" s="27" t="s">
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AE21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="27"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="26"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -4968,7 +4968,7 @@
         <v>2.1227707766832733</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4982,32 +4982,32 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="25" t="s">
+      <c r="X23" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
       <c r="AA23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="27" t="s">
+      <c r="AE23" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="27"/>
-      <c r="AG23" s="27"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="26"/>
       <c r="AH23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:42">
-      <c r="D24" s="25" t="s">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -5043,7 +5043,7 @@
       <c r="AO24" s="9"/>
       <c r="AP24" s="9"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D25" s="2">
         <v>1</v>
       </c>
@@ -5088,11 +5088,11 @@
       <c r="AO25" s="9"/>
       <c r="AP25" s="9"/>
     </row>
-    <row r="26" spans="1:42" ht="16" customHeight="1">
+    <row r="26" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1974</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="21">
@@ -5146,8 +5146,8 @@
       <c r="AO26" s="9"/>
       <c r="AP26" s="9"/>
     </row>
-    <row r="27" spans="1:42">
-      <c r="B27" s="28"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B27" s="25"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -5199,12 +5199,12 @@
       <c r="AO27" s="9"/>
       <c r="AP27" s="9"/>
     </row>
-    <row r="28" spans="1:42">
-      <c r="D28" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -5243,7 +5243,7 @@
       <c r="AO28" s="9"/>
       <c r="AP28" s="9"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -5289,7 +5289,7 @@
       <c r="AO29" s="8"/>
       <c r="AP29" s="8"/>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -5334,7 +5334,7 @@
       <c r="AO30" s="9"/>
       <c r="AP30" s="9"/>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -5369,7 +5369,7 @@
       <c r="AO31" s="9"/>
       <c r="AP31" s="9"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -5404,52 +5404,11 @@
       <c r="AO32" s="9"/>
       <c r="AP32" s="9"/>
     </row>
-    <row r="33" ht="16" customHeight="1"/>
-    <row r="40" ht="16" customHeight="1"/>
-    <row r="47" ht="16" customHeight="1"/>
+    <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="AE21:AG21"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="X7:Z7"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="AN2:AP2"/>
@@ -5459,6 +5418,47 @@
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AJ3:AL3"/>
     <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="AE21:AG21"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="AE23:AG23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added tests for degenerate cases.
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="with matrices - incremental" sheetId="1" r:id="rId1"/>
     <sheet name="with matrices - for testing" sheetId="5" r:id="rId2"/>
+    <sheet name="with matrices - testing degen" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="27">
   <si>
     <t>V</t>
   </si>
@@ -614,7 +615,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -674,10 +675,10 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -685,6 +686,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -1201,7 +1208,7 @@
       <c r="A5">
         <v>1950</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21">
@@ -1240,7 +1247,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -1258,7 +1265,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -1276,7 +1283,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AC5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -1298,7 +1305,7 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -1323,7 +1330,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="30"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -1339,7 +1346,7 @@
         <f t="shared" ref="T6" si="3">LN(F13) - LN(F6)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="25"/>
+      <c r="V6" s="30"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -1355,7 +1362,7 @@
         <f t="shared" ref="Z6" si="5">$M6*T6</f>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="25"/>
+      <c r="AC6" s="30"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -1375,30 +1382,30 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="X7" s="26" t="s">
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="X7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AE7" s="26" t="s">
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AE7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
@@ -1485,11 +1492,11 @@
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
       <c r="AH9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1574,7 +1581,7 @@
       <c r="A12">
         <v>1960</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="21">
@@ -1615,7 +1622,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="P12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -1633,7 +1640,7 @@
         <f t="shared" ref="T12:T13" si="13">LN(F19) - LN(F12)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -1651,7 +1658,7 @@
         <f t="shared" ref="Z12:Z13" si="15">$M12*T12</f>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="25" t="s">
+      <c r="AC12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -1673,7 +1680,7 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -1702,7 +1709,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="25"/>
+      <c r="P13" s="30"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -1718,7 +1725,7 @@
         <f t="shared" si="13"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="30"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -1734,7 +1741,7 @@
         <f t="shared" si="15"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="25"/>
+      <c r="AC13" s="30"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -1754,11 +1761,11 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -1766,21 +1773,21 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="X14" s="26" t="s">
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="X14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AE14" s="26" t="s">
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AE14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
@@ -1880,11 +1887,11 @@
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="26" t="s">
+      <c r="AE16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
       <c r="AH16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1969,7 +1976,7 @@
       <c r="A19">
         <v>1970</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="21">
@@ -2010,7 +2017,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="25" t="s">
+      <c r="P19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -2028,7 +2035,7 @@
         <f t="shared" ref="T19:T20" si="23">LN(F26) - LN(F19)</f>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="25" t="s">
+      <c r="V19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -2046,7 +2053,7 @@
         <f t="shared" ref="Z19:Z20" si="25">$M19*T19</f>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="25" t="s">
+      <c r="AC19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -2068,7 +2075,7 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -2097,7 +2104,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="25"/>
+      <c r="P20" s="30"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -2113,7 +2120,7 @@
         <f t="shared" si="23"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="30"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -2129,7 +2136,7 @@
         <f t="shared" si="25"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="25"/>
+      <c r="AC20" s="30"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -2149,11 +2156,11 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="D21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -2161,21 +2168,21 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="26" t="s">
+      <c r="R21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="X21" s="26" t="s">
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="X21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AE21" s="26" t="s">
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AE21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
@@ -2275,11 +2282,11 @@
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="26" t="s">
+      <c r="AE23" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
       <c r="AH23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2364,7 +2371,7 @@
       <c r="A26">
         <v>1980</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="21">
@@ -2405,7 +2412,7 @@
         <f>M26/L$26</f>
         <v>0.10561476584617054</v>
       </c>
-      <c r="P26" s="25" t="s">
+      <c r="P26" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q26" s="21">
@@ -2423,7 +2430,7 @@
         <f t="shared" ref="T26:T27" si="35">LN(F33) - LN(F26)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V26" s="25" t="s">
+      <c r="V26" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
@@ -2441,7 +2448,7 @@
         <f t="shared" ref="Z26:Z27" si="37">$M26*T26</f>
         <v>7.7700766953751215</v>
       </c>
-      <c r="AC26" s="25" t="s">
+      <c r="AC26" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD26" s="21">
@@ -2463,7 +2470,7 @@
       <c r="AK26" s="1"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -2492,7 +2499,7 @@
         <f>M27/L$26</f>
         <v>0.88988350592239895</v>
       </c>
-      <c r="P27" s="25"/>
+      <c r="P27" s="30"/>
       <c r="Q27" s="21">
         <v>2</v>
       </c>
@@ -2508,7 +2515,7 @@
         <f t="shared" si="35"/>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V27" s="25"/>
+      <c r="V27" s="30"/>
       <c r="W27" s="21">
         <v>2</v>
       </c>
@@ -2524,7 +2531,7 @@
         <f t="shared" si="37"/>
         <v>55.353010514175885</v>
       </c>
-      <c r="AC27" s="25"/>
+      <c r="AC27" s="30"/>
       <c r="AD27" s="21">
         <v>2</v>
       </c>
@@ -2544,11 +2551,11 @@
       <c r="AK27" s="1"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="D28" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2556,21 +2563,21 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="R28" s="26" t="s">
+      <c r="R28" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="X28" s="26" t="s">
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="X28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AE28" s="26" t="s">
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AE28" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF28" s="26"/>
-      <c r="AG28" s="26"/>
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="29"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
@@ -2668,11 +2675,11 @@
         <v>5</v>
       </c>
       <c r="AB30" s="8"/>
-      <c r="AE30" s="26" t="s">
+      <c r="AE30" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF30" s="26"/>
-      <c r="AG30" s="26"/>
+      <c r="AF30" s="29"/>
+      <c r="AG30" s="29"/>
       <c r="AH30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2762,7 @@
       <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="21">
@@ -2795,7 +2802,7 @@
         <f>M33/L$33</f>
         <v>5.7396961403155373E-2</v>
       </c>
-      <c r="P33" s="25" t="s">
+      <c r="P33" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q33" s="21">
@@ -2813,7 +2820,7 @@
         <f t="shared" ref="T33:T34" si="47">LN(F40) - LN(F33)</f>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V33" s="25" t="s">
+      <c r="V33" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W33" s="21">
@@ -2831,7 +2838,7 @@
         <f t="shared" ref="Z33:Z34" si="49">$M33*T33</f>
         <v>5.0235683675903013</v>
       </c>
-      <c r="AC33" s="25" t="s">
+      <c r="AC33" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD33" s="21">
@@ -2853,7 +2860,7 @@
       <c r="AK33" s="1"/>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="21">
         <v>2</v>
       </c>
@@ -2881,7 +2888,7 @@
         <f>M34/L$33</f>
         <v>0.94110538842717861</v>
       </c>
-      <c r="P34" s="25"/>
+      <c r="P34" s="30"/>
       <c r="Q34" s="21">
         <v>2</v>
       </c>
@@ -2897,7 +2904,7 @@
         <f t="shared" si="47"/>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V34" s="25"/>
+      <c r="V34" s="30"/>
       <c r="W34" s="21">
         <v>2</v>
       </c>
@@ -2913,7 +2920,7 @@
         <f t="shared" si="49"/>
         <v>71.350925324956492</v>
       </c>
-      <c r="AC34" s="25"/>
+      <c r="AC34" s="30"/>
       <c r="AD34" s="21">
         <v>2</v>
       </c>
@@ -2933,32 +2940,32 @@
       <c r="AK34" s="1"/>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D35" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="D35" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
       <c r="G35" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="R35" s="26" t="s">
+      <c r="R35" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="X35" s="26" t="s">
+      <c r="S35" s="29"/>
+      <c r="T35" s="29"/>
+      <c r="X35" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AE35" s="26" t="s">
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="29"/>
+      <c r="AE35" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF35" s="26"/>
-      <c r="AG35" s="26"/>
+      <c r="AF35" s="29"/>
+      <c r="AG35" s="29"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
@@ -3056,11 +3063,11 @@
         <v>5</v>
       </c>
       <c r="AB37" s="8"/>
-      <c r="AE37" s="26" t="s">
+      <c r="AE37" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF37" s="26"/>
-      <c r="AG37" s="26"/>
+      <c r="AF37" s="29"/>
+      <c r="AG37" s="29"/>
       <c r="AH37" s="1" t="s">
         <v>11</v>
       </c>
@@ -3143,7 +3150,7 @@
       <c r="A40">
         <v>2000</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="21">
@@ -3183,7 +3190,7 @@
         <f>M40/L$40</f>
         <v>2.5568845446814027E-2</v>
       </c>
-      <c r="P40" s="25" t="s">
+      <c r="P40" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q40" s="21">
@@ -3201,7 +3208,7 @@
         <f t="shared" ref="T40:T41" si="59">LN(F47) - LN(F40)</f>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V40" s="25" t="s">
+      <c r="V40" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W40" s="21">
@@ -3219,7 +3226,7 @@
         <f t="shared" ref="Z40:Z41" si="61">$M40*T40</f>
         <v>2.665651423580965</v>
       </c>
-      <c r="AC40" s="25" t="s">
+      <c r="AC40" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD40" s="21">
@@ -3241,7 +3248,7 @@
       <c r="AK40" s="1"/>
     </row>
     <row r="41" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B41" s="25"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="21">
         <v>2</v>
       </c>
@@ -3269,7 +3276,7 @@
         <f>M41/L$40</f>
         <v>0.97162630393947746</v>
       </c>
-      <c r="P41" s="25"/>
+      <c r="P41" s="30"/>
       <c r="Q41" s="21">
         <v>2</v>
       </c>
@@ -3285,7 +3292,7 @@
         <f t="shared" si="59"/>
         <v>0.11778303565638382</v>
       </c>
-      <c r="V41" s="25"/>
+      <c r="V41" s="30"/>
       <c r="W41" s="21">
         <v>2</v>
       </c>
@@ -3301,7 +3308,7 @@
         <f t="shared" si="61"/>
         <v>89.349241143602967</v>
       </c>
-      <c r="AC41" s="25"/>
+      <c r="AC41" s="30"/>
       <c r="AD41" s="21">
         <v>2</v>
       </c>
@@ -3321,32 +3328,32 @@
       <c r="AK41" s="1"/>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D42" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+      <c r="D42" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
       <c r="G42" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="R42" s="26" t="s">
+      <c r="R42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="X42" s="26" t="s">
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="X42" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Y42" s="26"/>
-      <c r="Z42" s="26"/>
-      <c r="AE42" s="26" t="s">
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AE42" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF42" s="26"/>
-      <c r="AG42" s="26"/>
+      <c r="AF42" s="29"/>
+      <c r="AG42" s="29"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
@@ -3444,11 +3451,11 @@
         <v>5</v>
       </c>
       <c r="AB44" s="8"/>
-      <c r="AE44" s="26" t="s">
+      <c r="AE44" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF44" s="26"/>
-      <c r="AG44" s="26"/>
+      <c r="AF44" s="29"/>
+      <c r="AG44" s="29"/>
       <c r="AH44" s="1" t="s">
         <v>11</v>
       </c>
@@ -3481,7 +3488,7 @@
       <c r="A47">
         <v>2010</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="21">
@@ -3504,7 +3511,7 @@
       <c r="AK47" s="1"/>
     </row>
     <row r="48" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B48" s="25"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="21">
         <v>2</v>
       </c>
@@ -3525,11 +3532,11 @@
       <c r="AK48" s="1"/>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D49" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
+      <c r="D49" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
       <c r="G49" s="7" t="s">
         <v>4</v>
       </c>
@@ -3606,50 +3613,38 @@
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="A1:AP1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="X42:Z42"/>
-    <mergeCell ref="AE42:AG42"/>
-    <mergeCell ref="X44:Z44"/>
-    <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="X38:Z38"/>
-    <mergeCell ref="AE38:AG38"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="V40:V41"/>
-    <mergeCell ref="AC40:AC41"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="X35:Z35"/>
-    <mergeCell ref="AE35:AG35"/>
-    <mergeCell ref="X37:Z37"/>
-    <mergeCell ref="AE37:AG37"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="V33:V34"/>
-    <mergeCell ref="AC33:AC34"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="X28:Z28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="X30:Z30"/>
-    <mergeCell ref="AE30:AG30"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AE24:AG24"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE9:AG9"/>
     <mergeCell ref="AE16:AG16"/>
     <mergeCell ref="X9:Z9"/>
     <mergeCell ref="X16:Z16"/>
@@ -3666,38 +3661,50 @@
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="X23:Z23"/>
     <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="AE30:AG30"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="AC33:AC34"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="X35:Z35"/>
+    <mergeCell ref="AE35:AG35"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="AE37:AG37"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="X38:Z38"/>
+    <mergeCell ref="AE38:AG38"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="V40:V41"/>
+    <mergeCell ref="AC40:AC41"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="X42:Z42"/>
+    <mergeCell ref="AE42:AG42"/>
+    <mergeCell ref="X44:Z44"/>
+    <mergeCell ref="AE44:AG44"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="A1:AP1"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3708,7 +3715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3913,7 +3920,7 @@
       <c r="A5">
         <v>1971</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="21">
@@ -3952,7 +3959,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -3970,7 +3977,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -3988,7 +3995,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AC5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -4010,7 +4017,7 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -4035,7 +4042,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="30"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -4051,7 +4058,7 @@
         <f t="shared" si="2"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="25"/>
+      <c r="V6" s="30"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -4067,7 +4074,7 @@
         <f t="shared" si="0"/>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="25"/>
+      <c r="AC6" s="30"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -4087,30 +4094,30 @@
       <c r="AK6" s="2"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="X7" s="26" t="s">
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="X7" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AE7" s="26" t="s">
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AE7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
@@ -4201,11 +4208,11 @@
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
       <c r="AH9" s="2" t="s">
         <v>11</v>
       </c>
@@ -4290,7 +4297,7 @@
       <c r="A12">
         <v>1972</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="21">
@@ -4331,7 +4338,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="P12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -4349,7 +4356,7 @@
         <f t="shared" si="7"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -4367,7 +4374,7 @@
         <f t="shared" si="8"/>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="25" t="s">
+      <c r="AC12" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -4389,7 +4396,7 @@
       <c r="AK12" s="2"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -4418,7 +4425,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="25"/>
+      <c r="P13" s="30"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -4434,7 +4441,7 @@
         <f t="shared" si="7"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="30"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -4450,7 +4457,7 @@
         <f t="shared" si="8"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="25"/>
+      <c r="AC13" s="30"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -4470,11 +4477,11 @@
       <c r="AK13" s="2"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -4482,21 +4489,21 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="X14" s="26" t="s">
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="X14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AE14" s="26" t="s">
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AE14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
@@ -4596,11 +4603,11 @@
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="26" t="s">
+      <c r="AE16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
       <c r="AH16" s="2" t="s">
         <v>11</v>
       </c>
@@ -4685,7 +4692,7 @@
       <c r="A19">
         <v>1973</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="21">
@@ -4726,7 +4733,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="25" t="s">
+      <c r="P19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -4744,7 +4751,7 @@
         <f t="shared" si="14"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="25" t="s">
+      <c r="V19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -4762,7 +4769,7 @@
         <f t="shared" si="15"/>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="25" t="s">
+      <c r="AC19" s="30" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -4784,7 +4791,7 @@
       <c r="AK19" s="2"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -4813,7 +4820,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="25"/>
+      <c r="P20" s="30"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -4829,7 +4836,7 @@
         <f t="shared" si="14"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="30"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -4845,7 +4852,7 @@
         <f t="shared" si="15"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="25"/>
+      <c r="AC20" s="30"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -4865,11 +4872,11 @@
       <c r="AK20" s="2"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="D21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -4877,21 +4884,21 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="26" t="s">
+      <c r="R21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="X21" s="26" t="s">
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="X21" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AE21" s="26" t="s">
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AE21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
@@ -4991,11 +4998,11 @@
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="26" t="s">
+      <c r="AE23" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
       <c r="AH23" s="2" t="s">
         <v>11</v>
       </c>
@@ -5092,7 +5099,7 @@
       <c r="A26">
         <v>1974</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="21">
@@ -5147,7 +5154,7 @@
       <c r="AP26" s="9"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -5200,11 +5207,11 @@
       <c r="AP27" s="9"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="D28" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -5409,6 +5416,47 @@
     <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="AE21:AG21"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="X7:Z7"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="AN2:AP2"/>
@@ -5418,6 +5466,1751 @@
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AJ3:AL3"/>
     <mergeCell ref="AN3:AP3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" customWidth="1"/>
+    <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.6640625" customWidth="1"/>
+    <col min="16" max="16" width="6" customWidth="1"/>
+    <col min="17" max="23" width="5.5" customWidth="1"/>
+    <col min="24" max="27" width="5.6640625" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" style="9" customWidth="1"/>
+    <col min="29" max="29" width="4.83203125" customWidth="1"/>
+    <col min="30" max="30" width="5" customWidth="1"/>
+    <col min="31" max="34" width="5.83203125" customWidth="1"/>
+    <col min="35" max="35" width="7.1640625" customWidth="1"/>
+    <col min="36" max="37" width="7.33203125" customWidth="1"/>
+    <col min="38" max="38" width="4.83203125" customWidth="1"/>
+    <col min="39" max="39" width="5.6640625" customWidth="1"/>
+    <col min="40" max="43" width="6.1640625" customWidth="1"/>
+    <col min="44" max="45" width="6.33203125" customWidth="1"/>
+    <col min="46" max="46" width="4.5" customWidth="1"/>
+    <col min="47" max="47" width="8.83203125" customWidth="1"/>
+    <col min="49" max="49" width="4.5" customWidth="1"/>
+    <col min="50" max="50" width="7.6640625" customWidth="1"/>
+    <col min="51" max="51" width="6.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AN2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D3" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="R3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="X3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AE3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AJ3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AN3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2</v>
+      </c>
+      <c r="F4" s="26">
+        <v>3</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="26">
+        <v>1</v>
+      </c>
+      <c r="S4" s="26">
+        <v>2</v>
+      </c>
+      <c r="T4" s="26">
+        <v>3</v>
+      </c>
+      <c r="X4" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="26">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="26">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="26">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="26">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="26">
+        <v>3</v>
+      </c>
+      <c r="AJ4" s="26">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL4" s="26">
+        <v>3</v>
+      </c>
+      <c r="AN4" s="26">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="26">
+        <v>2</v>
+      </c>
+      <c r="AP4" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1971</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="12">
+        <f>PRODUCT(D5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <f>G15/G8</f>
+        <v>3</v>
+      </c>
+      <c r="J5" s="18">
+        <f>G15-G8</f>
+        <v>120</v>
+      </c>
+      <c r="L5" s="14">
+        <f>(G15-G8) / (LN(G15) - LN(G8))</f>
+        <v>109.22870719522045</v>
+      </c>
+      <c r="M5" s="15" t="e">
+        <f>(G12-G5) / (LN(G12) - LN(G5))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N5" s="16" t="e">
+        <f>M5/L$5</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4" t="e">
+        <f>LN(D12) - LN(D5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S5" s="4">
+        <f>LN(E12) - LN(E5)</f>
+        <v>-0.69314718055994562</v>
+      </c>
+      <c r="T5" s="4">
+        <f>LN(F12) - LN(F5)</f>
+        <v>0.4054651081081645</v>
+      </c>
+      <c r="V5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="21">
+        <v>1</v>
+      </c>
+      <c r="X5" s="4" t="e">
+        <f>$M5*R5</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y5" s="4" t="e">
+        <f t="shared" ref="Y5:Z6" si="0">$M5*S5</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z5" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AC5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="4" t="e">
+        <f>$N5*R5</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AF5" s="4" t="e">
+        <f t="shared" ref="AF5:AG6" si="1">$N5*S5</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AG5" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B6" s="30"/>
+      <c r="C6" s="21">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="12">
+        <f>PRODUCT(D6:F6)</f>
+        <v>60</v>
+      </c>
+      <c r="M6" s="15">
+        <f>(G13-G6) / (LN(G13) - LN(G6))</f>
+        <v>86.561702453337787</v>
+      </c>
+      <c r="N6" s="16">
+        <f>M6/L$5</f>
+        <v>0.79248125036057815</v>
+      </c>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="21">
+        <v>2</v>
+      </c>
+      <c r="R6" s="4">
+        <f>LN(D13) - LN(D6)</f>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" ref="S6:T6" si="2">LN(E13) - LN(E6)</f>
+        <v>0.18232155679395468</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.28768207245178079</v>
+      </c>
+      <c r="V6" s="30"/>
+      <c r="W6" s="21">
+        <v>2</v>
+      </c>
+      <c r="X6" s="4">
+        <f>$M6*R6</f>
+        <v>19.315685693241733</v>
+      </c>
+      <c r="Y6" s="4">
+        <f t="shared" si="0"/>
+        <v>15.782064350027632</v>
+      </c>
+      <c r="Z6" s="4">
+        <f t="shared" si="0"/>
+        <v>24.902249956730611</v>
+      </c>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="4">
+        <f>$N6*R6</f>
+        <v>0.17683708055538475</v>
+      </c>
+      <c r="AF6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14448641529576037</v>
+      </c>
+      <c r="AG6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.22798264848290967</v>
+      </c>
+      <c r="AJ6" s="26"/>
+      <c r="AK6" s="26"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D7" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="26"/>
+      <c r="R7" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="X7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AE7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AJ7" s="26"/>
+      <c r="AK7" s="26"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13">
+        <f>SUM(G5:G6)</f>
+        <v>60</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="N8" s="26"/>
+      <c r="X8" s="4" t="e">
+        <f>SUM(X5:X6)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y8" s="4" t="e">
+        <f t="shared" ref="Y8:Z8" si="3">SUM(Y5:Y6)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z8" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AA8" s="18" t="e">
+        <f>SUM(X8:Z8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB8" s="19"/>
+      <c r="AE8" s="4" t="e">
+        <f>EXP(SUM(AE5:AE6))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AF8" s="4" t="e">
+        <f t="shared" ref="AF8:AG8" si="4">EXP(SUM(AF5:AF6))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AG8" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH8" s="17" t="e">
+        <f>PRODUCT(AE8:AG8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ8" s="4" t="e">
+        <f>X8</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AK8" s="4" t="e">
+        <f t="shared" ref="AK8:AL8" si="5">Y8</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AL8" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AN8" s="4" t="e">
+        <f>AE8</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AO8" s="4" t="e">
+        <f t="shared" ref="AO8:AP8" si="6">AF8</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AP8" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="G9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>M6/L12</f>
+        <v>0.41594614744177039</v>
+      </c>
+      <c r="N9" s="26"/>
+      <c r="X9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB9" s="8"/>
+      <c r="AE9" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D10" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="N10" s="26"/>
+      <c r="R10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="X10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AE10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D11" s="26">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26">
+        <v>2</v>
+      </c>
+      <c r="F11" s="26">
+        <v>3</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="N11" s="26"/>
+      <c r="R11" s="26">
+        <v>1</v>
+      </c>
+      <c r="S11" s="26">
+        <v>2</v>
+      </c>
+      <c r="T11" s="26">
+        <v>3</v>
+      </c>
+      <c r="X11" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="26">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="26">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="26">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="26">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="26">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="26"/>
+      <c r="AK11" s="26"/>
+    </row>
+    <row r="12" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1972</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="12">
+        <f>PRODUCT(D12:F12)</f>
+        <v>60</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="17">
+        <f>G22/G15</f>
+        <v>1.3277777777777777</v>
+      </c>
+      <c r="J12" s="18">
+        <f>G22-G15</f>
+        <v>59</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="L12" s="14">
+        <f>(G22-G15) / (LN(G22) - LN(G15))</f>
+        <v>208.10795576717257</v>
+      </c>
+      <c r="M12" s="15">
+        <f>(G19-G12) / (LN(G19) - LN(G12))</f>
+        <v>61.978488652901611</v>
+      </c>
+      <c r="N12" s="16">
+        <f>M12/L$12</f>
+        <v>0.29781892972050539</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>1</v>
+      </c>
+      <c r="R12" s="4">
+        <f>LN(D19) - LN(D12)</f>
+        <v>0.69314718055994518</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" ref="S12:T13" si="7">LN(E19) - LN(E12)</f>
+        <v>-0.916290731874155</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="7"/>
+        <v>0.28768207245178079</v>
+      </c>
+      <c r="V12" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="W12" s="21">
+        <v>1</v>
+      </c>
+      <c r="X12" s="4">
+        <f>$M12*R12</f>
+        <v>42.960214665125307</v>
+      </c>
+      <c r="Y12" s="4">
+        <f t="shared" ref="Y12:Z13" si="8">$M12*S12</f>
+        <v>-56.790314728221226</v>
+      </c>
+      <c r="Z12" s="4">
+        <f t="shared" si="8"/>
+        <v>17.830100063095916</v>
+      </c>
+      <c r="AC12" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="4">
+        <f>$N12*R12</f>
+        <v>0.20643235145314878</v>
+      </c>
+      <c r="AF12" s="4">
+        <f t="shared" ref="AF12:AG13" si="9">$N12*S12</f>
+        <v>-0.2728887250795794</v>
+      </c>
+      <c r="AG12" s="4">
+        <f t="shared" si="9"/>
+        <v>8.5677166917366238E-2</v>
+      </c>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B13" s="30"/>
+      <c r="C13" s="21">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4</v>
+      </c>
+      <c r="G13" s="12">
+        <f>PRODUCT(D13:F13)</f>
+        <v>120</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="M13" s="15">
+        <f>(G20-G13) / (LN(G20) - LN(G13))</f>
+        <v>145.77482362664972</v>
+      </c>
+      <c r="N13" s="16">
+        <f>M13/L$12</f>
+        <v>0.70047693798760857</v>
+      </c>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="21">
+        <v>2</v>
+      </c>
+      <c r="R13" s="4">
+        <f>LN(D20) - LN(D13)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="7"/>
+        <v>0.15415067982725827</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="7"/>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="V13" s="30"/>
+      <c r="W13" s="21">
+        <v>2</v>
+      </c>
+      <c r="X13" s="4">
+        <f>$M13*R13</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="4">
+        <f>$M13*S13</f>
+        <v>22.471288163746728</v>
+      </c>
+      <c r="Z13" s="4">
+        <f t="shared" si="8"/>
+        <v>32.52871183625318</v>
+      </c>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="4">
+        <f>$N13*R13</f>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="4">
+        <f t="shared" si="9"/>
+        <v>0.1079789961941061</v>
+      </c>
+      <c r="AG13" s="4">
+        <f t="shared" si="9"/>
+        <v>0.15630691155625842</v>
+      </c>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="R14" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="X14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AE14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="26"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="13">
+        <f>SUM(G12:G13)</f>
+        <v>180</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="X15" s="4">
+        <f>SUM(X12:X13)</f>
+        <v>42.960214665125307</v>
+      </c>
+      <c r="Y15" s="4">
+        <f t="shared" ref="Y15:Z15" si="10">SUM(Y12:Y13)</f>
+        <v>-34.319026564474498</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" si="10"/>
+        <v>50.358811899349092</v>
+      </c>
+      <c r="AA15" s="18">
+        <f>SUM(X15:Z15)</f>
+        <v>58.999999999999901</v>
+      </c>
+      <c r="AB15" s="19"/>
+      <c r="AE15" s="4">
+        <f>EXP(SUM(AE12:AE13))</f>
+        <v>1.2292845720892271</v>
+      </c>
+      <c r="AF15" s="4">
+        <f t="shared" ref="AF15:AG15" si="11">EXP(SUM(AF12:AF13))</f>
+        <v>0.84797024785237751</v>
+      </c>
+      <c r="AG15" s="4">
+        <f t="shared" si="11"/>
+        <v>1.2737739122298066</v>
+      </c>
+      <c r="AH15" s="17">
+        <f>PRODUCT(AE15:AG15)</f>
+        <v>1.3277777777777777</v>
+      </c>
+      <c r="AJ15" s="4" t="e">
+        <f>AJ8+X15</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AK15" s="4" t="e">
+        <f t="shared" ref="AK15:AL15" si="12">AK8+Y15</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AL15" s="4" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AN15" s="4" t="e">
+        <f>AN8*AE15</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AO15" s="4" t="e">
+        <f t="shared" ref="AO15:AP15" si="13">AO8*AF15</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AP15" s="4" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="X16" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="8"/>
+      <c r="AE16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ16" s="26"/>
+      <c r="AK16" s="26"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D17" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="N17" s="26"/>
+      <c r="R17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="X17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AE17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
+      <c r="AJ17" s="26"/>
+      <c r="AK17" s="26"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D18" s="26">
+        <v>1</v>
+      </c>
+      <c r="E18" s="26">
+        <v>2</v>
+      </c>
+      <c r="F18" s="26">
+        <v>3</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="N18" s="26"/>
+      <c r="R18" s="26">
+        <v>1</v>
+      </c>
+      <c r="S18" s="26">
+        <v>2</v>
+      </c>
+      <c r="T18" s="26">
+        <v>3</v>
+      </c>
+      <c r="X18" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="26">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="26">
+        <v>3</v>
+      </c>
+      <c r="AE18" s="26">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="26">
+        <v>2</v>
+      </c>
+      <c r="AG18" s="26">
+        <v>3</v>
+      </c>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="26"/>
+    </row>
+    <row r="19" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1973</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="21">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4</v>
+      </c>
+      <c r="G19" s="12">
+        <f>PRODUCT(D19:F19)</f>
+        <v>64</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="17">
+        <f>G29/G22</f>
+        <v>1.4142259414225942</v>
+      </c>
+      <c r="J19" s="18">
+        <f>G29-G22</f>
+        <v>99</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="14">
+        <f>(G29-G22) / (LN(G29) - LN(G22))</f>
+        <v>285.64640363823662</v>
+      </c>
+      <c r="M19" s="15">
+        <f>(G26-G19) / (LN(G26) - LN(G19))</f>
+        <v>56.712288666956283</v>
+      </c>
+      <c r="N19" s="16">
+        <f>M19/L$19</f>
+        <v>0.19854018095316492</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>1</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" ref="R19:T20" si="14">LN(D26) - LN(D19)</f>
+        <v>0.22314355131421015</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="14"/>
+        <v>-0.69314718055994529</v>
+      </c>
+      <c r="T19" s="4">
+        <f t="shared" si="14"/>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="V19" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="W19" s="21">
+        <v>1</v>
+      </c>
+      <c r="X19" s="4">
+        <f>$M19*R19</f>
+        <v>12.654981496301259</v>
+      </c>
+      <c r="Y19" s="4">
+        <f t="shared" ref="Y19:Z20" si="15">$M19*S19</f>
+        <v>-39.309962992602486</v>
+      </c>
+      <c r="Z19" s="4">
+        <f t="shared" si="15"/>
+        <v>12.654981496301232</v>
+      </c>
+      <c r="AC19" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="4">
+        <f>$N19*R19</f>
+        <v>4.4302961056455127E-2</v>
+      </c>
+      <c r="AF19" s="4">
+        <f t="shared" ref="AF19:AG20" si="16">$N19*S19</f>
+        <v>-0.13761756665554761</v>
+      </c>
+      <c r="AG19" s="4">
+        <f t="shared" si="16"/>
+        <v>4.4302961056455037E-2</v>
+      </c>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B20" s="30"/>
+      <c r="C20" s="21">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5</v>
+      </c>
+      <c r="G20" s="12">
+        <f>PRODUCT(D20:F20)</f>
+        <v>175</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="M20" s="15">
+        <f>(G27-G20) / (LN(G27) - LN(G20))</f>
+        <v>226.82814674545895</v>
+      </c>
+      <c r="N20" s="16">
+        <f>M20/L$19</f>
+        <v>0.79408717861097466</v>
+      </c>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="21">
+        <v>2</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" si="14"/>
+        <v>0.18232155679395468</v>
+      </c>
+      <c r="S20" s="4">
+        <f t="shared" si="14"/>
+        <v>0.13353139262452252</v>
+      </c>
+      <c r="T20" s="4">
+        <f t="shared" si="14"/>
+        <v>0.18232155679395468</v>
+      </c>
+      <c r="V20" s="30"/>
+      <c r="W20" s="21">
+        <v>2</v>
+      </c>
+      <c r="X20" s="4">
+        <f>$M20*R20</f>
+        <v>41.355660839319683</v>
+      </c>
+      <c r="Y20" s="4">
+        <f t="shared" si="15"/>
+        <v>30.288678321360688</v>
+      </c>
+      <c r="Z20" s="4">
+        <f t="shared" si="15"/>
+        <v>41.355660839319683</v>
+      </c>
+      <c r="AC20" s="30"/>
+      <c r="AD20" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE20" s="4">
+        <f>$N20*R20</f>
+        <v>0.14477921063447205</v>
+      </c>
+      <c r="AF20" s="4">
+        <f t="shared" si="16"/>
+        <v>0.10603556682520139</v>
+      </c>
+      <c r="AG20" s="4">
+        <f t="shared" si="16"/>
+        <v>0.14477921063447205</v>
+      </c>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="R21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="X21" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AE21" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+      <c r="AJ21" s="26"/>
+      <c r="AK21" s="26"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="13">
+        <f>SUM(G19:G20)</f>
+        <v>239</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="X22" s="4">
+        <f>SUM(X19:X20)</f>
+        <v>54.010642335620943</v>
+      </c>
+      <c r="Y22" s="4">
+        <f t="shared" ref="Y22:Z22" si="17">SUM(Y19:Y20)</f>
+        <v>-9.0212846712417978</v>
+      </c>
+      <c r="Z22" s="4">
+        <f t="shared" si="17"/>
+        <v>54.010642335620915</v>
+      </c>
+      <c r="AA22" s="18">
+        <f>SUM(X22:Z22)</f>
+        <v>99.000000000000057</v>
+      </c>
+      <c r="AB22" s="19"/>
+      <c r="AE22" s="4">
+        <f>EXP(SUM(AE19:AE20))</f>
+        <v>1.2081402233292473</v>
+      </c>
+      <c r="AF22" s="4">
+        <f t="shared" ref="AF22:AG22" si="18">EXP(SUM(AF19:AF20))</f>
+        <v>0.96891150261734849</v>
+      </c>
+      <c r="AG22" s="4">
+        <f t="shared" si="18"/>
+        <v>1.2081402233292473</v>
+      </c>
+      <c r="AH22" s="17">
+        <f>PRODUCT(AE22:AG22)</f>
+        <v>1.4142259414225939</v>
+      </c>
+      <c r="AJ22" s="4" t="e">
+        <f>AJ15+X22</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AK22" s="4" t="e">
+        <f t="shared" ref="AK22:AL22" si="19">AK15+Y22</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AL22" s="4" t="e">
+        <f t="shared" si="19"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AN22" s="4" t="e">
+        <f>AN15*AE22</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AO22" s="4" t="e">
+        <f t="shared" ref="AO22:AP22" si="20">AO15*AF22</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AP22" s="4" t="e">
+        <f t="shared" si="20"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="X23" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="8"/>
+      <c r="AE23" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ23" s="26"/>
+      <c r="AK23" s="26"/>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="10"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="9"/>
+      <c r="AM24" s="9"/>
+      <c r="AN24" s="9"/>
+      <c r="AO24" s="9"/>
+      <c r="AP24" s="9"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D25" s="26">
+        <v>1</v>
+      </c>
+      <c r="E25" s="26">
+        <v>2</v>
+      </c>
+      <c r="F25" s="26">
+        <v>3</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="8"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="9"/>
+      <c r="AM25" s="9"/>
+      <c r="AN25" s="9"/>
+      <c r="AO25" s="9"/>
+      <c r="AP25" s="9"/>
+    </row>
+    <row r="26" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1974</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5</v>
+      </c>
+      <c r="G26" s="12">
+        <f>PRODUCT(D26:F26)</f>
+        <v>50</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="9"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="22"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="9"/>
+      <c r="AP26" s="9"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B27" s="30"/>
+      <c r="C27" s="21">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4">
+        <v>8</v>
+      </c>
+      <c r="F27" s="4">
+        <v>6</v>
+      </c>
+      <c r="G27" s="12">
+        <f>PRODUCT(D27:F27)</f>
+        <v>288</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="9"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="22"/>
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="9"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="9"/>
+      <c r="AO27" s="9"/>
+      <c r="AP27" s="9"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="24"/>
+      <c r="AF28" s="24"/>
+      <c r="AG28" s="24"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="8"/>
+      <c r="AK28" s="8"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="9"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="13">
+        <f>SUM(G26:G27)</f>
+        <v>338</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="8"/>
+      <c r="AF29" s="8"/>
+      <c r="AG29" s="8"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="8"/>
+      <c r="AK29" s="8"/>
+      <c r="AL29" s="8"/>
+      <c r="AM29" s="9"/>
+      <c r="AN29" s="8"/>
+      <c r="AO29" s="8"/>
+      <c r="AP29" s="8"/>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="8"/>
+      <c r="AB30" s="8"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="24"/>
+      <c r="AF30" s="24"/>
+      <c r="AG30" s="24"/>
+      <c r="AH30" s="8"/>
+      <c r="AI30" s="9"/>
+      <c r="AJ30" s="8"/>
+      <c r="AK30" s="8"/>
+      <c r="AL30" s="9"/>
+      <c r="AM30" s="9"/>
+      <c r="AN30" s="9"/>
+      <c r="AO30" s="9"/>
+      <c r="AP30" s="9"/>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
+      <c r="AM31" s="9"/>
+      <c r="AN31" s="9"/>
+      <c r="AO31" s="9"/>
+      <c r="AP31" s="9"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="9"/>
+      <c r="AL32" s="9"/>
+      <c r="AM32" s="9"/>
+      <c r="AN32" s="9"/>
+      <c r="AO32" s="9"/>
+      <c r="AP32" s="9"/>
+    </row>
+    <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="50">
+    <mergeCell ref="AE21:AG21"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AE10:AG10"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="V5:V6"/>
@@ -5425,40 +7218,15 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="R7:T7"/>
     <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="AE21:AG21"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="A1:AP1"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AN3:AP3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Saved the .xlsx; no real changes.
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28700" windowHeight="17520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="with matrices - incremental" sheetId="1" r:id="rId1"/>
     <sheet name="with matrices - for testing" sheetId="5" r:id="rId2"/>
-    <sheet name="with matrices - testing degen" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="27">
   <si>
     <t>V</t>
   </si>
@@ -615,7 +614,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,12 +674,6 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1044,94 +1037,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="AJ2" s="27" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AN2" s="27" t="s">
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AN2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="X3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AE3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AJ3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AN3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="R3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="X3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AE3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AJ3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AN3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D4" s="1">
@@ -1208,7 +1201,7 @@
       <c r="A5">
         <v>1950</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21">
@@ -1247,7 +1240,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -1265,7 +1258,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="30" t="s">
+      <c r="V5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -1283,7 +1276,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="30" t="s">
+      <c r="AC5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -1305,7 +1298,7 @@
       <c r="AK5" s="1"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -1330,7 +1323,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="30"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -1346,7 +1339,7 @@
         <f t="shared" ref="T6" si="3">LN(F13) - LN(F6)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="30"/>
+      <c r="V6" s="28"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -1362,7 +1355,7 @@
         <f t="shared" ref="Z6" si="5">$M6*T6</f>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="30"/>
+      <c r="AC6" s="28"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -1382,30 +1375,30 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="D7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="R7" s="29" t="s">
+      <c r="R7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="X7" s="29" t="s">
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="X7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AE7" s="29" t="s">
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AE7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
@@ -1483,20 +1476,20 @@
         <v>0</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="X9" s="27" t="s">
+      <c r="X9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
       <c r="AA9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="29" t="s">
+      <c r="AE9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
       <c r="AH9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1504,31 +1497,31 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="1"/>
-      <c r="R10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="X10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AE10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
+      <c r="R10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="X10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AE10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
@@ -1581,7 +1574,7 @@
       <c r="A12">
         <v>1960</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="21">
@@ -1622,7 +1615,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="30" t="s">
+      <c r="P12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -1640,7 +1633,7 @@
         <f t="shared" ref="T12:T13" si="13">LN(F19) - LN(F12)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="30" t="s">
+      <c r="V12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -1658,7 +1651,7 @@
         <f t="shared" ref="Z12:Z13" si="15">$M12*T12</f>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="30" t="s">
+      <c r="AC12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -1680,7 +1673,7 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -1709,7 +1702,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="30"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -1725,7 +1718,7 @@
         <f t="shared" si="13"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="30"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -1741,7 +1734,7 @@
         <f t="shared" si="15"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="30"/>
+      <c r="AC13" s="28"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -1761,11 +1754,11 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="D14" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -1773,21 +1766,21 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="29" t="s">
+      <c r="R14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="X14" s="29" t="s">
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="X14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-      <c r="AE14" s="29" t="s">
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AE14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
@@ -1878,20 +1871,20 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="27" t="s">
+      <c r="X16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
       <c r="AA16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="29" t="s">
+      <c r="AE16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1899,31 +1892,31 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="1"/>
-      <c r="R17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="X17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AE17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
+      <c r="R17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="X17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AE17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
@@ -1976,7 +1969,7 @@
       <c r="A19">
         <v>1970</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="21">
@@ -2017,7 +2010,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="30" t="s">
+      <c r="P19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -2035,7 +2028,7 @@
         <f t="shared" ref="T19:T20" si="23">LN(F26) - LN(F19)</f>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="30" t="s">
+      <c r="V19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -2053,7 +2046,7 @@
         <f t="shared" ref="Z19:Z20" si="25">$M19*T19</f>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="30" t="s">
+      <c r="AC19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -2075,7 +2068,7 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -2104,7 +2097,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="30"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -2120,7 +2113,7 @@
         <f t="shared" si="23"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="30"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -2136,7 +2129,7 @@
         <f t="shared" si="25"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="30"/>
+      <c r="AC20" s="28"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -2156,11 +2149,11 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="D21" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -2168,21 +2161,21 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="29" t="s">
+      <c r="R21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="X21" s="29" t="s">
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="X21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-      <c r="AE21" s="29" t="s">
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AE21" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
@@ -2273,20 +2266,20 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="27" t="s">
+      <c r="X23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
       <c r="AA23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="29" t="s">
+      <c r="AE23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="29"/>
-      <c r="AG23" s="29"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
       <c r="AH23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2294,31 +2287,31 @@
       <c r="AK23" s="1"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="N24" s="1"/>
-      <c r="R24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="X24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AE24" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="27"/>
+      <c r="R24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="X24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AE24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
@@ -2371,7 +2364,7 @@
       <c r="A26">
         <v>1980</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="21">
@@ -2412,7 +2405,7 @@
         <f>M26/L$26</f>
         <v>0.10561476584617054</v>
       </c>
-      <c r="P26" s="30" t="s">
+      <c r="P26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q26" s="21">
@@ -2430,7 +2423,7 @@
         <f t="shared" ref="T26:T27" si="35">LN(F33) - LN(F26)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V26" s="30" t="s">
+      <c r="V26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
@@ -2448,7 +2441,7 @@
         <f t="shared" ref="Z26:Z27" si="37">$M26*T26</f>
         <v>7.7700766953751215</v>
       </c>
-      <c r="AC26" s="30" t="s">
+      <c r="AC26" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD26" s="21">
@@ -2470,7 +2463,7 @@
       <c r="AK26" s="1"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="30"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -2499,7 +2492,7 @@
         <f>M27/L$26</f>
         <v>0.88988350592239895</v>
       </c>
-      <c r="P27" s="30"/>
+      <c r="P27" s="28"/>
       <c r="Q27" s="21">
         <v>2</v>
       </c>
@@ -2515,7 +2508,7 @@
         <f t="shared" si="35"/>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V27" s="30"/>
+      <c r="V27" s="28"/>
       <c r="W27" s="21">
         <v>2</v>
       </c>
@@ -2531,7 +2524,7 @@
         <f t="shared" si="37"/>
         <v>55.353010514175885</v>
       </c>
-      <c r="AC27" s="30"/>
+      <c r="AC27" s="28"/>
       <c r="AD27" s="21">
         <v>2</v>
       </c>
@@ -2551,11 +2544,11 @@
       <c r="AK27" s="1"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="D28" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2563,21 +2556,21 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="R28" s="29" t="s">
+      <c r="R28" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="X28" s="29" t="s">
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="X28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="29"/>
-      <c r="AE28" s="29" t="s">
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AE28" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF28" s="29"/>
-      <c r="AG28" s="29"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="27"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
@@ -2666,20 +2659,20 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="X30" s="27" t="s">
+      <c r="X30" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="27"/>
+      <c r="Y30" s="25"/>
+      <c r="Z30" s="25"/>
       <c r="AA30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB30" s="8"/>
-      <c r="AE30" s="29" t="s">
+      <c r="AE30" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF30" s="29"/>
-      <c r="AG30" s="29"/>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
       <c r="AH30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2687,30 +2680,30 @@
       <c r="AK30" s="1"/>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="N31" s="1"/>
-      <c r="R31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="X31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="27"/>
-      <c r="Z31" s="27"/>
-      <c r="AE31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="27"/>
-      <c r="AG31" s="27"/>
+      <c r="R31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="X31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AE31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
@@ -2762,7 +2755,7 @@
       <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="21">
@@ -2802,7 +2795,7 @@
         <f>M33/L$33</f>
         <v>5.7396961403155373E-2</v>
       </c>
-      <c r="P33" s="30" t="s">
+      <c r="P33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q33" s="21">
@@ -2820,7 +2813,7 @@
         <f t="shared" ref="T33:T34" si="47">LN(F40) - LN(F33)</f>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V33" s="30" t="s">
+      <c r="V33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W33" s="21">
@@ -2838,7 +2831,7 @@
         <f t="shared" ref="Z33:Z34" si="49">$M33*T33</f>
         <v>5.0235683675903013</v>
       </c>
-      <c r="AC33" s="30" t="s">
+      <c r="AC33" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD33" s="21">
@@ -2860,7 +2853,7 @@
       <c r="AK33" s="1"/>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B34" s="30"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="21">
         <v>2</v>
       </c>
@@ -2888,7 +2881,7 @@
         <f>M34/L$33</f>
         <v>0.94110538842717861</v>
       </c>
-      <c r="P34" s="30"/>
+      <c r="P34" s="28"/>
       <c r="Q34" s="21">
         <v>2</v>
       </c>
@@ -2904,7 +2897,7 @@
         <f t="shared" si="47"/>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V34" s="30"/>
+      <c r="V34" s="28"/>
       <c r="W34" s="21">
         <v>2</v>
       </c>
@@ -2920,7 +2913,7 @@
         <f t="shared" si="49"/>
         <v>71.350925324956492</v>
       </c>
-      <c r="AC34" s="30"/>
+      <c r="AC34" s="28"/>
       <c r="AD34" s="21">
         <v>2</v>
       </c>
@@ -2940,32 +2933,32 @@
       <c r="AK34" s="1"/>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D35" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="D35" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="R35" s="29" t="s">
+      <c r="R35" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="X35" s="29" t="s">
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="X35" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y35" s="29"/>
-      <c r="Z35" s="29"/>
-      <c r="AE35" s="29" t="s">
+      <c r="Y35" s="27"/>
+      <c r="Z35" s="27"/>
+      <c r="AE35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF35" s="29"/>
-      <c r="AG35" s="29"/>
+      <c r="AF35" s="27"/>
+      <c r="AG35" s="27"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
@@ -3054,20 +3047,20 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="X37" s="27" t="s">
+      <c r="X37" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y37" s="27"/>
-      <c r="Z37" s="27"/>
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
       <c r="AA37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB37" s="8"/>
-      <c r="AE37" s="29" t="s">
+      <c r="AE37" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF37" s="29"/>
-      <c r="AG37" s="29"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
       <c r="AH37" s="1" t="s">
         <v>11</v>
       </c>
@@ -3075,30 +3068,30 @@
       <c r="AK37" s="1"/>
     </row>
     <row r="38" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="N38" s="1"/>
-      <c r="R38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="X38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="27"/>
-      <c r="Z38" s="27"/>
-      <c r="AE38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="27"/>
-      <c r="AG38" s="27"/>
+      <c r="R38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38" s="25"/>
+      <c r="T38" s="25"/>
+      <c r="X38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AE38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="25"/>
+      <c r="AG38" s="25"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
@@ -3150,7 +3143,7 @@
       <c r="A40">
         <v>2000</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="21">
@@ -3190,7 +3183,7 @@
         <f>M40/L$40</f>
         <v>2.5568845446814027E-2</v>
       </c>
-      <c r="P40" s="30" t="s">
+      <c r="P40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q40" s="21">
@@ -3208,7 +3201,7 @@
         <f t="shared" ref="T40:T41" si="59">LN(F47) - LN(F40)</f>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V40" s="30" t="s">
+      <c r="V40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W40" s="21">
@@ -3226,7 +3219,7 @@
         <f t="shared" ref="Z40:Z41" si="61">$M40*T40</f>
         <v>2.665651423580965</v>
       </c>
-      <c r="AC40" s="30" t="s">
+      <c r="AC40" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD40" s="21">
@@ -3248,7 +3241,7 @@
       <c r="AK40" s="1"/>
     </row>
     <row r="41" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B41" s="30"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="21">
         <v>2</v>
       </c>
@@ -3276,7 +3269,7 @@
         <f>M41/L$40</f>
         <v>0.97162630393947746</v>
       </c>
-      <c r="P41" s="30"/>
+      <c r="P41" s="28"/>
       <c r="Q41" s="21">
         <v>2</v>
       </c>
@@ -3292,7 +3285,7 @@
         <f t="shared" si="59"/>
         <v>0.11778303565638382</v>
       </c>
-      <c r="V41" s="30"/>
+      <c r="V41" s="28"/>
       <c r="W41" s="21">
         <v>2</v>
       </c>
@@ -3308,7 +3301,7 @@
         <f t="shared" si="61"/>
         <v>89.349241143602967</v>
       </c>
-      <c r="AC41" s="30"/>
+      <c r="AC41" s="28"/>
       <c r="AD41" s="21">
         <v>2</v>
       </c>
@@ -3328,32 +3321,32 @@
       <c r="AK41" s="1"/>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D42" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
+      <c r="D42" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
       <c r="G42" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="R42" s="29" t="s">
+      <c r="R42" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="X42" s="29" t="s">
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="X42" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AE42" s="29" t="s">
+      <c r="Y42" s="27"/>
+      <c r="Z42" s="27"/>
+      <c r="AE42" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF42" s="29"/>
-      <c r="AG42" s="29"/>
+      <c r="AF42" s="27"/>
+      <c r="AG42" s="27"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
@@ -3442,20 +3435,20 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="X44" s="27" t="s">
+      <c r="X44" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y44" s="27"/>
-      <c r="Z44" s="27"/>
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
       <c r="AA44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB44" s="8"/>
-      <c r="AE44" s="29" t="s">
+      <c r="AE44" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF44" s="29"/>
-      <c r="AG44" s="29"/>
+      <c r="AF44" s="27"/>
+      <c r="AG44" s="27"/>
       <c r="AH44" s="1" t="s">
         <v>11</v>
       </c>
@@ -3463,11 +3456,11 @@
       <c r="AK44" s="1"/>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D45" s="27" t="s">
+      <c r="D45" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
@@ -3488,7 +3481,7 @@
       <c r="A47">
         <v>2010</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="21">
@@ -3511,7 +3504,7 @@
       <c r="AK47" s="1"/>
     </row>
     <row r="48" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B48" s="30"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="21">
         <v>2</v>
       </c>
@@ -3532,11 +3525,11 @@
       <c r="AK48" s="1"/>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D49" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="D49" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
       <c r="G49" s="7" t="s">
         <v>4</v>
       </c>
@@ -3715,7 +3708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3756,94 +3749,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="AJ2" s="27" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AN2" s="27" t="s">
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AN2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="X3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AE3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AJ3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AN3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="R3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="X3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AE3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AJ3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AN3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="25"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D4" s="2">
@@ -3920,7 +3913,7 @@
       <c r="A5">
         <v>1971</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="21">
@@ -3959,7 +3952,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -3977,7 +3970,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="30" t="s">
+      <c r="V5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -3995,7 +3988,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="30" t="s">
+      <c r="AC5" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -4017,7 +4010,7 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -4042,7 +4035,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="30"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -4058,7 +4051,7 @@
         <f t="shared" si="2"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="30"/>
+      <c r="V6" s="28"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -4074,7 +4067,7 @@
         <f t="shared" si="0"/>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="30"/>
+      <c r="AC6" s="28"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -4094,30 +4087,30 @@
       <c r="AK6" s="2"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="D7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="R7" s="29" t="s">
+      <c r="R7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="X7" s="29" t="s">
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="X7" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AE7" s="29" t="s">
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AE7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
@@ -4199,20 +4192,20 @@
         <v>0.41594614744177039</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="X9" s="27" t="s">
+      <c r="X9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
       <c r="AA9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="29" t="s">
+      <c r="AE9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
       <c r="AH9" s="2" t="s">
         <v>11</v>
       </c>
@@ -4220,31 +4213,31 @@
       <c r="AK9" s="2"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="2"/>
-      <c r="R10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="X10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AE10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
+      <c r="R10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="X10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AE10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
@@ -4297,7 +4290,7 @@
       <c r="A12">
         <v>1972</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="21">
@@ -4338,7 +4331,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="30" t="s">
+      <c r="P12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -4356,7 +4349,7 @@
         <f t="shared" si="7"/>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="30" t="s">
+      <c r="V12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -4374,7 +4367,7 @@
         <f t="shared" si="8"/>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="30" t="s">
+      <c r="AC12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -4396,7 +4389,7 @@
       <c r="AK12" s="2"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -4425,7 +4418,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="30"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -4441,7 +4434,7 @@
         <f t="shared" si="7"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="30"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -4457,7 +4450,7 @@
         <f t="shared" si="8"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="30"/>
+      <c r="AC13" s="28"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -4477,11 +4470,11 @@
       <c r="AK13" s="2"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="D14" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -4489,21 +4482,21 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="29" t="s">
+      <c r="R14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="X14" s="29" t="s">
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="X14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-      <c r="AE14" s="29" t="s">
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AE14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
@@ -4594,20 +4587,20 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="27" t="s">
+      <c r="X16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
       <c r="AA16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="29" t="s">
+      <c r="AE16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="2" t="s">
         <v>11</v>
       </c>
@@ -4615,31 +4608,31 @@
       <c r="AK16" s="2"/>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="2"/>
-      <c r="R17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="X17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AE17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
+      <c r="R17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="X17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AE17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
@@ -4692,7 +4685,7 @@
       <c r="A19">
         <v>1973</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="21">
@@ -4733,7 +4726,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="30" t="s">
+      <c r="P19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -4751,7 +4744,7 @@
         <f t="shared" si="14"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="30" t="s">
+      <c r="V19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -4769,7 +4762,7 @@
         <f t="shared" si="15"/>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="30" t="s">
+      <c r="AC19" s="28" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -4791,7 +4784,7 @@
       <c r="AK19" s="2"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -4820,7 +4813,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="30"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -4836,7 +4829,7 @@
         <f t="shared" si="14"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="30"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -4852,7 +4845,7 @@
         <f t="shared" si="15"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="30"/>
+      <c r="AC20" s="28"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -4872,11 +4865,11 @@
       <c r="AK20" s="2"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="D21" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -4884,21 +4877,21 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="29" t="s">
+      <c r="R21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="X21" s="29" t="s">
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="X21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-      <c r="AE21" s="29" t="s">
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AE21" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
@@ -4989,20 +4982,20 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="27" t="s">
+      <c r="X23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
       <c r="AA23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="29" t="s">
+      <c r="AE23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="29"/>
-      <c r="AG23" s="29"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
       <c r="AH23" s="2" t="s">
         <v>11</v>
       </c>
@@ -5010,11 +5003,11 @@
       <c r="AK23" s="2"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -5099,7 +5092,7 @@
       <c r="A26">
         <v>1974</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="21">
@@ -5154,7 +5147,7 @@
       <c r="AP26" s="9"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="30"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -5207,11 +5200,11 @@
       <c r="AP27" s="9"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="D28" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -5470,1765 +5463,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" customWidth="1"/>
-    <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="11" width="3.1640625" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" customWidth="1"/>
-    <col min="13" max="13" width="8" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" customWidth="1"/>
-    <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="23" width="5.5" customWidth="1"/>
-    <col min="24" max="27" width="5.6640625" customWidth="1"/>
-    <col min="28" max="28" width="5.6640625" style="9" customWidth="1"/>
-    <col min="29" max="29" width="4.83203125" customWidth="1"/>
-    <col min="30" max="30" width="5" customWidth="1"/>
-    <col min="31" max="34" width="5.83203125" customWidth="1"/>
-    <col min="35" max="35" width="7.1640625" customWidth="1"/>
-    <col min="36" max="37" width="7.33203125" customWidth="1"/>
-    <col min="38" max="38" width="4.83203125" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" customWidth="1"/>
-    <col min="40" max="43" width="6.1640625" customWidth="1"/>
-    <col min="44" max="45" width="6.33203125" customWidth="1"/>
-    <col min="46" max="46" width="4.5" customWidth="1"/>
-    <col min="47" max="47" width="8.83203125" customWidth="1"/>
-    <col min="49" max="49" width="4.5" customWidth="1"/>
-    <col min="50" max="50" width="7.6640625" customWidth="1"/>
-    <col min="51" max="51" width="6.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="AJ2" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AN2" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="X3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AE3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AJ3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AN3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D4" s="26">
-        <v>1</v>
-      </c>
-      <c r="E4" s="26">
-        <v>2</v>
-      </c>
-      <c r="F4" s="26">
-        <v>3</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="26">
-        <v>1</v>
-      </c>
-      <c r="S4" s="26">
-        <v>2</v>
-      </c>
-      <c r="T4" s="26">
-        <v>3</v>
-      </c>
-      <c r="X4" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="26">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="26">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="26">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="26">
-        <v>2</v>
-      </c>
-      <c r="AG4" s="26">
-        <v>3</v>
-      </c>
-      <c r="AJ4" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="26">
-        <v>2</v>
-      </c>
-      <c r="AL4" s="26">
-        <v>3</v>
-      </c>
-      <c r="AN4" s="26">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="26">
-        <v>2</v>
-      </c>
-      <c r="AP4" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1971</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="21">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12">
-        <f>PRODUCT(D5:F5)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="17">
-        <f>G15/G8</f>
-        <v>3</v>
-      </c>
-      <c r="J5" s="18">
-        <f>G15-G8</f>
-        <v>120</v>
-      </c>
-      <c r="L5" s="14">
-        <f>(G15-G8) / (LN(G15) - LN(G8))</f>
-        <v>109.22870719522045</v>
-      </c>
-      <c r="M5" s="15" t="e">
-        <f>(G12-G5) / (LN(G12) - LN(G5))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N5" s="16" t="e">
-        <f>M5/L$5</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>1</v>
-      </c>
-      <c r="R5" s="4" t="e">
-        <f>LN(D12) - LN(D5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="S5" s="4">
-        <f>LN(E12) - LN(E5)</f>
-        <v>-0.69314718055994562</v>
-      </c>
-      <c r="T5" s="4">
-        <f>LN(F12) - LN(F5)</f>
-        <v>0.4054651081081645</v>
-      </c>
-      <c r="V5" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="W5" s="21">
-        <v>1</v>
-      </c>
-      <c r="X5" s="4" t="e">
-        <f>$M5*R5</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y5" s="4" t="e">
-        <f t="shared" ref="Y5:Z6" si="0">$M5*S5</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z5" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AC5" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="4" t="e">
-        <f>$N5*R5</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AF5" s="4" t="e">
-        <f t="shared" ref="AF5:AG6" si="1">$N5*S5</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AG5" s="4" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
-      <c r="C6" s="21">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>4</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="12">
-        <f>PRODUCT(D6:F6)</f>
-        <v>60</v>
-      </c>
-      <c r="M6" s="15">
-        <f>(G13-G6) / (LN(G13) - LN(G6))</f>
-        <v>86.561702453337787</v>
-      </c>
-      <c r="N6" s="16">
-        <f>M6/L$5</f>
-        <v>0.79248125036057815</v>
-      </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="21">
-        <v>2</v>
-      </c>
-      <c r="R6" s="4">
-        <f>LN(D13) - LN(D6)</f>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="S6" s="4">
-        <f t="shared" ref="S6:T6" si="2">LN(E13) - LN(E6)</f>
-        <v>0.18232155679395468</v>
-      </c>
-      <c r="T6" s="4">
-        <f t="shared" si="2"/>
-        <v>0.28768207245178079</v>
-      </c>
-      <c r="V6" s="30"/>
-      <c r="W6" s="21">
-        <v>2</v>
-      </c>
-      <c r="X6" s="4">
-        <f>$M6*R6</f>
-        <v>19.315685693241733</v>
-      </c>
-      <c r="Y6" s="4">
-        <f t="shared" si="0"/>
-        <v>15.782064350027632</v>
-      </c>
-      <c r="Z6" s="4">
-        <f t="shared" si="0"/>
-        <v>24.902249956730611</v>
-      </c>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="21">
-        <v>2</v>
-      </c>
-      <c r="AE6" s="4">
-        <f>$N6*R6</f>
-        <v>0.17683708055538475</v>
-      </c>
-      <c r="AF6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.14448641529576037</v>
-      </c>
-      <c r="AG6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22798264848290967</v>
-      </c>
-      <c r="AJ6" s="26"/>
-      <c r="AK6" s="26"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D7" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="26"/>
-      <c r="R7" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="X7" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AE7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="26"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="13">
-        <f>SUM(G5:G6)</f>
-        <v>60</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="N8" s="26"/>
-      <c r="X8" s="4" t="e">
-        <f>SUM(X5:X6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y8" s="4" t="e">
-        <f t="shared" ref="Y8:Z8" si="3">SUM(Y5:Y6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z8" s="4" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AA8" s="18" t="e">
-        <f>SUM(X8:Z8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AB8" s="19"/>
-      <c r="AE8" s="4" t="e">
-        <f>EXP(SUM(AE5:AE6))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AF8" s="4" t="e">
-        <f t="shared" ref="AF8:AG8" si="4">EXP(SUM(AF5:AF6))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AG8" s="4" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AH8" s="17" t="e">
-        <f>PRODUCT(AE8:AG8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AJ8" s="4" t="e">
-        <f>X8</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AK8" s="4" t="e">
-        <f t="shared" ref="AK8:AL8" si="5">Y8</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AL8" s="4" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AN8" s="4" t="e">
-        <f>AE8</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AO8" s="4" t="e">
-        <f t="shared" ref="AO8:AP8" si="6">AF8</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AP8" s="4" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="G9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f>M6/L12</f>
-        <v>0.41594614744177039</v>
-      </c>
-      <c r="N9" s="26"/>
-      <c r="X9" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB9" s="8"/>
-      <c r="AE9" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ9" s="26"/>
-      <c r="AK9" s="26"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D10" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="N10" s="26"/>
-      <c r="R10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="X10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AE10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AJ10" s="26"/>
-      <c r="AK10" s="26"/>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D11" s="26">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26">
-        <v>2</v>
-      </c>
-      <c r="F11" s="26">
-        <v>3</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="N11" s="26"/>
-      <c r="R11" s="26">
-        <v>1</v>
-      </c>
-      <c r="S11" s="26">
-        <v>2</v>
-      </c>
-      <c r="T11" s="26">
-        <v>3</v>
-      </c>
-      <c r="X11" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="26">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="26">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="26">
-        <v>2</v>
-      </c>
-      <c r="AG11" s="26">
-        <v>3</v>
-      </c>
-      <c r="AJ11" s="26"/>
-      <c r="AK11" s="26"/>
-    </row>
-    <row r="12" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1972</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="21">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>4</v>
-      </c>
-      <c r="E12" s="4">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12">
-        <f>PRODUCT(D12:F12)</f>
-        <v>60</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="17">
-        <f>G22/G15</f>
-        <v>1.3277777777777777</v>
-      </c>
-      <c r="J12" s="18">
-        <f>G22-G15</f>
-        <v>59</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="14">
-        <f>(G22-G15) / (LN(G22) - LN(G15))</f>
-        <v>208.10795576717257</v>
-      </c>
-      <c r="M12" s="15">
-        <f>(G19-G12) / (LN(G19) - LN(G12))</f>
-        <v>61.978488652901611</v>
-      </c>
-      <c r="N12" s="16">
-        <f>M12/L$12</f>
-        <v>0.29781892972050539</v>
-      </c>
-      <c r="P12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="21">
-        <v>1</v>
-      </c>
-      <c r="R12" s="4">
-        <f>LN(D19) - LN(D12)</f>
-        <v>0.69314718055994518</v>
-      </c>
-      <c r="S12" s="4">
-        <f t="shared" ref="S12:T13" si="7">LN(E19) - LN(E12)</f>
-        <v>-0.916290731874155</v>
-      </c>
-      <c r="T12" s="4">
-        <f t="shared" si="7"/>
-        <v>0.28768207245178079</v>
-      </c>
-      <c r="V12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="W12" s="21">
-        <v>1</v>
-      </c>
-      <c r="X12" s="4">
-        <f>$M12*R12</f>
-        <v>42.960214665125307</v>
-      </c>
-      <c r="Y12" s="4">
-        <f t="shared" ref="Y12:Z13" si="8">$M12*S12</f>
-        <v>-56.790314728221226</v>
-      </c>
-      <c r="Z12" s="4">
-        <f t="shared" si="8"/>
-        <v>17.830100063095916</v>
-      </c>
-      <c r="AC12" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD12" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="4">
-        <f>$N12*R12</f>
-        <v>0.20643235145314878</v>
-      </c>
-      <c r="AF12" s="4">
-        <f t="shared" ref="AF12:AG13" si="9">$N12*S12</f>
-        <v>-0.2728887250795794</v>
-      </c>
-      <c r="AG12" s="4">
-        <f t="shared" si="9"/>
-        <v>8.5677166917366238E-2</v>
-      </c>
-      <c r="AJ12" s="26"/>
-      <c r="AK12" s="26"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
-      <c r="C13" s="21">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4</v>
-      </c>
-      <c r="G13" s="12">
-        <f>PRODUCT(D13:F13)</f>
-        <v>120</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="M13" s="15">
-        <f>(G20-G13) / (LN(G20) - LN(G13))</f>
-        <v>145.77482362664972</v>
-      </c>
-      <c r="N13" s="16">
-        <f>M13/L$12</f>
-        <v>0.70047693798760857</v>
-      </c>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="21">
-        <v>2</v>
-      </c>
-      <c r="R13" s="4">
-        <f>LN(D20) - LN(D13)</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
-        <f t="shared" si="7"/>
-        <v>0.15415067982725827</v>
-      </c>
-      <c r="T13" s="4">
-        <f t="shared" si="7"/>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="V13" s="30"/>
-      <c r="W13" s="21">
-        <v>2</v>
-      </c>
-      <c r="X13" s="4">
-        <f>$M13*R13</f>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="4">
-        <f>$M13*S13</f>
-        <v>22.471288163746728</v>
-      </c>
-      <c r="Z13" s="4">
-        <f t="shared" si="8"/>
-        <v>32.52871183625318</v>
-      </c>
-      <c r="AC13" s="30"/>
-      <c r="AD13" s="21">
-        <v>2</v>
-      </c>
-      <c r="AE13" s="4">
-        <f>$N13*R13</f>
-        <v>0</v>
-      </c>
-      <c r="AF13" s="4">
-        <f t="shared" si="9"/>
-        <v>0.1079789961941061</v>
-      </c>
-      <c r="AG13" s="4">
-        <f t="shared" si="9"/>
-        <v>0.15630691155625842</v>
-      </c>
-      <c r="AJ13" s="26"/>
-      <c r="AK13" s="26"/>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D14" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="R14" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="X14" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-      <c r="AE14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
-      <c r="AJ14" s="26"/>
-      <c r="AK14" s="26"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="13">
-        <f>SUM(G12:G13)</f>
-        <v>180</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="X15" s="4">
-        <f>SUM(X12:X13)</f>
-        <v>42.960214665125307</v>
-      </c>
-      <c r="Y15" s="4">
-        <f t="shared" ref="Y15:Z15" si="10">SUM(Y12:Y13)</f>
-        <v>-34.319026564474498</v>
-      </c>
-      <c r="Z15" s="4">
-        <f t="shared" si="10"/>
-        <v>50.358811899349092</v>
-      </c>
-      <c r="AA15" s="18">
-        <f>SUM(X15:Z15)</f>
-        <v>58.999999999999901</v>
-      </c>
-      <c r="AB15" s="19"/>
-      <c r="AE15" s="4">
-        <f>EXP(SUM(AE12:AE13))</f>
-        <v>1.2292845720892271</v>
-      </c>
-      <c r="AF15" s="4">
-        <f t="shared" ref="AF15:AG15" si="11">EXP(SUM(AF12:AF13))</f>
-        <v>0.84797024785237751</v>
-      </c>
-      <c r="AG15" s="4">
-        <f t="shared" si="11"/>
-        <v>1.2737739122298066</v>
-      </c>
-      <c r="AH15" s="17">
-        <f>PRODUCT(AE15:AG15)</f>
-        <v>1.3277777777777777</v>
-      </c>
-      <c r="AJ15" s="4" t="e">
-        <f>AJ8+X15</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AK15" s="4" t="e">
-        <f t="shared" ref="AK15:AL15" si="12">AK8+Y15</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AL15" s="4" t="e">
-        <f t="shared" si="12"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AN15" s="4" t="e">
-        <f>AN8*AE15</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AO15" s="4" t="e">
-        <f t="shared" ref="AO15:AP15" si="13">AO8*AF15</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AP15" s="4" t="e">
-        <f t="shared" si="13"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="X16" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB16" s="8"/>
-      <c r="AE16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
-      <c r="AH16" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ16" s="26"/>
-      <c r="AK16" s="26"/>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D17" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="N17" s="26"/>
-      <c r="R17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="X17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AE17" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AJ17" s="26"/>
-      <c r="AK17" s="26"/>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D18" s="26">
-        <v>1</v>
-      </c>
-      <c r="E18" s="26">
-        <v>2</v>
-      </c>
-      <c r="F18" s="26">
-        <v>3</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="N18" s="26"/>
-      <c r="R18" s="26">
-        <v>1</v>
-      </c>
-      <c r="S18" s="26">
-        <v>2</v>
-      </c>
-      <c r="T18" s="26">
-        <v>3</v>
-      </c>
-      <c r="X18" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="26">
-        <v>2</v>
-      </c>
-      <c r="Z18" s="26">
-        <v>3</v>
-      </c>
-      <c r="AE18" s="26">
-        <v>1</v>
-      </c>
-      <c r="AF18" s="26">
-        <v>2</v>
-      </c>
-      <c r="AG18" s="26">
-        <v>3</v>
-      </c>
-      <c r="AJ18" s="26"/>
-      <c r="AK18" s="26"/>
-    </row>
-    <row r="19" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1973</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="21">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4">
-        <v>2</v>
-      </c>
-      <c r="F19" s="4">
-        <v>4</v>
-      </c>
-      <c r="G19" s="12">
-        <f>PRODUCT(D19:F19)</f>
-        <v>64</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="17">
-        <f>G29/G22</f>
-        <v>1.4142259414225942</v>
-      </c>
-      <c r="J19" s="18">
-        <f>G29-G22</f>
-        <v>99</v>
-      </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="14">
-        <f>(G29-G22) / (LN(G29) - LN(G22))</f>
-        <v>285.64640363823662</v>
-      </c>
-      <c r="M19" s="15">
-        <f>(G26-G19) / (LN(G26) - LN(G19))</f>
-        <v>56.712288666956283</v>
-      </c>
-      <c r="N19" s="16">
-        <f>M19/L$19</f>
-        <v>0.19854018095316492</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="21">
-        <v>1</v>
-      </c>
-      <c r="R19" s="4">
-        <f t="shared" ref="R19:T20" si="14">LN(D26) - LN(D19)</f>
-        <v>0.22314355131421015</v>
-      </c>
-      <c r="S19" s="4">
-        <f t="shared" si="14"/>
-        <v>-0.69314718055994529</v>
-      </c>
-      <c r="T19" s="4">
-        <f t="shared" si="14"/>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="V19" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="W19" s="21">
-        <v>1</v>
-      </c>
-      <c r="X19" s="4">
-        <f>$M19*R19</f>
-        <v>12.654981496301259</v>
-      </c>
-      <c r="Y19" s="4">
-        <f t="shared" ref="Y19:Z20" si="15">$M19*S19</f>
-        <v>-39.309962992602486</v>
-      </c>
-      <c r="Z19" s="4">
-        <f t="shared" si="15"/>
-        <v>12.654981496301232</v>
-      </c>
-      <c r="AC19" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD19" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="4">
-        <f>$N19*R19</f>
-        <v>4.4302961056455127E-2</v>
-      </c>
-      <c r="AF19" s="4">
-        <f t="shared" ref="AF19:AG20" si="16">$N19*S19</f>
-        <v>-0.13761756665554761</v>
-      </c>
-      <c r="AG19" s="4">
-        <f t="shared" si="16"/>
-        <v>4.4302961056455037E-2</v>
-      </c>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="26"/>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
-      <c r="C20" s="21">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5</v>
-      </c>
-      <c r="E20" s="4">
-        <v>7</v>
-      </c>
-      <c r="F20" s="4">
-        <v>5</v>
-      </c>
-      <c r="G20" s="12">
-        <f>PRODUCT(D20:F20)</f>
-        <v>175</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="M20" s="15">
-        <f>(G27-G20) / (LN(G27) - LN(G20))</f>
-        <v>226.82814674545895</v>
-      </c>
-      <c r="N20" s="16">
-        <f>M20/L$19</f>
-        <v>0.79408717861097466</v>
-      </c>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="21">
-        <v>2</v>
-      </c>
-      <c r="R20" s="4">
-        <f t="shared" si="14"/>
-        <v>0.18232155679395468</v>
-      </c>
-      <c r="S20" s="4">
-        <f t="shared" si="14"/>
-        <v>0.13353139262452252</v>
-      </c>
-      <c r="T20" s="4">
-        <f t="shared" si="14"/>
-        <v>0.18232155679395468</v>
-      </c>
-      <c r="V20" s="30"/>
-      <c r="W20" s="21">
-        <v>2</v>
-      </c>
-      <c r="X20" s="4">
-        <f>$M20*R20</f>
-        <v>41.355660839319683</v>
-      </c>
-      <c r="Y20" s="4">
-        <f t="shared" si="15"/>
-        <v>30.288678321360688</v>
-      </c>
-      <c r="Z20" s="4">
-        <f t="shared" si="15"/>
-        <v>41.355660839319683</v>
-      </c>
-      <c r="AC20" s="30"/>
-      <c r="AD20" s="21">
-        <v>2</v>
-      </c>
-      <c r="AE20" s="4">
-        <f>$N20*R20</f>
-        <v>0.14477921063447205</v>
-      </c>
-      <c r="AF20" s="4">
-        <f t="shared" si="16"/>
-        <v>0.10603556682520139</v>
-      </c>
-      <c r="AG20" s="4">
-        <f t="shared" si="16"/>
-        <v>0.14477921063447205</v>
-      </c>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="26"/>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D21" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="R21" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="X21" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-      <c r="AE21" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="26"/>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="13">
-        <f>SUM(G19:G20)</f>
-        <v>239</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="X22" s="4">
-        <f>SUM(X19:X20)</f>
-        <v>54.010642335620943</v>
-      </c>
-      <c r="Y22" s="4">
-        <f t="shared" ref="Y22:Z22" si="17">SUM(Y19:Y20)</f>
-        <v>-9.0212846712417978</v>
-      </c>
-      <c r="Z22" s="4">
-        <f t="shared" si="17"/>
-        <v>54.010642335620915</v>
-      </c>
-      <c r="AA22" s="18">
-        <f>SUM(X22:Z22)</f>
-        <v>99.000000000000057</v>
-      </c>
-      <c r="AB22" s="19"/>
-      <c r="AE22" s="4">
-        <f>EXP(SUM(AE19:AE20))</f>
-        <v>1.2081402233292473</v>
-      </c>
-      <c r="AF22" s="4">
-        <f t="shared" ref="AF22:AG22" si="18">EXP(SUM(AF19:AF20))</f>
-        <v>0.96891150261734849</v>
-      </c>
-      <c r="AG22" s="4">
-        <f t="shared" si="18"/>
-        <v>1.2081402233292473</v>
-      </c>
-      <c r="AH22" s="17">
-        <f>PRODUCT(AE22:AG22)</f>
-        <v>1.4142259414225939</v>
-      </c>
-      <c r="AJ22" s="4" t="e">
-        <f>AJ15+X22</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AK22" s="4" t="e">
-        <f t="shared" ref="AK22:AL22" si="19">AK15+Y22</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AL22" s="4" t="e">
-        <f t="shared" si="19"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AN22" s="4" t="e">
-        <f>AN15*AE22</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AO22" s="4" t="e">
-        <f t="shared" ref="AO22:AP22" si="20">AO15*AF22</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AP22" s="4" t="e">
-        <f t="shared" si="20"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="X23" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
-      <c r="AA23" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB23" s="8"/>
-      <c r="AE23" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF23" s="29"/>
-      <c r="AG23" s="29"/>
-      <c r="AH23" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ23" s="26"/>
-      <c r="AK23" s="26"/>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D24" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="10"/>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="10"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="8"/>
-      <c r="AK24" s="8"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
-      <c r="AP24" s="9"/>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D25" s="26">
-        <v>1</v>
-      </c>
-      <c r="E25" s="26">
-        <v>2</v>
-      </c>
-      <c r="F25" s="26">
-        <v>3</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="8"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AJ25" s="8"/>
-      <c r="AK25" s="8"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
-      <c r="AP25" s="9"/>
-    </row>
-    <row r="26" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1974</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="21">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4">
-        <v>10</v>
-      </c>
-      <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4">
-        <v>5</v>
-      </c>
-      <c r="G26" s="12">
-        <f>PRODUCT(D26:F26)</f>
-        <v>50</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="9"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="22"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B27" s="30"/>
-      <c r="C27" s="21">
-        <v>2</v>
-      </c>
-      <c r="D27" s="4">
-        <v>6</v>
-      </c>
-      <c r="E27" s="4">
-        <v>8</v>
-      </c>
-      <c r="F27" s="4">
-        <v>6</v>
-      </c>
-      <c r="G27" s="12">
-        <f>PRODUCT(D27:F27)</f>
-        <v>288</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="9"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="22"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="8"/>
-      <c r="AK27" s="8"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="D28" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="9"/>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-      <c r="AG28" s="24"/>
-      <c r="AH28" s="9"/>
-      <c r="AI28" s="9"/>
-      <c r="AJ28" s="8"/>
-      <c r="AK28" s="8"/>
-      <c r="AL28" s="9"/>
-      <c r="AM28" s="9"/>
-      <c r="AN28" s="9"/>
-      <c r="AO28" s="9"/>
-      <c r="AP28" s="9"/>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="13">
-        <f>SUM(G26:G27)</f>
-        <v>338</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="19"/>
-      <c r="AB29" s="19"/>
-      <c r="AC29" s="9"/>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="8"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="9"/>
-      <c r="AJ29" s="8"/>
-      <c r="AK29" s="8"/>
-      <c r="AL29" s="8"/>
-      <c r="AM29" s="9"/>
-      <c r="AN29" s="8"/>
-      <c r="AO29" s="8"/>
-      <c r="AP29" s="8"/>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="10"/>
-      <c r="Y30" s="10"/>
-      <c r="Z30" s="10"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="24"/>
-      <c r="AF30" s="24"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="8"/>
-      <c r="AI30" s="9"/>
-      <c r="AJ30" s="8"/>
-      <c r="AK30" s="8"/>
-      <c r="AL30" s="9"/>
-      <c r="AM30" s="9"/>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="9"/>
-      <c r="AP30" s="9"/>
-    </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AI31" s="9"/>
-      <c r="AJ31" s="9"/>
-      <c r="AK31" s="9"/>
-      <c r="AL31" s="9"/>
-      <c r="AM31" s="9"/>
-      <c r="AN31" s="9"/>
-      <c r="AO31" s="9"/>
-      <c r="AP31" s="9"/>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="9"/>
-      <c r="AJ32" s="9"/>
-      <c r="AK32" s="9"/>
-      <c r="AL32" s="9"/>
-      <c r="AM32" s="9"/>
-      <c r="AN32" s="9"/>
-      <c r="AO32" s="9"/>
-      <c r="AP32" s="9"/>
-    </row>
-    <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="AE21:AG21"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="A1:AP1"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AN3:AP3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests for deltaV and D
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -3709,7 +3709,7 @@
   <dimension ref="A1:AP47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+      <selection activeCell="AG28" sqref="AG28:AH28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3813,12 +3813,12 @@
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="R3" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="S3" s="27"/>
       <c r="T3" s="27"/>
       <c r="X3" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Y3" s="27"/>
       <c r="Z3" s="27"/>
@@ -4224,17 +4224,17 @@
       <c r="K10" s="9"/>
       <c r="N10" s="2"/>
       <c r="R10" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="S10" s="27"/>
       <c r="T10" s="27"/>
       <c r="X10" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Y10" s="27"/>
       <c r="Z10" s="27"/>
       <c r="AE10" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="AF10" s="27"/>
       <c r="AG10" s="27"/>
@@ -4619,17 +4619,17 @@
       <c r="K17" s="9"/>
       <c r="N17" s="2"/>
       <c r="R17" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="S17" s="27"/>
       <c r="T17" s="27"/>
       <c r="X17" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Y17" s="27"/>
       <c r="Z17" s="27"/>
       <c r="AE17" s="27" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="AF17" s="27"/>
       <c r="AG17" s="27"/>
@@ -5224,16 +5224,40 @@
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="9"/>
+      <c r="X28" s="24">
+        <f>X8+X15+X22</f>
+        <v>166.76092297970456</v>
+      </c>
+      <c r="Y28" s="24">
+        <f t="shared" ref="Y28:AA28" si="21">Y8+Y15+Y22</f>
+        <v>-52.795437028546971</v>
+      </c>
+      <c r="Z28" s="24">
+        <f t="shared" si="21"/>
+        <v>144.03451404884231</v>
+      </c>
+      <c r="AA28" s="24">
+        <f t="shared" si="21"/>
+        <v>257.99999999999994</v>
+      </c>
       <c r="AC28" s="9"/>
       <c r="AD28" s="9"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-      <c r="AG28" s="24"/>
-      <c r="AH28" s="9"/>
+      <c r="AE28" s="24">
+        <f>AE8*AE15*AE22</f>
+        <v>2.6155208515192934</v>
+      </c>
+      <c r="AF28" s="24">
+        <f t="shared" ref="AF28:AH28" si="22">AF8*AF15*AF22</f>
+        <v>0.7609663039470701</v>
+      </c>
+      <c r="AG28" s="24">
+        <f t="shared" si="22"/>
+        <v>2.1227707766832733</v>
+      </c>
+      <c r="AH28" s="24">
+        <f t="shared" si="22"/>
+        <v>4.2249999999999996</v>
+      </c>
       <c r="AI28" s="9"/>
       <c r="AJ28" s="8"/>
       <c r="AK28" s="8"/>
@@ -5271,14 +5295,20 @@
       <c r="W29" s="9"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
+      <c r="Z29" s="9">
+        <f>SUM(X28:Z28)</f>
+        <v>257.99999999999989</v>
+      </c>
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="9"/>
       <c r="AD29" s="9"/>
       <c r="AE29" s="8"/>
       <c r="AF29" s="8"/>
-      <c r="AG29" s="8"/>
+      <c r="AG29" s="8">
+        <f>AE28*AF28*AG28</f>
+        <v>4.2249999999999988</v>
+      </c>
       <c r="AH29" s="19"/>
       <c r="AI29" s="9"/>
       <c r="AJ29" s="8"/>

</xml_diff>

<commit_message>
Figuring out how to get 1s and 0s in first year.
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/LMDIR/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LMDIR/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14720" yWindow="460" windowWidth="32720" windowHeight="18620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="with matrices - incremental" sheetId="1" r:id="rId1"/>
     <sheet name="with matrices - for testing" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="27">
   <si>
     <t>V</t>
   </si>
@@ -465,8 +465,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,7 +583,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -613,8 +613,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,6 +685,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -687,7 +706,7 @@
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -702,6 +721,11 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -716,6 +740,11 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -993,14 +1022,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D45" sqref="D45:F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -1036,97 +1065,97 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="AJ2" s="25" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AN2" s="25" t="s">
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AN2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-    </row>
-    <row r="3" spans="1:42">
-      <c r="D3" s="25" t="s">
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="R3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="X3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AE3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AJ3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AN3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="R3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="X3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AE3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AJ3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AN3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="28"/>
+      <c r="AP3" s="28"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -1197,11 +1226,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1950</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21">
@@ -1240,7 +1269,7 @@
         <f>M5/L$5</f>
         <v>0.29525619714283424</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="21">
@@ -1258,7 +1287,7 @@
         <f>LN(F12) - LN(F5)</f>
         <v>0.4054651081081645</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W5" s="21">
@@ -1276,7 +1305,7 @@
         <f t="shared" si="0"/>
         <v>14.762809857141708</v>
       </c>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD5" s="21">
@@ -1297,8 +1326,8 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:42">
-      <c r="B6" s="28"/>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B6" s="31"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -1323,7 +1352,7 @@
         <f>M6/L$5</f>
         <v>0.70195500086538765</v>
       </c>
-      <c r="P6" s="28"/>
+      <c r="P6" s="31"/>
       <c r="Q6" s="21">
         <v>2</v>
       </c>
@@ -1339,7 +1368,7 @@
         <f t="shared" ref="T6" si="3">LN(F13) - LN(F6)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V6" s="28"/>
+      <c r="V6" s="31"/>
       <c r="W6" s="21">
         <v>2</v>
       </c>
@@ -1355,7 +1384,7 @@
         <f t="shared" ref="Z6" si="5">$M6*T6</f>
         <v>24.902249956730611</v>
       </c>
-      <c r="AC6" s="28"/>
+      <c r="AC6" s="31"/>
       <c r="AD6" s="21">
         <v>2</v>
       </c>
@@ -1374,35 +1403,35 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:42">
-      <c r="D7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="X7" s="27" t="s">
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="X7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AE7" s="27" t="s">
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AE7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
@@ -1469,63 +1498,63 @@
         <v>1.3794101155854785</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="G9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="X9" s="25" t="s">
+      <c r="X9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
       <c r="AA9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB9" s="8"/>
-      <c r="AE9" s="27" t="s">
+      <c r="AE9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
       <c r="AH9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:42">
-      <c r="D10" s="25" t="s">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="N10" s="1"/>
-      <c r="R10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="X10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AE10" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
+      <c r="R10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="X10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AE10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -1570,11 +1599,11 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1960</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="21">
@@ -1615,7 +1644,7 @@
         <f>M12/L$12</f>
         <v>0.29781892972050539</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
@@ -1633,7 +1662,7 @@
         <f t="shared" ref="T12:T13" si="13">LN(F19) - LN(F12)</f>
         <v>0.28768207245178079</v>
       </c>
-      <c r="V12" s="28" t="s">
+      <c r="V12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -1651,7 +1680,7 @@
         <f t="shared" ref="Z12:Z13" si="15">$M12*T12</f>
         <v>17.830100063095916</v>
       </c>
-      <c r="AC12" s="28" t="s">
+      <c r="AC12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -1672,8 +1701,8 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:42">
-      <c r="B13" s="28"/>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B13" s="31"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
@@ -1702,7 +1731,7 @@
         <f>M13/L$12</f>
         <v>0.70047693798760857</v>
       </c>
-      <c r="P13" s="28"/>
+      <c r="P13" s="31"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
@@ -1718,7 +1747,7 @@
         <f t="shared" si="13"/>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V13" s="28"/>
+      <c r="V13" s="31"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -1734,7 +1763,7 @@
         <f t="shared" si="15"/>
         <v>32.52871183625318</v>
       </c>
-      <c r="AC13" s="28"/>
+      <c r="AC13" s="31"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -1753,12 +1782,12 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:42">
-      <c r="D14" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D14" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
@@ -1766,25 +1795,25 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="R14" s="27" t="s">
+      <c r="R14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="X14" s="27" t="s">
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="X14" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AE14" s="27" t="s">
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AE14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
@@ -1857,7 +1886,7 @@
         <v>1.7570566194986847</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1871,56 +1900,56 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="X16" s="25" t="s">
+      <c r="X16" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
       <c r="AA16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AE16" s="27" t="s">
+      <c r="AE16" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
       <c r="AH16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:42">
-      <c r="D17" s="25" t="s">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="N17" s="1"/>
-      <c r="R17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="X17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AE17" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
+      <c r="R17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="X17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AE17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D18" s="1">
         <v>1</v>
       </c>
@@ -1965,11 +1994,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1970</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="21">
@@ -2010,7 +2039,7 @@
         <f>M19/L$19</f>
         <v>0.19854018095316492</v>
       </c>
-      <c r="P19" s="28" t="s">
+      <c r="P19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
@@ -2028,7 +2057,7 @@
         <f t="shared" ref="T19:T20" si="23">LN(F26) - LN(F19)</f>
         <v>0.22314355131420971</v>
       </c>
-      <c r="V19" s="28" t="s">
+      <c r="V19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -2046,7 +2075,7 @@
         <f t="shared" ref="Z19:Z20" si="25">$M19*T19</f>
         <v>12.654981496301232</v>
       </c>
-      <c r="AC19" s="28" t="s">
+      <c r="AC19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -2067,8 +2096,8 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:42">
-      <c r="B20" s="28"/>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B20" s="31"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -2097,7 +2126,7 @@
         <f>M20/L$19</f>
         <v>0.79408717861097466</v>
       </c>
-      <c r="P20" s="28"/>
+      <c r="P20" s="31"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
@@ -2113,7 +2142,7 @@
         <f t="shared" si="23"/>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V20" s="28"/>
+      <c r="V20" s="31"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
@@ -2129,7 +2158,7 @@
         <f t="shared" si="25"/>
         <v>41.355660839319683</v>
       </c>
-      <c r="AC20" s="28"/>
+      <c r="AC20" s="31"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
@@ -2148,12 +2177,12 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:42">
-      <c r="D21" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D21" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
@@ -2161,25 +2190,25 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="27" t="s">
+      <c r="R21" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="X21" s="27" t="s">
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="X21" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
-      <c r="AE21" s="27" t="s">
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AE21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="27"/>
+      <c r="AF21" s="30"/>
+      <c r="AG21" s="30"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2252,7 +2281,7 @@
         <v>2.1227707766832733</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2266,56 +2295,56 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="25" t="s">
+      <c r="X23" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="28"/>
       <c r="AA23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="27" t="s">
+      <c r="AE23" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="27"/>
-      <c r="AG23" s="27"/>
+      <c r="AF23" s="30"/>
+      <c r="AG23" s="30"/>
       <c r="AH23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:42">
-      <c r="D24" s="25" t="s">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="N24" s="1"/>
-      <c r="R24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="X24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
-      <c r="AE24" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="25"/>
+      <c r="R24" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="X24" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AE24" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D25" s="1">
         <v>1</v>
       </c>
@@ -2360,11 +2389,11 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1980</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="21">
@@ -2405,7 +2434,7 @@
         <f>M26/L$26</f>
         <v>0.10561476584617054</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q26" s="21">
@@ -2423,7 +2452,7 @@
         <f t="shared" ref="T26:T27" si="35">LN(F33) - LN(F26)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="V26" s="28" t="s">
+      <c r="V26" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
@@ -2441,7 +2470,7 @@
         <f t="shared" ref="Z26:Z27" si="37">$M26*T26</f>
         <v>7.7700766953751215</v>
       </c>
-      <c r="AC26" s="28" t="s">
+      <c r="AC26" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD26" s="21">
@@ -2462,8 +2491,8 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:42">
-      <c r="B27" s="28"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B27" s="31"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -2492,7 +2521,7 @@
         <f>M27/L$26</f>
         <v>0.88988350592239895</v>
       </c>
-      <c r="P27" s="28"/>
+      <c r="P27" s="31"/>
       <c r="Q27" s="21">
         <v>2</v>
       </c>
@@ -2508,7 +2537,7 @@
         <f t="shared" si="35"/>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V27" s="28"/>
+      <c r="V27" s="31"/>
       <c r="W27" s="21">
         <v>2</v>
       </c>
@@ -2524,7 +2553,7 @@
         <f t="shared" si="37"/>
         <v>55.353010514175885</v>
       </c>
-      <c r="AC27" s="28"/>
+      <c r="AC27" s="31"/>
       <c r="AD27" s="21">
         <v>2</v>
       </c>
@@ -2543,12 +2572,12 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:42">
-      <c r="D28" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2556,25 +2585,25 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="R28" s="27" t="s">
+      <c r="R28" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="X28" s="27" t="s">
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="X28" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y28" s="27"/>
-      <c r="Z28" s="27"/>
-      <c r="AE28" s="27" t="s">
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AE28" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF28" s="27"/>
-      <c r="AG28" s="27"/>
+      <c r="AF28" s="30"/>
+      <c r="AG28" s="30"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2646,7 +2675,7 @@
         <v>2.4822221852499999</v>
       </c>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2659,55 +2688,55 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="X30" s="25" t="s">
+      <c r="X30" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
       <c r="AA30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB30" s="8"/>
-      <c r="AE30" s="27" t="s">
+      <c r="AE30" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF30" s="27"/>
-      <c r="AG30" s="27"/>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
       <c r="AH30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:42">
-      <c r="D31" s="25" t="s">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D31" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="N31" s="1"/>
-      <c r="R31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="X31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AE31" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="25"/>
-      <c r="AG31" s="25"/>
+      <c r="R31" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="X31" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AE31" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="28"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D32" s="1">
         <v>1</v>
       </c>
@@ -2751,11 +2780,11 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1990</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="21">
@@ -2795,7 +2824,7 @@
         <f>M33/L$33</f>
         <v>5.7396961403155373E-2</v>
       </c>
-      <c r="P33" s="28" t="s">
+      <c r="P33" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q33" s="21">
@@ -2813,7 +2842,7 @@
         <f t="shared" ref="T33:T34" si="47">LN(F40) - LN(F33)</f>
         <v>0.15415067982725827</v>
       </c>
-      <c r="V33" s="28" t="s">
+      <c r="V33" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W33" s="21">
@@ -2831,7 +2860,7 @@
         <f t="shared" ref="Z33:Z34" si="49">$M33*T33</f>
         <v>5.0235683675903013</v>
       </c>
-      <c r="AC33" s="28" t="s">
+      <c r="AC33" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD33" s="21">
@@ -2852,8 +2881,8 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:42">
-      <c r="B34" s="28"/>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B34" s="31"/>
       <c r="C34" s="21">
         <v>2</v>
       </c>
@@ -2881,7 +2910,7 @@
         <f>M34/L$33</f>
         <v>0.94110538842717861</v>
       </c>
-      <c r="P34" s="28"/>
+      <c r="P34" s="31"/>
       <c r="Q34" s="21">
         <v>2</v>
       </c>
@@ -2897,7 +2926,7 @@
         <f t="shared" si="47"/>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V34" s="28"/>
+      <c r="V34" s="31"/>
       <c r="W34" s="21">
         <v>2</v>
       </c>
@@ -2913,7 +2942,7 @@
         <f t="shared" si="49"/>
         <v>71.350925324956492</v>
       </c>
-      <c r="AC34" s="28"/>
+      <c r="AC34" s="31"/>
       <c r="AD34" s="21">
         <v>2</v>
       </c>
@@ -2932,37 +2961,37 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:42">
-      <c r="D35" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D35" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="R35" s="27" t="s">
+      <c r="R35" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="X35" s="27" t="s">
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="X35" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y35" s="27"/>
-      <c r="Z35" s="27"/>
-      <c r="AE35" s="27" t="s">
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+      <c r="AE35" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF35" s="27"/>
-      <c r="AG35" s="27"/>
+      <c r="AF35" s="30"/>
+      <c r="AG35" s="30"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -3034,7 +3063,7 @@
         <v>2.8396167479260592</v>
       </c>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3047,55 +3076,55 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="X37" s="25" t="s">
+      <c r="X37" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
+      <c r="Y37" s="28"/>
+      <c r="Z37" s="28"/>
       <c r="AA37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB37" s="8"/>
-      <c r="AE37" s="27" t="s">
+      <c r="AE37" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF37" s="27"/>
-      <c r="AG37" s="27"/>
+      <c r="AF37" s="30"/>
+      <c r="AG37" s="30"/>
       <c r="AH37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:42">
-      <c r="D38" s="25" t="s">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D38" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="N38" s="1"/>
-      <c r="R38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
-      <c r="X38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
-      <c r="AE38" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="25"/>
-      <c r="AG38" s="25"/>
+      <c r="R38" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="X38" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="28"/>
+      <c r="Z38" s="28"/>
+      <c r="AE38" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="28"/>
+      <c r="AG38" s="28"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D39" s="1">
         <v>1</v>
       </c>
@@ -3139,11 +3168,11 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2000</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="21">
@@ -3183,7 +3212,7 @@
         <f>M40/L$40</f>
         <v>2.5568845446814027E-2</v>
       </c>
-      <c r="P40" s="28" t="s">
+      <c r="P40" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q40" s="21">
@@ -3201,7 +3230,7 @@
         <f t="shared" ref="T40:T41" si="59">LN(F47) - LN(F40)</f>
         <v>0.13353139262452252</v>
       </c>
-      <c r="V40" s="28" t="s">
+      <c r="V40" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W40" s="21">
@@ -3219,7 +3248,7 @@
         <f t="shared" ref="Z40:Z41" si="61">$M40*T40</f>
         <v>2.665651423580965</v>
       </c>
-      <c r="AC40" s="28" t="s">
+      <c r="AC40" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD40" s="21">
@@ -3240,8 +3269,8 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="1:42">
-      <c r="B41" s="28"/>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B41" s="31"/>
       <c r="C41" s="21">
         <v>2</v>
       </c>
@@ -3269,7 +3298,7 @@
         <f>M41/L$40</f>
         <v>0.97162630393947746</v>
       </c>
-      <c r="P41" s="28"/>
+      <c r="P41" s="31"/>
       <c r="Q41" s="21">
         <v>2</v>
       </c>
@@ -3285,7 +3314,7 @@
         <f t="shared" si="59"/>
         <v>0.11778303565638382</v>
       </c>
-      <c r="V41" s="28"/>
+      <c r="V41" s="31"/>
       <c r="W41" s="21">
         <v>2</v>
       </c>
@@ -3301,7 +3330,7 @@
         <f t="shared" si="61"/>
         <v>89.349241143602967</v>
       </c>
-      <c r="AC41" s="28"/>
+      <c r="AC41" s="31"/>
       <c r="AD41" s="21">
         <v>2</v>
       </c>
@@ -3320,37 +3349,37 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="1:42">
-      <c r="D42" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D42" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
       <c r="G42" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="R42" s="27" t="s">
+      <c r="R42" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="X42" s="27" t="s">
+      <c r="S42" s="30"/>
+      <c r="T42" s="30"/>
+      <c r="X42" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="27"/>
-      <c r="AE42" s="27" t="s">
+      <c r="Y42" s="30"/>
+      <c r="Z42" s="30"/>
+      <c r="AE42" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF42" s="27"/>
-      <c r="AG42" s="27"/>
+      <c r="AF42" s="30"/>
+      <c r="AG42" s="30"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -3422,7 +3451,7 @@
         <v>3.1947998282292427</v>
       </c>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3435,36 +3464,36 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="X44" s="25" t="s">
+      <c r="X44" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y44" s="25"/>
-      <c r="Z44" s="25"/>
+      <c r="Y44" s="28"/>
+      <c r="Z44" s="28"/>
       <c r="AA44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB44" s="8"/>
-      <c r="AE44" s="27" t="s">
+      <c r="AE44" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF44" s="27"/>
-      <c r="AG44" s="27"/>
+      <c r="AF44" s="30"/>
+      <c r="AG44" s="30"/>
       <c r="AH44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="1:42">
-      <c r="D45" s="25" t="s">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D45" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D46" s="1">
         <v>1</v>
       </c>
@@ -3477,11 +3506,11 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2010</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="21">
@@ -3503,8 +3532,8 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="1:42">
-      <c r="B48" s="28"/>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B48" s="31"/>
       <c r="C48" s="21">
         <v>2</v>
       </c>
@@ -3524,12 +3553,12 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="1:37">
-      <c r="D49" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="D49" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
       <c r="G49" s="7" t="s">
         <v>4</v>
       </c>
@@ -3544,7 +3573,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -3558,7 +3587,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -3571,15 +3600,15 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="1:37" ht="17">
+    <row r="54" spans="1:37" ht="17" x14ac:dyDescent="0.2">
       <c r="P54" s="20" t="s">
         <v>14</v>
       </c>
@@ -3592,13 +3621,13 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="U55" s="6"/>
       <c r="V55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="U56" s="6"/>
       <c r="V56" t="s">
         <v>17</v>
@@ -3705,14 +3734,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AP47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI15" sqref="AI15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -3748,172 +3777,114 @@
     <col min="51" max="51" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="AJ2" s="25" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AN2" s="25" t="s">
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AN2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-    </row>
-    <row r="3" spans="1:42">
-      <c r="D3" s="25" t="s">
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="R3" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="X3" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AE3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AJ3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AN3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-    </row>
-    <row r="4" spans="1:42">
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="2">
-        <v>1</v>
-      </c>
-      <c r="S4" s="2">
-        <v>2</v>
-      </c>
-      <c r="T4" s="2">
-        <v>3</v>
-      </c>
-      <c r="X4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AL4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AN4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AP4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42">
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D4" s="27">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27">
+        <v>2</v>
+      </c>
+      <c r="F4" s="27">
+        <v>3</v>
+      </c>
+      <c r="AJ4" s="27"/>
+      <c r="AK4" s="27"/>
+      <c r="AL4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="27"/>
+      <c r="AP4" s="27"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1971</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="21">
@@ -3932,85 +3903,15 @@
         <f>PRODUCT(D5:F5)</f>
         <v>20</v>
       </c>
-      <c r="I5" s="17">
-        <f>G15/G8</f>
-        <v>2.25</v>
-      </c>
-      <c r="J5" s="18">
-        <f>G15-G8</f>
-        <v>100</v>
-      </c>
-      <c r="L5" s="14">
-        <f>(G15-G8) / (LN(G15) - LN(G8))</f>
-        <v>123.31517311882152</v>
-      </c>
-      <c r="M5" s="15">
-        <f>(G12-G5) / (LN(G12) - LN(G5))</f>
-        <v>36.409569065073498</v>
-      </c>
-      <c r="N5" s="16">
-        <f>M5/L$5</f>
-        <v>0.29525619714283424</v>
-      </c>
-      <c r="P5" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>1</v>
-      </c>
-      <c r="R5" s="4">
-        <f>LN(D12) - LN(D5)</f>
-        <v>1.3862943611198906</v>
-      </c>
-      <c r="S5" s="4">
-        <f>LN(E12) - LN(E5)</f>
-        <v>-0.69314718055994562</v>
-      </c>
-      <c r="T5" s="4">
-        <f>LN(F12) - LN(F5)</f>
-        <v>0.4054651081081645</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="W5" s="21">
-        <v>1</v>
-      </c>
-      <c r="X5" s="4">
-        <f>$M5*R5</f>
-        <v>50.474380285716599</v>
-      </c>
-      <c r="Y5" s="4">
-        <f t="shared" ref="Y5:Z6" si="0">$M5*S5</f>
-        <v>-25.23719014285831</v>
-      </c>
-      <c r="Z5" s="4">
-        <f t="shared" si="0"/>
-        <v>14.762809857141708</v>
-      </c>
-      <c r="AC5" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="4">
-        <f>$N5*R5</f>
-        <v>0.40931200118481387</v>
-      </c>
-      <c r="AF5" s="4">
-        <f t="shared" ref="AF5:AG6" si="1">$N5*S5</f>
-        <v>-0.20465600059240702</v>
-      </c>
-      <c r="AG5" s="4">
-        <f t="shared" si="1"/>
-        <v>0.11971608589412482</v>
-      </c>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
-    </row>
-    <row r="6" spans="1:42">
-      <c r="B6" s="28"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AN5" s="27"/>
+      <c r="AO5" s="27"/>
+      <c r="AP5" s="27"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B6" s="31"/>
       <c r="C6" s="21">
         <v>2</v>
       </c>
@@ -4027,221 +3928,89 @@
         <f>PRODUCT(D6:F6)</f>
         <v>60</v>
       </c>
-      <c r="M6" s="15">
-        <f>(G13-G6) / (LN(G13) - LN(G6))</f>
-        <v>86.561702453337787</v>
-      </c>
-      <c r="N6" s="16">
-        <f>M6/L$5</f>
-        <v>0.70195500086538765</v>
-      </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="21">
-        <v>2</v>
-      </c>
-      <c r="R6" s="4">
-        <f>LN(D13) - LN(D6)</f>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="S6" s="4">
-        <f t="shared" ref="S6:T6" si="2">LN(E13) - LN(E6)</f>
-        <v>0.18232155679395468</v>
-      </c>
-      <c r="T6" s="4">
-        <f t="shared" si="2"/>
-        <v>0.28768207245178079</v>
-      </c>
-      <c r="V6" s="28"/>
-      <c r="W6" s="21">
-        <v>2</v>
-      </c>
-      <c r="X6" s="4">
-        <f>$M6*R6</f>
-        <v>19.315685693241733</v>
-      </c>
-      <c r="Y6" s="4">
-        <f t="shared" si="0"/>
-        <v>15.782064350027632</v>
-      </c>
-      <c r="Z6" s="4">
-        <f t="shared" si="0"/>
-        <v>24.902249956730611</v>
-      </c>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="21">
-        <v>2</v>
-      </c>
-      <c r="AE6" s="4">
-        <f>$N6*R6</f>
-        <v>0.15663673175587176</v>
-      </c>
-      <c r="AF6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12798152855707928</v>
-      </c>
-      <c r="AG6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2019398694168463</v>
-      </c>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-    </row>
-    <row r="7" spans="1:42">
-      <c r="D7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="7" t="s">
+      <c r="AJ6" s="27"/>
+      <c r="AK6" s="27"/>
+      <c r="AL6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27"/>
+      <c r="AP6" s="27"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="R7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="X7" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AE7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-    </row>
-    <row r="8" spans="1:42">
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="27"/>
+      <c r="AL7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="13">
         <f>SUM(G5:G6)</f>
         <v>80</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="N8" s="2"/>
-      <c r="X8" s="4">
-        <f>SUM(X5:X6)</f>
-        <v>69.790065978958324</v>
-      </c>
-      <c r="Y8" s="4">
-        <f t="shared" ref="Y8:Z8" si="3">SUM(Y5:Y6)</f>
-        <v>-9.4551257928306782</v>
-      </c>
-      <c r="Z8" s="4">
-        <f t="shared" si="3"/>
-        <v>39.665059813872318</v>
-      </c>
-      <c r="AA8" s="18">
-        <f>SUM(X8:Z8)</f>
-        <v>99.999999999999972</v>
-      </c>
-      <c r="AB8" s="19"/>
-      <c r="AE8" s="4">
-        <f>EXP(SUM(AE5:AE6))</f>
-        <v>1.7611178208755378</v>
-      </c>
-      <c r="AF8" s="4">
-        <f t="shared" ref="AF8:AG8" si="4">EXP(SUM(AF5:AF6))</f>
-        <v>0.92619130570893327</v>
-      </c>
-      <c r="AG8" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3794101155854785</v>
-      </c>
-      <c r="AH8" s="17">
-        <f>PRODUCT(AE8:AG8)</f>
-        <v>2.2500000000000004</v>
-      </c>
-      <c r="AJ8" s="4">
-        <f>X8</f>
-        <v>69.790065978958324</v>
-      </c>
-      <c r="AK8" s="4">
-        <f t="shared" ref="AK8:AL8" si="5">Y8</f>
-        <v>-9.4551257928306782</v>
-      </c>
-      <c r="AL8" s="4">
-        <f t="shared" si="5"/>
-        <v>39.665059813872318</v>
-      </c>
-      <c r="AN8" s="4">
-        <f>AE8</f>
-        <v>1.7611178208755378</v>
-      </c>
-      <c r="AO8" s="4">
-        <f t="shared" ref="AO8:AP8" si="6">AF8</f>
-        <v>0.92619130570893327</v>
-      </c>
-      <c r="AP8" s="4">
-        <f t="shared" si="6"/>
-        <v>1.3794101155854785</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
       <c r="G9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="M9">
-        <f>M6/L12</f>
-        <v>0.41594614744177039</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="X9" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB9" s="8"/>
-      <c r="AE9" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-    </row>
-    <row r="10" spans="1:42">
-      <c r="D10" s="25" t="s">
+      <c r="AJ9" s="27"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="N10" s="2"/>
-      <c r="R10" s="25" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="R10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="X10" s="25" t="s">
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="X10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AE10" s="25" t="s">
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AE10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="2"/>
-    </row>
-    <row r="11" spans="1:42">
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AJ10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK10" s="28"/>
+      <c r="AL10" s="28"/>
+      <c r="AN10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO10" s="28"/>
+      <c r="AP10" s="28"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D11" s="2">
         <v>1</v>
       </c>
@@ -4251,105 +4020,114 @@
       <c r="F11" s="2">
         <v>3</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="N11" s="2"/>
-      <c r="R11" s="2">
-        <v>1</v>
-      </c>
-      <c r="S11" s="2">
-        <v>2</v>
-      </c>
-      <c r="T11" s="2">
-        <v>3</v>
-      </c>
-      <c r="X11" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="2">
-        <v>2</v>
-      </c>
-      <c r="AG11" s="2">
-        <v>3</v>
-      </c>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-    </row>
-    <row r="12" spans="1:42" ht="16" customHeight="1">
+      <c r="R11" s="27">
+        <v>1</v>
+      </c>
+      <c r="S11" s="27">
+        <v>2</v>
+      </c>
+      <c r="T11" s="27">
+        <v>3</v>
+      </c>
+      <c r="X11" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="27">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="27">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="27">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="27">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1972</v>
-      </c>
-      <c r="B12" s="28" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="21">
         <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="12">
         <f>PRODUCT(D12:F12)</f>
-        <v>60</v>
-      </c>
-      <c r="H12" s="9"/>
+        <v>20</v>
+      </c>
       <c r="I12" s="17">
-        <f>G22/G15</f>
-        <v>1.3277777777777777</v>
+        <f>G15/G8</f>
+        <v>1</v>
       </c>
       <c r="J12" s="18">
-        <f>G22-G15</f>
-        <v>59</v>
-      </c>
-      <c r="K12" s="9"/>
+        <f>G15-G8</f>
+        <v>0</v>
+      </c>
       <c r="L12" s="14">
-        <f>(G22-G15) / (LN(G22) - LN(G15))</f>
-        <v>208.10795576717257</v>
+        <f>G15</f>
+        <v>80</v>
       </c>
       <c r="M12" s="15">
-        <f>(G19-G12) / (LN(G19) - LN(G12))</f>
-        <v>61.978488652901611</v>
+        <f>G12</f>
+        <v>20</v>
       </c>
       <c r="N12" s="16">
         <f>M12/L$12</f>
-        <v>0.29781892972050539</v>
-      </c>
-      <c r="P12" s="28" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="P12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q12" s="21">
         <v>1</v>
       </c>
       <c r="R12" s="4">
-        <f>LN(D19) - LN(D12)</f>
-        <v>0.69314718055994518</v>
+        <f>LN(D12) - LN(D5)</f>
+        <v>0</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" ref="S12:T13" si="7">LN(E19) - LN(E12)</f>
-        <v>-0.916290731874155</v>
+        <f>LN(E12) - LN(E5)</f>
+        <v>0</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="7"/>
-        <v>0.28768207245178079</v>
-      </c>
-      <c r="V12" s="28" t="s">
+        <f>LN(F12) - LN(F5)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="21">
@@ -4357,17 +4135,17 @@
       </c>
       <c r="X12" s="4">
         <f>$M12*R12</f>
-        <v>42.960214665125307</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="4">
-        <f t="shared" ref="Y12:Z13" si="8">$M12*S12</f>
-        <v>-56.790314728221226</v>
+        <f>$M12*S12</f>
+        <v>0</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="8"/>
-        <v>17.830100063095916</v>
-      </c>
-      <c r="AC12" s="28" t="s">
+        <f>$M12*T12</f>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD12" s="21">
@@ -4375,66 +4153,60 @@
       </c>
       <c r="AE12" s="4">
         <f>$N12*R12</f>
-        <v>0.20643235145314878</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="4">
-        <f t="shared" ref="AF12:AG13" si="9">$N12*S12</f>
-        <v>-0.2728887250795794</v>
+        <f>$N12*S12</f>
+        <v>0</v>
       </c>
       <c r="AG12" s="4">
-        <f t="shared" si="9"/>
-        <v>8.5677166917366238E-2</v>
-      </c>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-    </row>
-    <row r="13" spans="1:42">
-      <c r="B13" s="28"/>
+        <f>$N12*T12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B13" s="31"/>
       <c r="C13" s="21">
         <v>2</v>
       </c>
       <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4">
         <v>5</v>
       </c>
-      <c r="E13" s="4">
-        <v>6</v>
-      </c>
       <c r="F13" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="12">
         <f>PRODUCT(D13:F13)</f>
-        <v>120</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+        <v>60</v>
+      </c>
       <c r="M13" s="15">
-        <f>(G20-G13) / (LN(G20) - LN(G13))</f>
-        <v>145.77482362664972</v>
+        <f>G13</f>
+        <v>60</v>
       </c>
       <c r="N13" s="16">
         <f>M13/L$12</f>
-        <v>0.70047693798760857</v>
-      </c>
-      <c r="P13" s="28"/>
+        <v>0.75</v>
+      </c>
+      <c r="P13" s="31"/>
       <c r="Q13" s="21">
         <v>2</v>
       </c>
       <c r="R13" s="4">
-        <f>LN(D20) - LN(D13)</f>
+        <f>LN(D13) - LN(D6)</f>
         <v>0</v>
       </c>
       <c r="S13" s="4">
-        <f t="shared" si="7"/>
-        <v>0.15415067982725827</v>
+        <f>LN(E13) - LN(E6)</f>
+        <v>0</v>
       </c>
       <c r="T13" s="4">
-        <f t="shared" si="7"/>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="V13" s="28"/>
+        <f>LN(F13) - LN(F6)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="31"/>
       <c r="W13" s="21">
         <v>2</v>
       </c>
@@ -4444,13 +4216,13 @@
       </c>
       <c r="Y13" s="4">
         <f>$M13*S13</f>
-        <v>22.471288163746728</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="4">
-        <f t="shared" si="8"/>
-        <v>32.52871183625318</v>
-      </c>
-      <c r="AC13" s="28"/>
+        <f>$M13*T13</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="31"/>
       <c r="AD13" s="21">
         <v>2</v>
       </c>
@@ -4459,184 +4231,152 @@
         <v>0</v>
       </c>
       <c r="AF13" s="4">
-        <f t="shared" si="9"/>
-        <v>0.1079789961941061</v>
+        <f>$N13*S13</f>
+        <v>0</v>
       </c>
       <c r="AG13" s="4">
-        <f t="shared" si="9"/>
-        <v>0.15630691155625842</v>
-      </c>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-    </row>
-    <row r="14" spans="1:42">
-      <c r="D14" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+        <f>$N13*T13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D14" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="R14" s="27" t="s">
+      <c r="R14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="X14" s="27" t="s">
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="X14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AE14" s="27" t="s">
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AE14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-    </row>
-    <row r="15" spans="1:42">
-      <c r="A15" s="9"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="G15" s="13">
         <f>SUM(G12:G13)</f>
-        <v>180</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="K15" s="3"/>
       <c r="X15" s="4">
         <f>SUM(X12:X13)</f>
-        <v>42.960214665125307</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="4">
-        <f t="shared" ref="Y15:Z15" si="10">SUM(Y12:Y13)</f>
-        <v>-34.319026564474498</v>
+        <f t="shared" ref="Y15:Z15" si="0">SUM(Y12:Y13)</f>
+        <v>0</v>
       </c>
       <c r="Z15" s="4">
-        <f t="shared" si="10"/>
-        <v>50.358811899349092</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="AA15" s="18">
         <f>SUM(X15:Z15)</f>
-        <v>58.999999999999901</v>
-      </c>
-      <c r="AB15" s="19"/>
+        <v>0</v>
+      </c>
       <c r="AE15" s="4">
         <f>EXP(SUM(AE12:AE13))</f>
-        <v>1.2292845720892271</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="4">
-        <f t="shared" ref="AF15:AG15" si="11">EXP(SUM(AF12:AF13))</f>
-        <v>0.84797024785237751</v>
+        <f t="shared" ref="AF15:AG15" si="1">EXP(SUM(AF12:AF13))</f>
+        <v>1</v>
       </c>
       <c r="AG15" s="4">
-        <f t="shared" si="11"/>
-        <v>1.2737739122298066</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AH15" s="17">
         <f>PRODUCT(AE15:AG15)</f>
-        <v>1.3277777777777777</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="4">
-        <f>AJ8+X15</f>
-        <v>112.75028064408363</v>
+        <f>X15</f>
+        <v>0</v>
       </c>
       <c r="AK15" s="4">
-        <f t="shared" ref="AK15:AL15" si="12">AK8+Y15</f>
-        <v>-43.774152357305177</v>
+        <f t="shared" ref="AK15" si="2">Y15</f>
+        <v>0</v>
       </c>
       <c r="AL15" s="4">
-        <f t="shared" si="12"/>
-        <v>90.023871713221411</v>
+        <f t="shared" ref="AL15" si="3">Z15</f>
+        <v>0</v>
       </c>
       <c r="AN15" s="4">
-        <f>AN8*AE15</f>
-        <v>2.1649149668336976</v>
+        <f>AE15</f>
+        <v>1</v>
       </c>
       <c r="AO15" s="4">
-        <f t="shared" ref="AO15:AP15" si="13">AO8*AF15</f>
-        <v>0.78538267106072124</v>
+        <f t="shared" ref="AO15" si="4">AF15</f>
+        <v>1</v>
       </c>
       <c r="AP15" s="4">
-        <f t="shared" si="13"/>
-        <v>1.7570566194986847</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
+        <f t="shared" ref="AP15" si="5">AG15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="G16" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="X16" s="25" t="s">
+      <c r="X16" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
-      <c r="AA16" s="2" t="s">
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AB16" s="8"/>
-      <c r="AE16" s="27" t="s">
+      <c r="AE16" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="2" t="s">
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
-    </row>
-    <row r="17" spans="1:42">
-      <c r="D17" s="25" t="s">
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="N17" s="2"/>
-      <c r="R17" s="25" t="s">
+      <c r="R17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="X17" s="25" t="s">
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="X17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AE17" s="25" t="s">
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AE17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
-    </row>
-    <row r="18" spans="1:42">
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D18" s="2">
         <v>1</v>
       </c>
@@ -4647,10 +4387,7 @@
         <v>3</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-      <c r="N18" s="2"/>
       <c r="R18" s="2">
         <v>1</v>
       </c>
@@ -4678,73 +4415,71 @@
       <c r="AG18" s="2">
         <v>3</v>
       </c>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
-    </row>
-    <row r="19" spans="1:42" ht="16" customHeight="1">
+    </row>
+    <row r="19" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1973</v>
-      </c>
-      <c r="B19" s="28" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="21">
         <v>1</v>
       </c>
       <c r="D19" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E19" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="12">
         <f>PRODUCT(D19:F19)</f>
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="17">
-        <f>G29/G22</f>
-        <v>1.4142259414225942</v>
+        <f>G22/G15</f>
+        <v>2.25</v>
       </c>
       <c r="J19" s="18">
-        <f>G29-G22</f>
-        <v>99</v>
+        <f>G22-G15</f>
+        <v>100</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="14">
-        <f>(G29-G22) / (LN(G29) - LN(G22))</f>
-        <v>285.64640363823662</v>
+        <f>(G22-G15) / (LN(G22) - LN(G15))</f>
+        <v>123.31517311882152</v>
       </c>
       <c r="M19" s="15">
-        <f>(G26-G19) / (LN(G26) - LN(G19))</f>
-        <v>56.712288666956283</v>
+        <f>(G19-G12) / (LN(G19) - LN(G12))</f>
+        <v>36.409569065073498</v>
       </c>
       <c r="N19" s="16">
         <f>M19/L$19</f>
-        <v>0.19854018095316492</v>
-      </c>
-      <c r="P19" s="28" t="s">
+        <v>0.29525619714283424</v>
+      </c>
+      <c r="P19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="Q19" s="21">
         <v>1</v>
       </c>
       <c r="R19" s="4">
-        <f t="shared" ref="R19:T20" si="14">LN(D26) - LN(D19)</f>
-        <v>0.22314355131421015</v>
+        <f>LN(D19) - LN(D12)</f>
+        <v>1.3862943611198906</v>
       </c>
       <c r="S19" s="4">
-        <f t="shared" si="14"/>
-        <v>-0.69314718055994529</v>
+        <f>LN(E19) - LN(E12)</f>
+        <v>-0.69314718055994562</v>
       </c>
       <c r="T19" s="4">
-        <f t="shared" si="14"/>
-        <v>0.22314355131420971</v>
-      </c>
-      <c r="V19" s="28" t="s">
+        <f>LN(F19) - LN(F12)</f>
+        <v>0.4054651081081645</v>
+      </c>
+      <c r="V19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="W19" s="21">
@@ -4752,17 +4487,17 @@
       </c>
       <c r="X19" s="4">
         <f>$M19*R19</f>
-        <v>12.654981496301259</v>
+        <v>50.474380285716599</v>
       </c>
       <c r="Y19" s="4">
-        <f t="shared" ref="Y19:Z20" si="15">$M19*S19</f>
-        <v>-39.309962992602486</v>
+        <f>$M19*S19</f>
+        <v>-25.23719014285831</v>
       </c>
       <c r="Z19" s="4">
-        <f t="shared" si="15"/>
-        <v>12.654981496301232</v>
-      </c>
-      <c r="AC19" s="28" t="s">
+        <f>$M19*T19</f>
+        <v>14.762809857141708</v>
+      </c>
+      <c r="AC19" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AD19" s="21">
@@ -4770,21 +4505,21 @@
       </c>
       <c r="AE19" s="4">
         <f>$N19*R19</f>
-        <v>4.4302961056455127E-2</v>
+        <v>0.40931200118481387</v>
       </c>
       <c r="AF19" s="4">
-        <f t="shared" ref="AF19:AG20" si="16">$N19*S19</f>
-        <v>-0.13761756665554761</v>
+        <f>$N19*S19</f>
+        <v>-0.20465600059240702</v>
       </c>
       <c r="AG19" s="4">
-        <f t="shared" si="16"/>
-        <v>4.4302961056455037E-2</v>
+        <f>$N19*T19</f>
+        <v>0.11971608589412482</v>
       </c>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="1:42">
-      <c r="B20" s="28"/>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B20" s="31"/>
       <c r="C20" s="21">
         <v>2</v>
       </c>
@@ -4792,183 +4527,179 @@
         <v>5</v>
       </c>
       <c r="E20" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G20" s="12">
         <f>PRODUCT(D20:F20)</f>
-        <v>175</v>
+        <v>120</v>
       </c>
       <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="M20" s="15">
-        <f>(G27-G20) / (LN(G27) - LN(G20))</f>
-        <v>226.82814674545895</v>
+        <f>(G20-G13) / (LN(G20) - LN(G13))</f>
+        <v>86.561702453337787</v>
       </c>
       <c r="N20" s="16">
         <f>M20/L$19</f>
-        <v>0.79408717861097466</v>
-      </c>
-      <c r="P20" s="28"/>
+        <v>0.70195500086538765</v>
+      </c>
+      <c r="P20" s="31"/>
       <c r="Q20" s="21">
         <v>2</v>
       </c>
       <c r="R20" s="4">
-        <f t="shared" si="14"/>
+        <f>LN(D20) - LN(D13)</f>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="S20" s="4">
+        <f>LN(E20) - LN(E13)</f>
         <v>0.18232155679395468</v>
       </c>
-      <c r="S20" s="4">
-        <f t="shared" si="14"/>
-        <v>0.13353139262452252</v>
-      </c>
       <c r="T20" s="4">
-        <f t="shared" si="14"/>
-        <v>0.18232155679395468</v>
-      </c>
-      <c r="V20" s="28"/>
+        <f>LN(F20) - LN(F13)</f>
+        <v>0.28768207245178079</v>
+      </c>
+      <c r="V20" s="31"/>
       <c r="W20" s="21">
         <v>2</v>
       </c>
       <c r="X20" s="4">
         <f>$M20*R20</f>
-        <v>41.355660839319683</v>
+        <v>19.315685693241733</v>
       </c>
       <c r="Y20" s="4">
-        <f t="shared" si="15"/>
-        <v>30.288678321360688</v>
+        <f>$M20*S20</f>
+        <v>15.782064350027632</v>
       </c>
       <c r="Z20" s="4">
-        <f t="shared" si="15"/>
-        <v>41.355660839319683</v>
-      </c>
-      <c r="AC20" s="28"/>
+        <f>$M20*T20</f>
+        <v>24.902249956730611</v>
+      </c>
+      <c r="AC20" s="31"/>
       <c r="AD20" s="21">
         <v>2</v>
       </c>
       <c r="AE20" s="4">
         <f>$N20*R20</f>
-        <v>0.14477921063447205</v>
+        <v>0.15663673175587176</v>
       </c>
       <c r="AF20" s="4">
-        <f t="shared" si="16"/>
-        <v>0.10603556682520139</v>
+        <f>$N20*S20</f>
+        <v>0.12798152855707928</v>
       </c>
       <c r="AG20" s="4">
-        <f t="shared" si="16"/>
-        <v>0.14477921063447205</v>
+        <f>$N20*T20</f>
+        <v>0.2019398694168463</v>
       </c>
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="1:42">
-      <c r="D21" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D21" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="R21" s="27" t="s">
+      <c r="N21" s="2"/>
+      <c r="R21" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="X21" s="27" t="s">
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="X21" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
-      <c r="AE21" s="27" t="s">
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AE21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="27"/>
+      <c r="AF21" s="30"/>
+      <c r="AG21" s="30"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="9"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
       <c r="G22" s="13">
         <f>SUM(G19:G20)</f>
-        <v>239</v>
+        <v>180</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
       <c r="K22" s="9"/>
+      <c r="N22" s="2"/>
       <c r="X22" s="4">
         <f>SUM(X19:X20)</f>
-        <v>54.010642335620943</v>
+        <v>69.790065978958324</v>
       </c>
       <c r="Y22" s="4">
-        <f t="shared" ref="Y22:Z22" si="17">SUM(Y19:Y20)</f>
-        <v>-9.0212846712417978</v>
+        <f t="shared" ref="Y22:Z22" si="6">SUM(Y19:Y20)</f>
+        <v>-9.4551257928306782</v>
       </c>
       <c r="Z22" s="4">
-        <f t="shared" si="17"/>
-        <v>54.010642335620915</v>
+        <f t="shared" si="6"/>
+        <v>39.665059813872318</v>
       </c>
       <c r="AA22" s="18">
         <f>SUM(X22:Z22)</f>
-        <v>99.000000000000057</v>
+        <v>99.999999999999972</v>
       </c>
       <c r="AB22" s="19"/>
       <c r="AE22" s="4">
         <f>EXP(SUM(AE19:AE20))</f>
-        <v>1.2081402233292473</v>
+        <v>1.7611178208755378</v>
       </c>
       <c r="AF22" s="4">
-        <f t="shared" ref="AF22:AG22" si="18">EXP(SUM(AF19:AF20))</f>
-        <v>0.96891150261734849</v>
+        <f t="shared" ref="AF22:AG22" si="7">EXP(SUM(AF19:AF20))</f>
+        <v>0.92619130570893327</v>
       </c>
       <c r="AG22" s="4">
-        <f t="shared" si="18"/>
-        <v>1.2081402233292473</v>
+        <f t="shared" si="7"/>
+        <v>1.3794101155854785</v>
       </c>
       <c r="AH22" s="17">
         <f>PRODUCT(AE22:AG22)</f>
-        <v>1.4142259414225939</v>
+        <v>2.2500000000000004</v>
       </c>
       <c r="AJ22" s="4">
-        <f>AJ15+X22</f>
-        <v>166.76092297970456</v>
+        <f>X22</f>
+        <v>69.790065978958324</v>
       </c>
       <c r="AK22" s="4">
-        <f t="shared" ref="AK22:AL22" si="19">AK15+Y22</f>
-        <v>-52.795437028546971</v>
+        <f t="shared" ref="AK22:AL22" si="8">Y22</f>
+        <v>-9.4551257928306782</v>
       </c>
       <c r="AL22" s="4">
-        <f t="shared" si="19"/>
-        <v>144.03451404884231</v>
+        <f t="shared" si="8"/>
+        <v>39.665059813872318</v>
       </c>
       <c r="AN22" s="4">
-        <f>AN15*AE22</f>
-        <v>2.6155208515192934</v>
+        <f>AE22</f>
+        <v>1.7611178208755378</v>
       </c>
       <c r="AO22" s="4">
-        <f t="shared" ref="AO22:AP22" si="20">AO15*AF22</f>
-        <v>0.7609663039470701</v>
+        <f t="shared" ref="AO22:AP22" si="9">AF22</f>
+        <v>0.92619130570893327</v>
       </c>
       <c r="AP22" s="4">
-        <f t="shared" si="20"/>
-        <v>2.1227707766832733</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42">
+        <f t="shared" si="9"/>
+        <v>1.3794101155854785</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4979,71 +4710,58 @@
         <v>0</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="X23" s="25" t="s">
+      <c r="N23" s="2"/>
+      <c r="X23" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="28"/>
       <c r="AA23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB23" s="8"/>
-      <c r="AE23" s="27" t="s">
+      <c r="AE23" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AF23" s="27"/>
-      <c r="AG23" s="27"/>
+      <c r="AF23" s="30"/>
+      <c r="AG23" s="30"/>
       <c r="AH23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="1:42">
-      <c r="D24" s="25" t="s">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="10"/>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="10"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="8"/>
-      <c r="AK24" s="8"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
-      <c r="AP24" s="9"/>
-    </row>
-    <row r="25" spans="1:42">
+      <c r="N24" s="27"/>
+      <c r="R24" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="X24" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AE24" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
+      <c r="AJ24" s="27"/>
+      <c r="AK24" s="27"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D25" s="2">
         <v>1</v>
       </c>
@@ -5057,154 +4775,226 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="8"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AJ25" s="8"/>
-      <c r="AK25" s="8"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
-      <c r="AP25" s="9"/>
-    </row>
-    <row r="26" spans="1:42" ht="16" customHeight="1">
+      <c r="N25" s="27"/>
+      <c r="R25" s="27">
+        <v>1</v>
+      </c>
+      <c r="S25" s="27">
+        <v>2</v>
+      </c>
+      <c r="T25" s="27">
+        <v>3</v>
+      </c>
+      <c r="X25" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="27">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="27">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF25" s="27">
+        <v>2</v>
+      </c>
+      <c r="AG25" s="27">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="27"/>
+      <c r="AK25" s="27"/>
+    </row>
+    <row r="26" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1974</v>
-      </c>
-      <c r="B26" s="28" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="21">
         <v>1</v>
       </c>
       <c r="D26" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G26" s="12">
         <f>PRODUCT(D26:F26)</f>
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="H26" s="9"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
+      <c r="I26" s="17">
+        <f>G29/G22</f>
+        <v>1.3277777777777777</v>
+      </c>
+      <c r="J26" s="18">
+        <f>G29-G22</f>
+        <v>59</v>
+      </c>
       <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="9"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="22"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-    </row>
-    <row r="27" spans="1:42">
-      <c r="B27" s="28"/>
+      <c r="L26" s="14">
+        <f>(G29-G22) / (LN(G29) - LN(G22))</f>
+        <v>208.10795576717257</v>
+      </c>
+      <c r="M26" s="15">
+        <f>(G26-G19) / (LN(G26) - LN(G19))</f>
+        <v>61.978488652901611</v>
+      </c>
+      <c r="N26" s="16">
+        <f>M26/L$26</f>
+        <v>0.29781892972050539</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>1</v>
+      </c>
+      <c r="R26" s="4">
+        <f>LN(D26) - LN(D19)</f>
+        <v>0.69314718055994518</v>
+      </c>
+      <c r="S26" s="4">
+        <f>LN(E26) - LN(E19)</f>
+        <v>-0.916290731874155</v>
+      </c>
+      <c r="T26" s="4">
+        <f>LN(F26) - LN(F19)</f>
+        <v>0.28768207245178079</v>
+      </c>
+      <c r="V26" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="W26" s="21">
+        <v>1</v>
+      </c>
+      <c r="X26" s="4">
+        <f>$M26*R26</f>
+        <v>42.960214665125307</v>
+      </c>
+      <c r="Y26" s="4">
+        <f>$M26*S26</f>
+        <v>-56.790314728221226</v>
+      </c>
+      <c r="Z26" s="4">
+        <f>$M26*T26</f>
+        <v>17.830100063095916</v>
+      </c>
+      <c r="AC26" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="4">
+        <f>$N26*R26</f>
+        <v>0.20643235145314878</v>
+      </c>
+      <c r="AF26" s="4">
+        <f>$N26*S26</f>
+        <v>-0.2728887250795794</v>
+      </c>
+      <c r="AG26" s="4">
+        <f>$N26*T26</f>
+        <v>8.5677166917366238E-2</v>
+      </c>
+      <c r="AJ26" s="27"/>
+      <c r="AK26" s="27"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B27" s="31"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
       <c r="D27" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" s="12">
         <f>PRODUCT(D27:F27)</f>
-        <v>288</v>
+        <v>175</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="9"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="22"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="8"/>
-      <c r="AK27" s="8"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-    </row>
-    <row r="28" spans="1:42">
-      <c r="D28" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="M27" s="15">
+        <f>(G27-G20) / (LN(G27) - LN(G20))</f>
+        <v>145.77482362664972</v>
+      </c>
+      <c r="N27" s="16">
+        <f>M27/L$26</f>
+        <v>0.70047693798760857</v>
+      </c>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="21">
+        <v>2</v>
+      </c>
+      <c r="R27" s="4">
+        <f>LN(D27) - LN(D20)</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="4">
+        <f>LN(E27) - LN(E20)</f>
+        <v>0.15415067982725827</v>
+      </c>
+      <c r="T27" s="4">
+        <f>LN(F27) - LN(F20)</f>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="V27" s="25"/>
+      <c r="W27" s="21">
+        <v>2</v>
+      </c>
+      <c r="X27" s="4">
+        <f>$M27*R27</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="4">
+        <f>$M27*S27</f>
+        <v>22.471288163746728</v>
+      </c>
+      <c r="Z27" s="4">
+        <f>$M27*T27</f>
+        <v>32.52871183625318</v>
+      </c>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE27" s="4">
+        <f>$N27*R27</f>
+        <v>0</v>
+      </c>
+      <c r="AF27" s="4">
+        <f>$N27*S27</f>
+        <v>0.1079789961941061</v>
+      </c>
+      <c r="AG27" s="4">
+        <f>$N27*T27</f>
+        <v>0.15630691155625842</v>
+      </c>
+      <c r="AJ27" s="27"/>
+      <c r="AK27" s="27"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="7" t="s">
         <v>4</v>
       </c>
@@ -5212,62 +5002,25 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="24">
-        <f>X8+X15+X22</f>
-        <v>166.76092297970456</v>
-      </c>
-      <c r="Y28" s="24">
-        <f t="shared" ref="Y28:AA28" si="21">Y8+Y15+Y22</f>
-        <v>-52.795437028546971</v>
-      </c>
-      <c r="Z28" s="24">
-        <f t="shared" si="21"/>
-        <v>144.03451404884231</v>
-      </c>
-      <c r="AA28" s="24">
-        <f t="shared" si="21"/>
-        <v>257.99999999999994</v>
-      </c>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="24">
-        <f>AE8*AE15*AE22</f>
-        <v>2.6155208515192934</v>
-      </c>
-      <c r="AF28" s="24">
-        <f t="shared" ref="AF28:AH28" si="22">AF8*AF15*AF22</f>
-        <v>0.7609663039470701</v>
-      </c>
-      <c r="AG28" s="24">
-        <f t="shared" si="22"/>
-        <v>2.1227707766832733</v>
-      </c>
-      <c r="AH28" s="24">
-        <f t="shared" si="22"/>
-        <v>4.2249999999999996</v>
-      </c>
-      <c r="AI28" s="9"/>
-      <c r="AJ28" s="8"/>
-      <c r="AK28" s="8"/>
-      <c r="AL28" s="9"/>
-      <c r="AM28" s="9"/>
-      <c r="AN28" s="9"/>
-      <c r="AO28" s="9"/>
-      <c r="AP28" s="9"/>
-    </row>
-    <row r="29" spans="1:42">
+      <c r="R28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="X28" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AE28" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF28" s="30"/>
+      <c r="AG28" s="30"/>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -5276,50 +5029,71 @@
       <c r="F29" s="9"/>
       <c r="G29" s="13">
         <f>SUM(G26:G27)</f>
-        <v>338</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="9">
-        <f>SUM(X28:Z28)</f>
-        <v>257.99999999999989</v>
-      </c>
-      <c r="AA29" s="19"/>
+      <c r="X29" s="4">
+        <f>SUM(X26:X27)</f>
+        <v>42.960214665125307</v>
+      </c>
+      <c r="Y29" s="4">
+        <f t="shared" ref="Y29:Z29" si="10">SUM(Y26:Y27)</f>
+        <v>-34.319026564474498</v>
+      </c>
+      <c r="Z29" s="4">
+        <f t="shared" si="10"/>
+        <v>50.358811899349092</v>
+      </c>
+      <c r="AA29" s="18">
+        <f>SUM(X29:Z29)</f>
+        <v>58.999999999999901</v>
+      </c>
       <c r="AB29" s="19"/>
-      <c r="AC29" s="9"/>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="8">
-        <f>AE28*AF28*AG28</f>
-        <v>4.2249999999999988</v>
-      </c>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="9"/>
-      <c r="AJ29" s="8"/>
-      <c r="AK29" s="8"/>
-      <c r="AL29" s="8"/>
-      <c r="AM29" s="9"/>
-      <c r="AN29" s="8"/>
-      <c r="AO29" s="8"/>
-      <c r="AP29" s="8"/>
-    </row>
-    <row r="30" spans="1:42">
+      <c r="AE29" s="4">
+        <f>EXP(SUM(AE26:AE27))</f>
+        <v>1.2292845720892271</v>
+      </c>
+      <c r="AF29" s="4">
+        <f t="shared" ref="AF29:AG29" si="11">EXP(SUM(AF26:AF27))</f>
+        <v>0.84797024785237751</v>
+      </c>
+      <c r="AG29" s="4">
+        <f t="shared" si="11"/>
+        <v>1.2737739122298066</v>
+      </c>
+      <c r="AH29" s="17">
+        <f>PRODUCT(AE29:AG29)</f>
+        <v>1.3277777777777777</v>
+      </c>
+      <c r="AJ29" s="4">
+        <f>AJ22+X29</f>
+        <v>112.75028064408363</v>
+      </c>
+      <c r="AK29" s="4">
+        <f t="shared" ref="AK29:AL29" si="12">AK22+Y29</f>
+        <v>-43.774152357305177</v>
+      </c>
+      <c r="AL29" s="4">
+        <f t="shared" si="12"/>
+        <v>90.023871713221411</v>
+      </c>
+      <c r="AN29" s="4">
+        <f>AN22*AE29</f>
+        <v>2.1649149668336976</v>
+      </c>
+      <c r="AO29" s="4">
+        <f t="shared" ref="AO29:AP29" si="13">AO22*AF29</f>
+        <v>0.78538267106072124</v>
+      </c>
+      <c r="AP29" s="4">
+        <f t="shared" si="13"/>
+        <v>1.7570566194986847</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -5329,166 +5103,694 @@
       <c r="G30" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="10"/>
-      <c r="Y30" s="10"/>
-      <c r="Z30" s="10"/>
-      <c r="AA30" s="8"/>
+      <c r="X30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="27" t="s">
+        <v>5</v>
+      </c>
       <c r="AB30" s="8"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="24"/>
-      <c r="AF30" s="24"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="8"/>
-      <c r="AI30" s="9"/>
-      <c r="AJ30" s="8"/>
-      <c r="AK30" s="8"/>
-      <c r="AL30" s="9"/>
-      <c r="AM30" s="9"/>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="9"/>
-      <c r="AP30" s="9"/>
-    </row>
-    <row r="31" spans="1:42">
+      <c r="AE30" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
+      <c r="AH30" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AI31" s="9"/>
-      <c r="AJ31" s="9"/>
-      <c r="AK31" s="9"/>
-      <c r="AL31" s="9"/>
-      <c r="AM31" s="9"/>
-      <c r="AN31" s="9"/>
-      <c r="AO31" s="9"/>
-      <c r="AP31" s="9"/>
-    </row>
-    <row r="32" spans="1:42">
+      <c r="N31" s="27"/>
+      <c r="R31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="X31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AE31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="28"/>
+      <c r="AJ31" s="27"/>
+      <c r="AK31" s="27"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="9"/>
-      <c r="AJ32" s="9"/>
-      <c r="AK32" s="9"/>
-      <c r="AL32" s="9"/>
-      <c r="AM32" s="9"/>
-      <c r="AN32" s="9"/>
-      <c r="AO32" s="9"/>
-      <c r="AP32" s="9"/>
-    </row>
-    <row r="33" ht="16" customHeight="1"/>
-    <row r="40" ht="16" customHeight="1"/>
-    <row r="47" ht="16" customHeight="1"/>
+      <c r="N32" s="27"/>
+      <c r="R32" s="27">
+        <v>1</v>
+      </c>
+      <c r="S32" s="27">
+        <v>2</v>
+      </c>
+      <c r="T32" s="27">
+        <v>3</v>
+      </c>
+      <c r="X32" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="27">
+        <v>2</v>
+      </c>
+      <c r="Z32" s="27">
+        <v>3</v>
+      </c>
+      <c r="AE32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="27">
+        <v>2</v>
+      </c>
+      <c r="AG32" s="27">
+        <v>3</v>
+      </c>
+      <c r="AJ32" s="27"/>
+      <c r="AK32" s="27"/>
+    </row>
+    <row r="33" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1974</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="21">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>5</v>
+      </c>
+      <c r="G33" s="12">
+        <f>PRODUCT(D33:F33)</f>
+        <v>50</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="17">
+        <f>G36/G29</f>
+        <v>1.4142259414225942</v>
+      </c>
+      <c r="J33" s="18">
+        <f>G36-G29</f>
+        <v>99</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" s="14">
+        <f>(G36-G29) / (LN(G36) - LN(G29))</f>
+        <v>285.64640363823662</v>
+      </c>
+      <c r="M33" s="15">
+        <f>(G33-G26) / (LN(G33) - LN(G26))</f>
+        <v>56.712288666956283</v>
+      </c>
+      <c r="N33" s="16">
+        <f>M33/L$33</f>
+        <v>0.19854018095316492</v>
+      </c>
+      <c r="P33" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>1</v>
+      </c>
+      <c r="R33" s="4">
+        <f>LN(D33) - LN(D26)</f>
+        <v>0.22314355131421015</v>
+      </c>
+      <c r="S33" s="4">
+        <f>LN(E33) - LN(E26)</f>
+        <v>-0.69314718055994529</v>
+      </c>
+      <c r="T33" s="4">
+        <f>LN(F33) - LN(F26)</f>
+        <v>0.22314355131420971</v>
+      </c>
+      <c r="V33" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="W33" s="21">
+        <v>1</v>
+      </c>
+      <c r="X33" s="4">
+        <f>$M33*R33</f>
+        <v>12.654981496301259</v>
+      </c>
+      <c r="Y33" s="4">
+        <f>$M33*S33</f>
+        <v>-39.309962992602486</v>
+      </c>
+      <c r="Z33" s="4">
+        <f>$M33*T33</f>
+        <v>12.654981496301232</v>
+      </c>
+      <c r="AC33" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD33" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="4">
+        <f>$N33*R33</f>
+        <v>4.4302961056455127E-2</v>
+      </c>
+      <c r="AF33" s="4">
+        <f>$N33*S33</f>
+        <v>-0.13761756665554761</v>
+      </c>
+      <c r="AG33" s="4">
+        <f>$N33*T33</f>
+        <v>4.4302961056455037E-2</v>
+      </c>
+      <c r="AJ33" s="27"/>
+      <c r="AK33" s="27"/>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B34" s="31"/>
+      <c r="C34" s="21">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>6</v>
+      </c>
+      <c r="E34" s="4">
+        <v>8</v>
+      </c>
+      <c r="F34" s="4">
+        <v>6</v>
+      </c>
+      <c r="G34" s="12">
+        <f>PRODUCT(D34:F34)</f>
+        <v>288</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="M34" s="15">
+        <f>(G34-G27) / (LN(G34) - LN(G27))</f>
+        <v>226.82814674545895</v>
+      </c>
+      <c r="N34" s="16">
+        <f>M34/L$33</f>
+        <v>0.79408717861097466</v>
+      </c>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="21">
+        <v>2</v>
+      </c>
+      <c r="R34" s="4">
+        <f>LN(D34) - LN(D27)</f>
+        <v>0.18232155679395468</v>
+      </c>
+      <c r="S34" s="4">
+        <f>LN(E34) - LN(E27)</f>
+        <v>0.13353139262452252</v>
+      </c>
+      <c r="T34" s="4">
+        <f>LN(F34) - LN(F27)</f>
+        <v>0.18232155679395468</v>
+      </c>
+      <c r="V34" s="25"/>
+      <c r="W34" s="21">
+        <v>2</v>
+      </c>
+      <c r="X34" s="4">
+        <f>$M34*R34</f>
+        <v>41.355660839319683</v>
+      </c>
+      <c r="Y34" s="4">
+        <f>$M34*S34</f>
+        <v>30.288678321360688</v>
+      </c>
+      <c r="Z34" s="4">
+        <f>$M34*T34</f>
+        <v>41.355660839319683</v>
+      </c>
+      <c r="AC34" s="25"/>
+      <c r="AD34" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="4">
+        <f>$N34*R34</f>
+        <v>0.14477921063447205</v>
+      </c>
+      <c r="AF34" s="4">
+        <f>$N34*S34</f>
+        <v>0.10603556682520139</v>
+      </c>
+      <c r="AG34" s="4">
+        <f>$N34*T34</f>
+        <v>0.14477921063447205</v>
+      </c>
+      <c r="AJ34" s="27"/>
+      <c r="AK34" s="27"/>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D35" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="R35" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="X35" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+      <c r="AE35" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF35" s="30"/>
+      <c r="AG35" s="30"/>
+      <c r="AJ35" s="27"/>
+      <c r="AK35" s="27"/>
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="13">
+        <f>SUM(G33:G34)</f>
+        <v>338</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="X36" s="4">
+        <f>SUM(X33:X34)</f>
+        <v>54.010642335620943</v>
+      </c>
+      <c r="Y36" s="4">
+        <f t="shared" ref="Y36:Z36" si="14">SUM(Y33:Y34)</f>
+        <v>-9.0212846712417978</v>
+      </c>
+      <c r="Z36" s="4">
+        <f t="shared" si="14"/>
+        <v>54.010642335620915</v>
+      </c>
+      <c r="AA36" s="18">
+        <f>SUM(X36:Z36)</f>
+        <v>99.000000000000057</v>
+      </c>
+      <c r="AB36" s="19"/>
+      <c r="AE36" s="4">
+        <f>EXP(SUM(AE33:AE34))</f>
+        <v>1.2081402233292473</v>
+      </c>
+      <c r="AF36" s="4">
+        <f t="shared" ref="AF36:AG36" si="15">EXP(SUM(AF33:AF34))</f>
+        <v>0.96891150261734849</v>
+      </c>
+      <c r="AG36" s="4">
+        <f t="shared" si="15"/>
+        <v>1.2081402233292473</v>
+      </c>
+      <c r="AH36" s="17">
+        <f>PRODUCT(AE36:AG36)</f>
+        <v>1.4142259414225939</v>
+      </c>
+      <c r="AJ36" s="4">
+        <f>AJ29+X36</f>
+        <v>166.76092297970456</v>
+      </c>
+      <c r="AK36" s="4">
+        <f t="shared" ref="AK36:AL36" si="16">AK29+Y36</f>
+        <v>-52.795437028546971</v>
+      </c>
+      <c r="AL36" s="4">
+        <f t="shared" si="16"/>
+        <v>144.03451404884231</v>
+      </c>
+      <c r="AN36" s="4">
+        <f>AN29*AE36</f>
+        <v>2.6155208515192934</v>
+      </c>
+      <c r="AO36" s="4">
+        <f t="shared" ref="AO36:AP36" si="17">AO29*AF36</f>
+        <v>0.7609663039470701</v>
+      </c>
+      <c r="AP36" s="4">
+        <f t="shared" si="17"/>
+        <v>2.1227707766832733</v>
+      </c>
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="X37" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y37" s="28"/>
+      <c r="Z37" s="28"/>
+      <c r="AA37" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB37" s="8"/>
+      <c r="AE37" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF37" s="30"/>
+      <c r="AG37" s="30"/>
+      <c r="AH37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ37" s="27"/>
+      <c r="AK37" s="27"/>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="9"/>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="9"/>
+      <c r="AI38" s="9"/>
+      <c r="AJ38" s="8"/>
+      <c r="AK38" s="8"/>
+      <c r="AL38" s="9"/>
+      <c r="AM38" s="9"/>
+      <c r="AN38" s="9"/>
+      <c r="AO38" s="9"/>
+      <c r="AP38" s="9"/>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="9"/>
+      <c r="AC39" s="9"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="8"/>
+      <c r="AF39" s="8"/>
+      <c r="AG39" s="8"/>
+      <c r="AH39" s="9"/>
+      <c r="AI39" s="9"/>
+      <c r="AJ39" s="8"/>
+      <c r="AK39" s="8"/>
+      <c r="AL39" s="9"/>
+      <c r="AM39" s="9"/>
+      <c r="AN39" s="9"/>
+      <c r="AO39" s="9"/>
+      <c r="AP39" s="9"/>
+    </row>
+    <row r="40" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V40" s="23"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="9"/>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="22"/>
+      <c r="AE40" s="8"/>
+      <c r="AF40" s="8"/>
+      <c r="AG40" s="8"/>
+      <c r="AH40" s="9"/>
+      <c r="AI40" s="9"/>
+      <c r="AJ40" s="8"/>
+      <c r="AK40" s="8"/>
+      <c r="AL40" s="9"/>
+      <c r="AM40" s="9"/>
+      <c r="AN40" s="9"/>
+      <c r="AO40" s="9"/>
+      <c r="AP40" s="9"/>
+    </row>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="V41" s="23"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="9"/>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="22"/>
+      <c r="AE41" s="8"/>
+      <c r="AF41" s="8"/>
+      <c r="AG41" s="8"/>
+      <c r="AH41" s="9"/>
+      <c r="AI41" s="9"/>
+      <c r="AJ41" s="8"/>
+      <c r="AK41" s="8"/>
+      <c r="AL41" s="9"/>
+      <c r="AM41" s="9"/>
+      <c r="AN41" s="9"/>
+      <c r="AO41" s="9"/>
+      <c r="AP41" s="9"/>
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="24">
+        <f>X22+X29+X36</f>
+        <v>166.76092297970456</v>
+      </c>
+      <c r="Y42" s="24">
+        <f t="shared" ref="Y42:AA42" si="18">Y22+Y29+Y36</f>
+        <v>-52.795437028546971</v>
+      </c>
+      <c r="Z42" s="24">
+        <f t="shared" si="18"/>
+        <v>144.03451404884231</v>
+      </c>
+      <c r="AA42" s="24">
+        <f t="shared" si="18"/>
+        <v>257.99999999999994</v>
+      </c>
+      <c r="AC42" s="9"/>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="24">
+        <f>AE22*AE29*AE36</f>
+        <v>2.6155208515192934</v>
+      </c>
+      <c r="AF42" s="24">
+        <f t="shared" ref="AF42:AH42" si="19">AF22*AF29*AF36</f>
+        <v>0.7609663039470701</v>
+      </c>
+      <c r="AG42" s="24">
+        <f t="shared" si="19"/>
+        <v>2.1227707766832733</v>
+      </c>
+      <c r="AH42" s="24">
+        <f t="shared" si="19"/>
+        <v>4.2249999999999996</v>
+      </c>
+      <c r="AI42" s="9"/>
+      <c r="AJ42" s="8"/>
+      <c r="AK42" s="8"/>
+      <c r="AL42" s="9"/>
+      <c r="AM42" s="9"/>
+      <c r="AN42" s="9"/>
+      <c r="AO42" s="9"/>
+      <c r="AP42" s="9"/>
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+      <c r="Z43" s="9">
+        <f>SUM(X42:Z42)</f>
+        <v>257.99999999999989</v>
+      </c>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="8"/>
+      <c r="AF43" s="8"/>
+      <c r="AG43" s="8">
+        <f>AE42*AF42*AG42</f>
+        <v>4.2249999999999988</v>
+      </c>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="9"/>
+      <c r="AJ43" s="8"/>
+      <c r="AK43" s="8"/>
+      <c r="AL43" s="8"/>
+      <c r="AM43" s="9"/>
+      <c r="AN43" s="8"/>
+      <c r="AO43" s="8"/>
+      <c r="AP43" s="8"/>
+    </row>
+    <row r="47" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="D24:F24"/>
+  <mergeCells count="58">
+    <mergeCell ref="AE30:AG30"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="AE35:AG35"/>
+    <mergeCell ref="X35:Z35"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="AE37:AG37"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="R31:T31"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="D28:F28"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="AE21:AG21"/>
     <mergeCell ref="X23:Z23"/>
     <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="P19:P20"/>
     <mergeCell ref="V19:V20"/>
     <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="R21:T21"/>
     <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="P12:P13"/>
     <mergeCell ref="V12:V13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="X7:Z7"/>
     <mergeCell ref="A1:AP1"/>
     <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="AJ10:AL10"/>
+    <mergeCell ref="AN10:AP10"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="R10:T10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
No real changes. Just stupid Excel.
</commit_message>
<xml_diff>
--- a/tests/testthat/LMDI_testing.xlsx
+++ b/tests/testthat/LMDI_testing.xlsx
@@ -20,7 +20,7 @@
     <sheet name="GH data -- correct" sheetId="10" r:id="rId6"/>
     <sheet name="GH data -- small numbers test" sheetId="11" r:id="rId7"/>
     <sheet name="GH data -- correct test" sheetId="12" r:id="rId8"/>
-    <sheet name="UK data -- errors" sheetId="13" r:id="rId9"/>
+    <sheet name="UK data -- fixed" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -15046,11 +15046,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D43" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="Q50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V59" sqref="V59:Y60"/>
+      <selection pane="bottomRight" activeCell="V82" sqref="V82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15829,7 +15829,7 @@
       <c r="B31" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="32">
@@ -15903,7 +15903,7 @@
     </row>
     <row r="32" spans="1:25">
       <c r="B32" s="55"/>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="32">
@@ -15974,7 +15974,7 @@
     </row>
     <row r="33" spans="2:25">
       <c r="B33" s="55"/>
-      <c r="C33" t="s">
+      <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="32">
@@ -16036,7 +16036,7 @@
     </row>
     <row r="34" spans="2:25">
       <c r="B34" s="55"/>
-      <c r="C34" t="s">
+      <c r="C34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="32">
@@ -16098,7 +16098,7 @@
     </row>
     <row r="35" spans="2:25">
       <c r="B35" s="55"/>
-      <c r="C35" t="s">
+      <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="32">
@@ -16160,7 +16160,7 @@
     </row>
     <row r="36" spans="2:25">
       <c r="B36" s="55"/>
-      <c r="C36" t="s">
+      <c r="C36" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="32">
@@ -16222,7 +16222,7 @@
     </row>
     <row r="37" spans="2:25">
       <c r="B37" s="55"/>
-      <c r="C37" t="s">
+      <c r="C37" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="32">
@@ -16284,7 +16284,7 @@
     </row>
     <row r="38" spans="2:25">
       <c r="B38" s="55"/>
-      <c r="C38" t="s">
+      <c r="C38" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="32">
@@ -16346,7 +16346,7 @@
     </row>
     <row r="39" spans="2:25">
       <c r="B39" s="55"/>
-      <c r="C39" t="s">
+      <c r="C39" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="32">
@@ -16408,7 +16408,7 @@
     </row>
     <row r="40" spans="2:25">
       <c r="B40" s="55"/>
-      <c r="C40" t="s">
+      <c r="C40" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="32">
@@ -16470,7 +16470,7 @@
     </row>
     <row r="41" spans="2:25">
       <c r="B41" s="55"/>
-      <c r="C41" t="s">
+      <c r="C41" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="32">
@@ -16532,7 +16532,7 @@
     </row>
     <row r="42" spans="2:25">
       <c r="B42" s="55"/>
-      <c r="C42" t="s">
+      <c r="C42" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D42" s="32">
@@ -16594,7 +16594,7 @@
     </row>
     <row r="43" spans="2:25">
       <c r="B43" s="55"/>
-      <c r="C43" t="s">
+      <c r="C43" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="32">
@@ -16656,7 +16656,7 @@
     </row>
     <row r="44" spans="2:25">
       <c r="B44" s="55"/>
-      <c r="C44" t="s">
+      <c r="C44" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D44" s="32">
@@ -16718,7 +16718,7 @@
     </row>
     <row r="45" spans="2:25">
       <c r="B45" s="55"/>
-      <c r="C45" t="s">
+      <c r="C45" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D45" s="32">
@@ -16780,7 +16780,7 @@
     </row>
     <row r="46" spans="2:25">
       <c r="B46" s="55"/>
-      <c r="C46" t="s">
+      <c r="C46" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D46" s="32">
@@ -16842,7 +16842,7 @@
     </row>
     <row r="47" spans="2:25">
       <c r="B47" s="55"/>
-      <c r="C47" t="s">
+      <c r="C47" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D47" s="32">
@@ -16904,7 +16904,7 @@
     </row>
     <row r="48" spans="2:25">
       <c r="B48" s="55"/>
-      <c r="C48" t="s">
+      <c r="C48" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D48" s="32">
@@ -16966,7 +16966,7 @@
     </row>
     <row r="49" spans="1:26">
       <c r="B49" s="55"/>
-      <c r="C49" t="s">
+      <c r="C49" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D49" s="32">
@@ -17028,7 +17028,7 @@
     </row>
     <row r="50" spans="1:26">
       <c r="B50" s="55"/>
-      <c r="C50" t="s">
+      <c r="C50" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D50" s="32">
@@ -17090,7 +17090,7 @@
     </row>
     <row r="51" spans="1:26">
       <c r="B51" s="55"/>
-      <c r="C51" t="s">
+      <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="32">
@@ -17152,7 +17152,7 @@
     </row>
     <row r="52" spans="1:26">
       <c r="B52" s="55"/>
-      <c r="C52" t="s">
+      <c r="C52" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D52" s="32">
@@ -17349,20 +17349,19 @@
       <c r="A59">
         <v>2004</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D59" s="47">
-        <v>7962.9211678178699</v>
+        <v>1</v>
       </c>
       <c r="E59" s="48">
-        <f>E31</f>
-        <v>0.168054744834221</v>
+        <v>1</v>
       </c>
       <c r="F59" s="47">
-        <v>0.49936451115254499</v>
-      </c>
-      <c r="G59" s="49">
+        <v>1</v>
+      </c>
+      <c r="G59" s="48">
         <v>0</v>
       </c>
       <c r="H59" s="50">
@@ -17390,15 +17389,15 @@
       </c>
       <c r="Q59" s="4">
         <f>LN(D59) - LN(D31)</f>
-        <v>6.6809539825722908E-3</v>
+        <v>-8.9758702384164852</v>
       </c>
       <c r="R59" s="4">
         <f t="shared" ref="Q59:T80" si="9">LN(E59) - LN(E31)</f>
-        <v>0</v>
+        <v>1.7834654905519454</v>
       </c>
       <c r="S59" s="4">
         <f t="shared" si="9"/>
-        <v>-4.2957156103365479E-2</v>
+        <v>0.65146181052866581</v>
       </c>
       <c r="T59" s="4"/>
       <c r="V59" s="4">
@@ -17422,7 +17421,7 @@
       <c r="B60" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D60" s="4">
@@ -17475,7 +17474,7 @@
         <v>-3.0427912375130539E-3</v>
       </c>
       <c r="V60" s="4">
-        <f t="shared" si="10"/>
+        <f>$N60*Q60</f>
         <v>1.1188553384386695E-2</v>
       </c>
       <c r="W60" s="4">
@@ -17493,7 +17492,7 @@
     </row>
     <row r="61" spans="1:26">
       <c r="B61" s="55"/>
-      <c r="C61" t="s">
+      <c r="C61" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D61" s="4">
@@ -17555,7 +17554,7 @@
     </row>
     <row r="62" spans="1:26">
       <c r="B62" s="55"/>
-      <c r="C62" t="s">
+      <c r="C62" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="4">
@@ -17617,7 +17616,7 @@
     </row>
     <row r="63" spans="1:26">
       <c r="B63" s="55"/>
-      <c r="C63" t="s">
+      <c r="C63" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D63" s="4">
@@ -17679,7 +17678,7 @@
     </row>
     <row r="64" spans="1:26">
       <c r="B64" s="55"/>
-      <c r="C64" t="s">
+      <c r="C64" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D64" s="4">
@@ -17741,7 +17740,7 @@
     </row>
     <row r="65" spans="2:25">
       <c r="B65" s="55"/>
-      <c r="C65" t="s">
+      <c r="C65" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D65" s="4">
@@ -17803,7 +17802,7 @@
     </row>
     <row r="66" spans="2:25">
       <c r="B66" s="55"/>
-      <c r="C66" t="s">
+      <c r="C66" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D66" s="4">
@@ -17865,7 +17864,7 @@
     </row>
     <row r="67" spans="2:25">
       <c r="B67" s="55"/>
-      <c r="C67" t="s">
+      <c r="C67" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D67" s="4">
@@ -17927,7 +17926,7 @@
     </row>
     <row r="68" spans="2:25">
       <c r="B68" s="55"/>
-      <c r="C68" t="s">
+      <c r="C68" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D68" s="4">
@@ -17989,7 +17988,7 @@
     </row>
     <row r="69" spans="2:25">
       <c r="B69" s="55"/>
-      <c r="C69" t="s">
+      <c r="C69" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D69" s="4">
@@ -18051,7 +18050,7 @@
     </row>
     <row r="70" spans="2:25">
       <c r="B70" s="55"/>
-      <c r="C70" t="s">
+      <c r="C70" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D70" s="4">
@@ -18113,7 +18112,7 @@
     </row>
     <row r="71" spans="2:25">
       <c r="B71" s="55"/>
-      <c r="C71" t="s">
+      <c r="C71" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D71" s="4">
@@ -18175,7 +18174,7 @@
     </row>
     <row r="72" spans="2:25">
       <c r="B72" s="55"/>
-      <c r="C72" t="s">
+      <c r="C72" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D72" s="4">
@@ -18237,7 +18236,7 @@
     </row>
     <row r="73" spans="2:25">
       <c r="B73" s="55"/>
-      <c r="C73" t="s">
+      <c r="C73" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D73" s="4">
@@ -18299,7 +18298,7 @@
     </row>
     <row r="74" spans="2:25">
       <c r="B74" s="55"/>
-      <c r="C74" t="s">
+      <c r="C74" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D74" s="4">
@@ -18361,7 +18360,7 @@
     </row>
     <row r="75" spans="2:25">
       <c r="B75" s="55"/>
-      <c r="C75" t="s">
+      <c r="C75" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D75" s="4">
@@ -18423,7 +18422,7 @@
     </row>
     <row r="76" spans="2:25">
       <c r="B76" s="55"/>
-      <c r="C76" t="s">
+      <c r="C76" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D76" s="4">
@@ -18485,7 +18484,7 @@
     </row>
     <row r="77" spans="2:25">
       <c r="B77" s="55"/>
-      <c r="C77" t="s">
+      <c r="C77" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D77" s="4">
@@ -18547,7 +18546,7 @@
     </row>
     <row r="78" spans="2:25">
       <c r="B78" s="55"/>
-      <c r="C78" t="s">
+      <c r="C78" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D78" s="4">
@@ -18609,7 +18608,7 @@
     </row>
     <row r="79" spans="2:25">
       <c r="B79" s="55"/>
-      <c r="C79" t="s">
+      <c r="C79" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D79" s="4">
@@ -18671,7 +18670,7 @@
     </row>
     <row r="80" spans="2:25">
       <c r="B80" s="55"/>
-      <c r="C80" t="s">
+      <c r="C80" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D80" s="4">
@@ -20180,10 +20179,10 @@
   <dimension ref="A1:AF55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="S26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF55" sqref="AF55"/>
+      <selection pane="bottomRight" activeCell="AF54" sqref="AF54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>